<commit_message>
test chuc nang them
</commit_message>
<xml_diff>
--- a/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LINH\CNTT\NAM 5\QTDACNTT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LINH\CNTT\NAM 5\QTDACNTT\BTL_QTDACNTT_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$67</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -36,7 +36,7 @@
     <author>Nguyen Duc Tien</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0">
+    <comment ref="H49" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0">
+    <comment ref="J49" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0">
+    <comment ref="A50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="0" shapeId="0">
+    <comment ref="H51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I24" authorId="0" shapeId="0">
+    <comment ref="I51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0" shapeId="0">
+    <comment ref="J51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0">
+    <comment ref="A52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="0" shapeId="0">
+    <comment ref="H53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="0" shapeId="0">
+    <comment ref="I53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0">
+    <comment ref="A54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="77">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -308,9 +308,6 @@
   </si>
   <si>
     <t>1.</t>
-  </si>
-  <si>
-    <t>Test với tham số mặc định</t>
   </si>
   <si>
     <t>No.</t>
@@ -429,6 +426,22 @@
   </si>
   <si>
     <t>1.1-2</t>
+  </si>
+  <si>
+    <t>Test chức năng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chức năng xem
+</t>
+  </si>
+  <si>
+    <t>Click vào button xem để xem, mỗi lần click sẽ hiển thị ngẫu nhiên ra một confession</t>
+  </si>
+  <si>
+    <t>LinhNT</t>
+  </si>
+  <si>
+    <t>15/12/2018</t>
   </si>
 </sst>
 </file>
@@ -939,7 +952,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1237,6 +1250,30 @@
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1244,95 +1281,95 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1854,13 +1891,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="127" t="s">
+      <c r="O6" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
-      <c r="S6" s="127"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="135"/>
+      <c r="S6" s="135"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -1870,11 +1907,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="127"/>
-      <c r="P7" s="127"/>
-      <c r="Q7" s="127"/>
-      <c r="R7" s="127"/>
-      <c r="S7" s="127"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="135"/>
+      <c r="R7" s="135"/>
+      <c r="S7" s="135"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -1929,12 +1966,12 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="128">
+      <c r="E11" s="136">
         <f ca="1">TODAY()</f>
-        <v>43441</v>
-      </c>
-      <c r="F11" s="128"/>
-      <c r="G11" s="128"/>
+        <v>43449</v>
+      </c>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
       <c r="H11" s="72"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
@@ -2794,8 +2831,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2827,7 +2864,7 @@
       </c>
       <c r="I1" s="101">
         <f>COUNTIF(H1:H786,"OK")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J1" s="82" t="s">
         <v>23</v>
@@ -2895,7 +2932,7 @@
       <c r="H4" s="85"/>
       <c r="I4" s="102">
         <f>COUNTIF(H3:H788,"Result")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J4" s="89"/>
       <c r="K4" s="90"/>
@@ -2930,695 +2967,398 @@
       <c r="A7" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="129" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="129"/>
-      <c r="J7" s="129"/>
-      <c r="K7" s="129"/>
+      <c r="B7" s="164" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="164"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="164"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="164"/>
+      <c r="I7" s="164"/>
+      <c r="J7" s="164"/>
+      <c r="K7" s="164"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="132" t="s">
+      <c r="C8" s="138"/>
+      <c r="D8" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="133"/>
-      <c r="D8" s="132" t="s">
+      <c r="E8" s="138"/>
+      <c r="F8" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="133"/>
-      <c r="F8" s="132" t="s">
+      <c r="G8" s="138"/>
+      <c r="H8" s="165" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="133"/>
-      <c r="H8" s="131" t="s">
+      <c r="I8" s="165"/>
+      <c r="J8" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="131"/>
-      <c r="J8" s="118" t="s">
+      <c r="K8" s="47" t="s">
         <v>40</v>
-      </c>
-      <c r="K8" s="47" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="150" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="151"/>
-      <c r="D9" s="142" t="s">
+      <c r="B9" s="139" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="140"/>
+      <c r="D9" s="148" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="149"/>
+      <c r="F9" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="143"/>
-      <c r="F9" s="120" t="s">
-        <v>44</v>
-      </c>
       <c r="G9" s="121"/>
-      <c r="H9" s="140" t="s">
+      <c r="H9" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="141"/>
+      <c r="I9" s="155"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="137"/>
+      <c r="K9" s="161"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="152"/>
-      <c r="C10" s="153"/>
-      <c r="D10" s="144"/>
-      <c r="E10" s="145"/>
+        <v>44</v>
+      </c>
+      <c r="B10" s="141"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="150"/>
+      <c r="E10" s="151"/>
       <c r="F10" s="122"/>
       <c r="G10" s="123"/>
       <c r="H10" s="117" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="117" t="s">
+      <c r="J10" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="138"/>
+      <c r="K10" s="162"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="152"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="145"/>
+        <v>48</v>
+      </c>
+      <c r="B11" s="141"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="151"/>
       <c r="F11" s="122"/>
       <c r="G11" s="123"/>
       <c r="H11" s="50" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="138"/>
+      <c r="K11" s="162"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="152"/>
-      <c r="C12" s="153"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="145"/>
+        <v>50</v>
+      </c>
+      <c r="B12" s="141"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="151"/>
       <c r="F12" s="122"/>
       <c r="G12" s="123"/>
       <c r="H12" s="117" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="117" t="s">
-        <v>53</v>
-      </c>
       <c r="J12" s="117"/>
-      <c r="K12" s="138"/>
+      <c r="K12" s="162"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>981</v>
       </c>
-      <c r="B13" s="154"/>
-      <c r="C13" s="155"/>
-      <c r="D13" s="146"/>
-      <c r="E13" s="147"/>
+      <c r="B13" s="143"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="152"/>
+      <c r="E13" s="153"/>
       <c r="F13" s="124"/>
       <c r="G13" s="125"/>
       <c r="H13" s="53" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="139"/>
+      <c r="K13" s="163"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="135" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="136"/>
-      <c r="D14" s="135" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="146" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="147"/>
+      <c r="D14" s="146" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="147"/>
+      <c r="F14" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="136"/>
-      <c r="F14" s="135" t="s">
+      <c r="G14" s="147"/>
+      <c r="H14" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="136"/>
-      <c r="H14" s="158" t="s">
+      <c r="I14" s="145"/>
+      <c r="J14" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="158"/>
-      <c r="J14" s="126" t="s">
+      <c r="K14" s="56" t="s">
         <v>40</v>
-      </c>
-      <c r="K14" s="56" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="10.5" customHeight="1">
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="150" t="s">
+      <c r="B15" s="139" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="140"/>
+      <c r="D15" s="148" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="149"/>
+      <c r="F15" s="120" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="121"/>
+      <c r="H15" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="157"/>
+      <c r="J15" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="151"/>
-      <c r="D15" s="142" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="143"/>
-      <c r="F15" s="120" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="121"/>
-      <c r="H15" s="148" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="149"/>
-      <c r="J15" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" s="137"/>
+      <c r="K15" s="161"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="126" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="152"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="145"/>
+        <v>44</v>
+      </c>
+      <c r="B16" s="141"/>
+      <c r="C16" s="142"/>
+      <c r="D16" s="150"/>
+      <c r="E16" s="151"/>
       <c r="F16" s="122"/>
       <c r="G16" s="123"/>
       <c r="H16" s="126" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="126" t="s">
+      <c r="J16" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="126" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="138"/>
+      <c r="K16" s="162"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="152"/>
-      <c r="C17" s="153"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="145"/>
+        <v>57</v>
+      </c>
+      <c r="B17" s="141"/>
+      <c r="C17" s="142"/>
+      <c r="D17" s="150"/>
+      <c r="E17" s="151"/>
       <c r="F17" s="122"/>
       <c r="G17" s="123"/>
       <c r="H17" s="50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I17" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="J17" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="K17" s="138"/>
+      <c r="K17" s="162"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="126" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="152"/>
-      <c r="C18" s="153"/>
-      <c r="D18" s="144"/>
-      <c r="E18" s="145"/>
+        <v>50</v>
+      </c>
+      <c r="B18" s="141"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="150"/>
+      <c r="E18" s="151"/>
       <c r="F18" s="122"/>
       <c r="G18" s="123"/>
       <c r="H18" s="126" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="I18" s="126" t="s">
-        <v>53</v>
-      </c>
       <c r="J18" s="126"/>
-      <c r="K18" s="138"/>
+      <c r="K18" s="162"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>921</v>
       </c>
-      <c r="B19" s="154"/>
-      <c r="C19" s="155"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="147"/>
+      <c r="B19" s="143"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="152"/>
+      <c r="E19" s="153"/>
       <c r="F19" s="124"/>
       <c r="G19" s="125"/>
       <c r="H19" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I19" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J19" s="48"/>
-      <c r="K19" s="138"/>
-    </row>
-    <row r="20" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A20" s="99" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="134" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="134"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="129"/>
-      <c r="H20" s="129"/>
-      <c r="I20" s="129"/>
-      <c r="J20" s="129"/>
-      <c r="K20" s="129"/>
+      <c r="K19" s="162"/>
+    </row>
+    <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A20" s="127" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="137" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="138"/>
+      <c r="D20" s="137" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="138"/>
+      <c r="F20" s="137" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="138"/>
+      <c r="H20" s="165" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="165"/>
+      <c r="J20" s="128" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="47" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A21" s="100" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="156" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="156"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="157"/>
-      <c r="I21" s="157"/>
-      <c r="J21" s="157"/>
-      <c r="K21" s="157"/>
-    </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A22" s="126" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="135" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="136"/>
-      <c r="D22" s="135" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="136"/>
-      <c r="F22" s="135" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="136"/>
-      <c r="H22" s="158" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" s="158"/>
-      <c r="J22" s="126" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" s="126" t="s">
+      <c r="A21" s="48">
+        <v>1</v>
+      </c>
+      <c r="B21" s="139" t="s">
         <v>41</v>
       </c>
+      <c r="C21" s="140"/>
+      <c r="D21" s="148" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="149"/>
+      <c r="F21" s="129" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="130"/>
+      <c r="H21" s="154" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="155"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="161"/>
+    </row>
+    <row r="22" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A22" s="127" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="141"/>
+      <c r="C22" s="142"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="151"/>
+      <c r="F22" s="131"/>
+      <c r="G22" s="132"/>
+      <c r="H22" s="127" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="127" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="127" t="s">
+        <v>47</v>
+      </c>
+      <c r="K22" s="162"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A23" s="48">
-        <f>A15+1</f>
-        <v>3</v>
-      </c>
-      <c r="B23" s="150" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="151"/>
-      <c r="D23" s="142" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="143"/>
-      <c r="F23" s="142" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="143"/>
-      <c r="H23" s="140" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="141"/>
+      <c r="A23" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="141"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="150"/>
+      <c r="E23" s="151"/>
+      <c r="F23" s="131"/>
+      <c r="G23" s="132"/>
+      <c r="H23" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="137"/>
+      <c r="K23" s="162"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A24" s="126" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="152"/>
-      <c r="C24" s="153"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="145"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="126" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="126" t="s">
-        <v>47</v>
-      </c>
-      <c r="J24" s="126" t="s">
-        <v>48</v>
-      </c>
-      <c r="K24" s="138"/>
+      <c r="A24" s="127" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="141"/>
+      <c r="C24" s="142"/>
+      <c r="D24" s="150"/>
+      <c r="E24" s="151"/>
+      <c r="F24" s="131"/>
+      <c r="G24" s="132"/>
+      <c r="H24" s="127" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="127"/>
+      <c r="K24" s="162"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A25" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="152"/>
-      <c r="C25" s="153"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="50"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="138"/>
-    </row>
-    <row r="26" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A26" s="126" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="152"/>
-      <c r="C26" s="153"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="145"/>
-      <c r="H26" s="126" t="s">
-        <v>52</v>
-      </c>
-      <c r="I26" s="126"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="138"/>
-    </row>
-    <row r="27" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A27" s="51">
-        <v>922</v>
-      </c>
-      <c r="B27" s="154"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="146"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="146"/>
-      <c r="G27" s="147"/>
-      <c r="H27" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="50"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="139"/>
-    </row>
-    <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A28" s="117" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="132" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="133"/>
-      <c r="D28" s="132" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="133"/>
-      <c r="F28" s="132" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="133"/>
-      <c r="H28" s="130" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="130"/>
-      <c r="J28" s="117" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="119" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A29" s="48">
-        <v>4</v>
-      </c>
-      <c r="B29" s="150" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="151"/>
-      <c r="D29" s="142" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="143"/>
-      <c r="F29" s="142" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="143"/>
-      <c r="H29" s="148" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="149"/>
-      <c r="J29" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="K29" s="137"/>
-    </row>
-    <row r="30" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A30" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="152"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="145"/>
-      <c r="H30" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="I30" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="J30" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="K30" s="138"/>
-    </row>
-    <row r="31" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A31" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="152"/>
-      <c r="C31" s="153"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="145"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
-      <c r="H31" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="J31" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="K31" s="138"/>
-    </row>
-    <row r="32" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A32" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="152"/>
-      <c r="C32" s="153"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="145"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="145"/>
-      <c r="H32" s="117" t="s">
-        <v>52</v>
-      </c>
-      <c r="I32" s="117" t="s">
+      <c r="A25" s="51">
+        <v>981</v>
+      </c>
+      <c r="B25" s="143"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="152"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="133"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="J32" s="117"/>
-      <c r="K32" s="138"/>
-    </row>
-    <row r="33" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A33" s="51">
-        <v>823</v>
-      </c>
-      <c r="B33" s="154"/>
-      <c r="C33" s="155"/>
-      <c r="D33" s="146"/>
-      <c r="E33" s="147"/>
-      <c r="F33" s="146"/>
-      <c r="G33" s="147"/>
-      <c r="H33" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="I33" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="J33" s="48"/>
-      <c r="K33" s="139"/>
-    </row>
-    <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A34" s="117" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="132" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="133"/>
-      <c r="D34" s="132" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="133"/>
-      <c r="F34" s="132" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" s="133"/>
-      <c r="H34" s="130" t="s">
-        <v>39</v>
-      </c>
-      <c r="I34" s="130"/>
-      <c r="J34" s="117" t="s">
-        <v>40</v>
-      </c>
-      <c r="K34" s="119" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A35" s="48">
-        <v>5</v>
-      </c>
-      <c r="B35" s="150" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="151"/>
-      <c r="D35" s="142" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="143"/>
-      <c r="F35" s="142" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" s="143"/>
-      <c r="H35" s="148" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="149"/>
-      <c r="J35" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="K35" s="137"/>
-    </row>
-    <row r="36" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A36" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="152"/>
-      <c r="C36" s="153"/>
-      <c r="D36" s="144"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="144"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="I36" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="J36" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="K36" s="138"/>
-    </row>
-    <row r="37" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A37" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="152"/>
-      <c r="C37" s="153"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="J37" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="K37" s="138"/>
-    </row>
-    <row r="38" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A38" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="152"/>
-      <c r="C38" s="153"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="145"/>
-      <c r="F38" s="144"/>
-      <c r="G38" s="145"/>
-      <c r="H38" s="117" t="s">
-        <v>52</v>
-      </c>
-      <c r="I38" s="117" t="s">
-        <v>53</v>
-      </c>
-      <c r="J38" s="117"/>
-      <c r="K38" s="138"/>
-    </row>
-    <row r="39" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A39" s="51">
-        <v>823</v>
-      </c>
-      <c r="B39" s="154"/>
-      <c r="C39" s="155"/>
-      <c r="D39" s="146"/>
-      <c r="E39" s="147"/>
-      <c r="F39" s="146"/>
-      <c r="G39" s="147"/>
-      <c r="H39" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="I39" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="J39" s="48"/>
-      <c r="K39" s="139"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="163"/>
     </row>
     <row r="40" spans="1:11" s="58" customFormat="1">
       <c r="A40" s="62"/>
@@ -3669,145 +3409,426 @@
       <c r="J46" s="62"/>
       <c r="K46" s="62"/>
     </row>
-    <row r="47" spans="1:11" s="58" customFormat="1">
-      <c r="A47" s="62"/>
-      <c r="H47" s="62"/>
-      <c r="I47" s="62"/>
-      <c r="J47" s="62"/>
-      <c r="K47" s="62"/>
-    </row>
-    <row r="48" spans="1:11" s="58" customFormat="1">
-      <c r="A48" s="62"/>
-      <c r="H48" s="62"/>
-      <c r="I48" s="62"/>
-      <c r="J48" s="62"/>
-      <c r="K48" s="62"/>
-    </row>
-    <row r="49" spans="1:11" s="58" customFormat="1">
-      <c r="A49" s="62"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="62"/>
-      <c r="J49" s="62"/>
-      <c r="K49" s="62"/>
-    </row>
-    <row r="50" spans="1:11" s="58" customFormat="1">
-      <c r="A50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
-    </row>
-    <row r="51" spans="1:11" s="58" customFormat="1">
-      <c r="A51" s="62"/>
-      <c r="H51" s="62"/>
-      <c r="I51" s="62"/>
-      <c r="J51" s="62"/>
-      <c r="K51" s="62"/>
-    </row>
-    <row r="52" spans="1:11" s="58" customFormat="1">
-      <c r="A52" s="62"/>
-      <c r="H52" s="62"/>
-      <c r="I52" s="62"/>
-      <c r="J52" s="62"/>
-      <c r="K52" s="62"/>
-    </row>
-    <row r="53" spans="1:11" s="58" customFormat="1">
-      <c r="A53" s="62"/>
-      <c r="H53" s="62"/>
-      <c r="I53" s="62"/>
-      <c r="J53" s="62"/>
-      <c r="K53" s="62"/>
-    </row>
-    <row r="54" spans="1:11" s="58" customFormat="1">
-      <c r="A54" s="62"/>
-      <c r="H54" s="62"/>
-      <c r="I54" s="62"/>
-      <c r="J54" s="62"/>
-      <c r="K54" s="62"/>
-    </row>
-    <row r="55" spans="1:11" s="58" customFormat="1">
-      <c r="A55" s="62"/>
-      <c r="H55" s="62"/>
-      <c r="I55" s="62"/>
-      <c r="J55" s="62"/>
-      <c r="K55" s="62"/>
-    </row>
-    <row r="56" spans="1:11" s="58" customFormat="1">
-      <c r="A56" s="62"/>
-      <c r="H56" s="62"/>
-      <c r="I56" s="62"/>
-      <c r="J56" s="62"/>
-      <c r="K56" s="62"/>
-    </row>
-    <row r="57" spans="1:11" s="58" customFormat="1">
-      <c r="A57" s="62"/>
-      <c r="H57" s="62"/>
-      <c r="I57" s="62"/>
-      <c r="J57" s="62"/>
-      <c r="K57" s="62"/>
-    </row>
-    <row r="58" spans="1:11" s="58" customFormat="1">
-      <c r="A58" s="62"/>
-      <c r="H58" s="62"/>
-      <c r="I58" s="62"/>
-      <c r="J58" s="62"/>
-      <c r="K58" s="62"/>
-    </row>
-    <row r="59" spans="1:11" s="58" customFormat="1">
-      <c r="A59" s="62"/>
-      <c r="H59" s="62"/>
-      <c r="I59" s="62"/>
-      <c r="J59" s="62"/>
-      <c r="K59" s="62"/>
-    </row>
-    <row r="60" spans="1:11" s="58" customFormat="1">
-      <c r="A60" s="62"/>
-      <c r="H60" s="62"/>
-      <c r="I60" s="62"/>
-      <c r="J60" s="62"/>
-      <c r="K60" s="62"/>
-    </row>
-    <row r="61" spans="1:11" s="58" customFormat="1">
-      <c r="A61" s="62"/>
-      <c r="H61" s="62"/>
-      <c r="I61" s="62"/>
-      <c r="J61" s="62"/>
-      <c r="K61" s="62"/>
-    </row>
-    <row r="62" spans="1:11" s="58" customFormat="1">
-      <c r="A62" s="62"/>
-      <c r="H62" s="62"/>
-      <c r="I62" s="62"/>
-      <c r="J62" s="62"/>
-      <c r="K62" s="62"/>
-    </row>
-    <row r="63" spans="1:11" s="58" customFormat="1">
-      <c r="A63" s="62"/>
-      <c r="H63" s="62"/>
-      <c r="I63" s="62"/>
-      <c r="J63" s="62"/>
-      <c r="K63" s="62"/>
-    </row>
-    <row r="64" spans="1:11" s="58" customFormat="1">
-      <c r="A64" s="62"/>
-      <c r="H64" s="62"/>
-      <c r="I64" s="62"/>
-      <c r="J64" s="62"/>
-      <c r="K64" s="62"/>
-    </row>
-    <row r="65" spans="1:11" s="58" customFormat="1">
-      <c r="A65" s="62"/>
-      <c r="H65" s="62"/>
-      <c r="I65" s="62"/>
-      <c r="J65" s="62"/>
-      <c r="K65" s="62"/>
-    </row>
-    <row r="66" spans="1:11" s="58" customFormat="1">
-      <c r="A66" s="62"/>
-      <c r="H66" s="62"/>
-      <c r="I66" s="62"/>
-      <c r="J66" s="62"/>
-      <c r="K66" s="62"/>
+    <row r="47" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A47" s="99" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="166" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="166"/>
+      <c r="D47" s="164"/>
+      <c r="E47" s="164"/>
+      <c r="F47" s="164"/>
+      <c r="G47" s="164"/>
+      <c r="H47" s="164"/>
+      <c r="I47" s="164"/>
+      <c r="J47" s="164"/>
+      <c r="K47" s="164"/>
+    </row>
+    <row r="48" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A48" s="100" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="158" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="158"/>
+      <c r="D48" s="159"/>
+      <c r="E48" s="159"/>
+      <c r="F48" s="159"/>
+      <c r="G48" s="159"/>
+      <c r="H48" s="159"/>
+      <c r="I48" s="159"/>
+      <c r="J48" s="159"/>
+      <c r="K48" s="159"/>
+    </row>
+    <row r="49" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A49" s="126" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="146" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="147"/>
+      <c r="D49" s="146" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="147"/>
+      <c r="F49" s="146" t="s">
+        <v>37</v>
+      </c>
+      <c r="G49" s="147"/>
+      <c r="H49" s="145" t="s">
+        <v>38</v>
+      </c>
+      <c r="I49" s="145"/>
+      <c r="J49" s="126" t="s">
+        <v>39</v>
+      </c>
+      <c r="K49" s="126" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A50" s="48">
+        <f>A15+1</f>
+        <v>3</v>
+      </c>
+      <c r="B50" s="139" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="140"/>
+      <c r="D50" s="148" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" s="149"/>
+      <c r="F50" s="148" t="s">
+        <v>67</v>
+      </c>
+      <c r="G50" s="149"/>
+      <c r="H50" s="154" t="s">
+        <v>10</v>
+      </c>
+      <c r="I50" s="155"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="161"/>
+    </row>
+    <row r="51" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A51" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="141"/>
+      <c r="C51" s="142"/>
+      <c r="D51" s="150"/>
+      <c r="E51" s="151"/>
+      <c r="F51" s="150"/>
+      <c r="G51" s="151"/>
+      <c r="H51" s="126" t="s">
+        <v>45</v>
+      </c>
+      <c r="I51" s="126" t="s">
+        <v>46</v>
+      </c>
+      <c r="J51" s="126" t="s">
+        <v>47</v>
+      </c>
+      <c r="K51" s="162"/>
+    </row>
+    <row r="52" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A52" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="141"/>
+      <c r="C52" s="142"/>
+      <c r="D52" s="150"/>
+      <c r="E52" s="151"/>
+      <c r="F52" s="150"/>
+      <c r="G52" s="151"/>
+      <c r="H52" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="I52" s="50"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="162"/>
+    </row>
+    <row r="53" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A53" s="126" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="141"/>
+      <c r="C53" s="142"/>
+      <c r="D53" s="150"/>
+      <c r="E53" s="151"/>
+      <c r="F53" s="150"/>
+      <c r="G53" s="151"/>
+      <c r="H53" s="126" t="s">
+        <v>51</v>
+      </c>
+      <c r="I53" s="126"/>
+      <c r="J53" s="126"/>
+      <c r="K53" s="162"/>
+    </row>
+    <row r="54" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A54" s="51">
+        <v>922</v>
+      </c>
+      <c r="B54" s="143"/>
+      <c r="C54" s="144"/>
+      <c r="D54" s="152"/>
+      <c r="E54" s="153"/>
+      <c r="F54" s="152"/>
+      <c r="G54" s="153"/>
+      <c r="H54" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I54" s="50"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="163"/>
+    </row>
+    <row r="55" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A55" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="137" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="138"/>
+      <c r="D55" s="137" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" s="138"/>
+      <c r="F55" s="137" t="s">
+        <v>37</v>
+      </c>
+      <c r="G55" s="138"/>
+      <c r="H55" s="160" t="s">
+        <v>38</v>
+      </c>
+      <c r="I55" s="160"/>
+      <c r="J55" s="117" t="s">
+        <v>39</v>
+      </c>
+      <c r="K55" s="119" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A56" s="48">
+        <v>4</v>
+      </c>
+      <c r="B56" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="140"/>
+      <c r="D56" s="148" t="s">
+        <v>66</v>
+      </c>
+      <c r="E56" s="149"/>
+      <c r="F56" s="148" t="s">
+        <v>67</v>
+      </c>
+      <c r="G56" s="149"/>
+      <c r="H56" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="I56" s="157"/>
+      <c r="J56" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="K56" s="161"/>
+    </row>
+    <row r="57" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A57" s="117" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="141"/>
+      <c r="C57" s="142"/>
+      <c r="D57" s="150"/>
+      <c r="E57" s="151"/>
+      <c r="F57" s="150"/>
+      <c r="G57" s="151"/>
+      <c r="H57" s="117" t="s">
+        <v>45</v>
+      </c>
+      <c r="I57" s="117" t="s">
+        <v>46</v>
+      </c>
+      <c r="J57" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="K57" s="162"/>
+    </row>
+    <row r="58" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A58" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="141"/>
+      <c r="C58" s="142"/>
+      <c r="D58" s="150"/>
+      <c r="E58" s="151"/>
+      <c r="F58" s="150"/>
+      <c r="G58" s="151"/>
+      <c r="H58" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="I58" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="J58" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="K58" s="162"/>
+    </row>
+    <row r="59" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A59" s="117" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="141"/>
+      <c r="C59" s="142"/>
+      <c r="D59" s="150"/>
+      <c r="E59" s="151"/>
+      <c r="F59" s="150"/>
+      <c r="G59" s="151"/>
+      <c r="H59" s="117" t="s">
+        <v>51</v>
+      </c>
+      <c r="I59" s="117" t="s">
+        <v>52</v>
+      </c>
+      <c r="J59" s="117"/>
+      <c r="K59" s="162"/>
+    </row>
+    <row r="60" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A60" s="51">
+        <v>823</v>
+      </c>
+      <c r="B60" s="143"/>
+      <c r="C60" s="144"/>
+      <c r="D60" s="152"/>
+      <c r="E60" s="153"/>
+      <c r="F60" s="152"/>
+      <c r="G60" s="153"/>
+      <c r="H60" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I60" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="J60" s="48"/>
+      <c r="K60" s="163"/>
+    </row>
+    <row r="61" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A61" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="137" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="138"/>
+      <c r="D61" s="137" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="138"/>
+      <c r="F61" s="137" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" s="138"/>
+      <c r="H61" s="160" t="s">
+        <v>38</v>
+      </c>
+      <c r="I61" s="160"/>
+      <c r="J61" s="117" t="s">
+        <v>39</v>
+      </c>
+      <c r="K61" s="119" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A62" s="48">
+        <v>5</v>
+      </c>
+      <c r="B62" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="140"/>
+      <c r="D62" s="148" t="s">
+        <v>66</v>
+      </c>
+      <c r="E62" s="149"/>
+      <c r="F62" s="148" t="s">
+        <v>67</v>
+      </c>
+      <c r="G62" s="149"/>
+      <c r="H62" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="I62" s="157"/>
+      <c r="J62" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="K62" s="161"/>
+    </row>
+    <row r="63" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A63" s="117" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="141"/>
+      <c r="C63" s="142"/>
+      <c r="D63" s="150"/>
+      <c r="E63" s="151"/>
+      <c r="F63" s="150"/>
+      <c r="G63" s="151"/>
+      <c r="H63" s="117" t="s">
+        <v>45</v>
+      </c>
+      <c r="I63" s="117" t="s">
+        <v>46</v>
+      </c>
+      <c r="J63" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="K63" s="162"/>
+    </row>
+    <row r="64" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A64" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="141"/>
+      <c r="C64" s="142"/>
+      <c r="D64" s="150"/>
+      <c r="E64" s="151"/>
+      <c r="F64" s="150"/>
+      <c r="G64" s="151"/>
+      <c r="H64" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="I64" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="J64" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="K64" s="162"/>
+    </row>
+    <row r="65" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A65" s="117" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" s="141"/>
+      <c r="C65" s="142"/>
+      <c r="D65" s="150"/>
+      <c r="E65" s="151"/>
+      <c r="F65" s="150"/>
+      <c r="G65" s="151"/>
+      <c r="H65" s="117" t="s">
+        <v>51</v>
+      </c>
+      <c r="I65" s="117" t="s">
+        <v>52</v>
+      </c>
+      <c r="J65" s="117"/>
+      <c r="K65" s="162"/>
+    </row>
+    <row r="66" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A66" s="51">
+        <v>823</v>
+      </c>
+      <c r="B66" s="143"/>
+      <c r="C66" s="144"/>
+      <c r="D66" s="152"/>
+      <c r="E66" s="153"/>
+      <c r="F66" s="152"/>
+      <c r="G66" s="153"/>
+      <c r="H66" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I66" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="J66" s="48"/>
+      <c r="K66" s="163"/>
     </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
       <c r="A67" s="62"/>
@@ -4020,61 +4041,69 @@
       <c r="K96" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B35:C39"/>
-    <mergeCell ref="D29:E33"/>
-    <mergeCell ref="D35:E39"/>
-    <mergeCell ref="F35:G39"/>
+  <mergeCells count="54">
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B47:K47"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="D50:E54"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G54"/>
+    <mergeCell ref="K62:K66"/>
+    <mergeCell ref="F56:G60"/>
+    <mergeCell ref="K56:K60"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H62:I62"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="D9:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C27"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B48:K48"/>
     <mergeCell ref="D15:E19"/>
     <mergeCell ref="B15:C19"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B20:K20"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="K23:K27"/>
-    <mergeCell ref="D23:E27"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G27"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:E25"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B62:C66"/>
+    <mergeCell ref="D56:E60"/>
+    <mergeCell ref="D62:E66"/>
+    <mergeCell ref="F62:G66"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="B50:C54"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="B56:C60"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="H35:I35">
+  <conditionalFormatting sqref="H62:I62">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34:I34">
+  <conditionalFormatting sqref="H61:I61">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>

</xml_diff>

<commit_message>
test chuc nang xem
</commit_message>
<xml_diff>
--- a/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="80">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -372,12 +372,6 @@
   </si>
   <si>
     <t>Subtopic(abnormality)</t>
-  </si>
-  <si>
-    <t>Không có tham số dòng lệnh, nhưng nhập từ Task Manager</t>
-  </si>
-  <si>
-    <t>BUG21312</t>
   </si>
   <si>
     <t>1.2.1-1</t>
@@ -442,6 +436,21 @@
   </si>
   <si>
     <t>15/12/2018</t>
+  </si>
+  <si>
+    <t>Chức năng thêm</t>
+  </si>
+  <si>
+    <t>Click vào button thêm để thêm mới một confession khi muốn chia sẻ tâm sự của mình với mọi người</t>
+  </si>
+  <si>
+    <t>Không chạy được</t>
+  </si>
+  <si>
+    <t>BUG21</t>
+  </si>
+  <si>
+    <t>LongLN</t>
   </si>
 </sst>
 </file>
@@ -1281,12 +1290,75 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1307,69 +1379,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2832,7 +2841,7 @@
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C13"/>
+      <selection activeCell="B21" sqref="B21:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2967,39 +2976,39 @@
       <c r="A7" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="164" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
-      <c r="E7" s="164"/>
-      <c r="F7" s="164"/>
-      <c r="G7" s="164"/>
-      <c r="H7" s="164"/>
-      <c r="I7" s="164"/>
-      <c r="J7" s="164"/>
-      <c r="K7" s="164"/>
+      <c r="B7" s="137" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="137"/>
+      <c r="I7" s="137"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="137"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="137" t="s">
+      <c r="B8" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="138"/>
-      <c r="D8" s="137" t="s">
+      <c r="C8" s="141"/>
+      <c r="D8" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="138"/>
-      <c r="F8" s="137" t="s">
+      <c r="E8" s="141"/>
+      <c r="F8" s="140" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="138"/>
-      <c r="H8" s="165" t="s">
+      <c r="G8" s="141"/>
+      <c r="H8" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="165"/>
+      <c r="I8" s="139"/>
       <c r="J8" s="118" t="s">
         <v>39</v>
       </c>
@@ -3011,33 +3020,33 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="139" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="148" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="149"/>
+      <c r="B9" s="160" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="161"/>
+      <c r="D9" s="150" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="151"/>
       <c r="F9" s="120" t="s">
         <v>43</v>
       </c>
       <c r="G9" s="121"/>
-      <c r="H9" s="154" t="s">
+      <c r="H9" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="155"/>
+      <c r="I9" s="149"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="161"/>
+      <c r="K9" s="145"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="141"/>
-      <c r="C10" s="142"/>
-      <c r="D10" s="150"/>
-      <c r="E10" s="151"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="163"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="153"/>
       <c r="F10" s="122"/>
       <c r="G10" s="123"/>
       <c r="H10" s="117" t="s">
@@ -3049,33 +3058,33 @@
       <c r="J10" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="162"/>
+      <c r="K10" s="146"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="141"/>
-      <c r="C11" s="142"/>
-      <c r="D11" s="150"/>
-      <c r="E11" s="151"/>
+      <c r="B11" s="162"/>
+      <c r="C11" s="163"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="153"/>
       <c r="F11" s="122"/>
       <c r="G11" s="123"/>
       <c r="H11" s="50" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="162"/>
+      <c r="K11" s="146"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="141"/>
-      <c r="C12" s="142"/>
-      <c r="D12" s="150"/>
-      <c r="E12" s="151"/>
+      <c r="B12" s="162"/>
+      <c r="C12" s="163"/>
+      <c r="D12" s="152"/>
+      <c r="E12" s="153"/>
       <c r="F12" s="122"/>
       <c r="G12" s="123"/>
       <c r="H12" s="117" t="s">
@@ -3085,45 +3094,45 @@
         <v>52</v>
       </c>
       <c r="J12" s="117"/>
-      <c r="K12" s="162"/>
+      <c r="K12" s="146"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>981</v>
       </c>
-      <c r="B13" s="143"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="152"/>
-      <c r="E13" s="153"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="165"/>
+      <c r="D13" s="154"/>
+      <c r="E13" s="155"/>
       <c r="F13" s="124"/>
       <c r="G13" s="125"/>
       <c r="H13" s="53" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="163"/>
+      <c r="K13" s="147"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="146" t="s">
+      <c r="B14" s="143" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="147"/>
-      <c r="D14" s="146" t="s">
+      <c r="C14" s="144"/>
+      <c r="D14" s="143" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="147"/>
-      <c r="F14" s="146" t="s">
+      <c r="E14" s="144"/>
+      <c r="F14" s="143" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="147"/>
-      <c r="H14" s="145" t="s">
+      <c r="G14" s="144"/>
+      <c r="H14" s="166" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="145"/>
+      <c r="I14" s="166"/>
       <c r="J14" s="126" t="s">
         <v>39</v>
       </c>
@@ -3135,16 +3144,16 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="139" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="140"/>
-      <c r="D15" s="148" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="149"/>
+      <c r="B15" s="160" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="161"/>
+      <c r="D15" s="150" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="151"/>
       <c r="F15" s="120" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="G15" s="121"/>
       <c r="H15" s="156" t="s">
@@ -3152,18 +3161,18 @@
       </c>
       <c r="I15" s="157"/>
       <c r="J15" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="K15" s="161"/>
+        <v>78</v>
+      </c>
+      <c r="K15" s="145"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="141"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="150"/>
-      <c r="E16" s="151"/>
+      <c r="B16" s="162"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="152"/>
+      <c r="E16" s="153"/>
       <c r="F16" s="122"/>
       <c r="G16" s="123"/>
       <c r="H16" s="126" t="s">
@@ -3175,37 +3184,35 @@
       <c r="J16" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="162"/>
+      <c r="K16" s="146"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="141"/>
-      <c r="C17" s="142"/>
-      <c r="D17" s="150"/>
-      <c r="E17" s="151"/>
+        <v>55</v>
+      </c>
+      <c r="B17" s="162"/>
+      <c r="C17" s="163"/>
+      <c r="D17" s="152"/>
+      <c r="E17" s="153"/>
       <c r="F17" s="122"/>
       <c r="G17" s="123"/>
       <c r="H17" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17" s="50" t="s">
-        <v>58</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="I17" s="50"/>
       <c r="J17" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="K17" s="162"/>
+        <v>79</v>
+      </c>
+      <c r="K17" s="146"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="126" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="141"/>
-      <c r="C18" s="142"/>
-      <c r="D18" s="150"/>
-      <c r="E18" s="151"/>
+      <c r="B18" s="162"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="152"/>
+      <c r="E18" s="153"/>
       <c r="F18" s="122"/>
       <c r="G18" s="123"/>
       <c r="H18" s="126" t="s">
@@ -3215,47 +3222,45 @@
         <v>52</v>
       </c>
       <c r="J18" s="126"/>
-      <c r="K18" s="162"/>
+      <c r="K18" s="146"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>921</v>
       </c>
-      <c r="B19" s="143"/>
-      <c r="C19" s="144"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="153"/>
+      <c r="B19" s="164"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="154"/>
+      <c r="E19" s="155"/>
       <c r="F19" s="124"/>
       <c r="G19" s="125"/>
       <c r="H19" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="50" t="s">
-        <v>60</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="162"/>
+      <c r="K19" s="146"/>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A20" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="137" t="s">
+      <c r="B20" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="138"/>
-      <c r="D20" s="137" t="s">
+      <c r="C20" s="141"/>
+      <c r="D20" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="138"/>
-      <c r="F20" s="137" t="s">
+      <c r="E20" s="141"/>
+      <c r="F20" s="140" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="138"/>
-      <c r="H20" s="165" t="s">
+      <c r="G20" s="141"/>
+      <c r="H20" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="165"/>
+      <c r="I20" s="139"/>
       <c r="J20" s="128" t="s">
         <v>39</v>
       </c>
@@ -3267,33 +3272,33 @@
       <c r="A21" s="48">
         <v>1</v>
       </c>
-      <c r="B21" s="139" t="s">
+      <c r="B21" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="140"/>
-      <c r="D21" s="148" t="s">
+      <c r="C21" s="161"/>
+      <c r="D21" s="150" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="149"/>
+      <c r="E21" s="151"/>
       <c r="F21" s="129" t="s">
         <v>43</v>
       </c>
       <c r="G21" s="130"/>
-      <c r="H21" s="154" t="s">
+      <c r="H21" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="155"/>
+      <c r="I21" s="149"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="161"/>
+      <c r="K21" s="145"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="141"/>
-      <c r="C22" s="142"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="151"/>
+      <c r="B22" s="162"/>
+      <c r="C22" s="163"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="153"/>
       <c r="F22" s="131"/>
       <c r="G22" s="132"/>
       <c r="H22" s="127" t="s">
@@ -3305,16 +3310,16 @@
       <c r="J22" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="K22" s="162"/>
+      <c r="K22" s="146"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="141"/>
-      <c r="C23" s="142"/>
-      <c r="D23" s="150"/>
-      <c r="E23" s="151"/>
+      <c r="B23" s="162"/>
+      <c r="C23" s="163"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="153"/>
       <c r="F23" s="131"/>
       <c r="G23" s="132"/>
       <c r="H23" s="50" t="s">
@@ -3322,16 +3327,16 @@
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="162"/>
+      <c r="K23" s="146"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="141"/>
-      <c r="C24" s="142"/>
-      <c r="D24" s="150"/>
-      <c r="E24" s="151"/>
+      <c r="B24" s="162"/>
+      <c r="C24" s="163"/>
+      <c r="D24" s="152"/>
+      <c r="E24" s="153"/>
       <c r="F24" s="131"/>
       <c r="G24" s="132"/>
       <c r="H24" s="127" t="s">
@@ -3341,16 +3346,16 @@
         <v>52</v>
       </c>
       <c r="J24" s="127"/>
-      <c r="K24" s="162"/>
+      <c r="K24" s="146"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>981</v>
       </c>
-      <c r="B25" s="143"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="152"/>
-      <c r="E25" s="153"/>
+      <c r="B25" s="164"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="155"/>
       <c r="F25" s="133"/>
       <c r="G25" s="134"/>
       <c r="H25" s="53" t="s">
@@ -3358,7 +3363,7 @@
       </c>
       <c r="I25" s="53"/>
       <c r="J25" s="54"/>
-      <c r="K25" s="163"/>
+      <c r="K25" s="147"/>
     </row>
     <row r="40" spans="1:11" s="58" customFormat="1">
       <c r="A40" s="62"/>
@@ -3411,27 +3416,27 @@
     </row>
     <row r="47" spans="1:11" ht="10.5" customHeight="1">
       <c r="A47" s="99" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" s="166" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="166"/>
-      <c r="D47" s="164"/>
-      <c r="E47" s="164"/>
-      <c r="F47" s="164"/>
-      <c r="G47" s="164"/>
-      <c r="H47" s="164"/>
-      <c r="I47" s="164"/>
-      <c r="J47" s="164"/>
-      <c r="K47" s="164"/>
+        <v>59</v>
+      </c>
+      <c r="B47" s="142" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="142"/>
+      <c r="D47" s="137"/>
+      <c r="E47" s="137"/>
+      <c r="F47" s="137"/>
+      <c r="G47" s="137"/>
+      <c r="H47" s="137"/>
+      <c r="I47" s="137"/>
+      <c r="J47" s="137"/>
+      <c r="K47" s="137"/>
     </row>
     <row r="48" spans="1:11" ht="10.5" customHeight="1">
       <c r="A48" s="100" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B48" s="158" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C48" s="158"/>
       <c r="D48" s="159"/>
@@ -3447,22 +3452,22 @@
       <c r="A49" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="B49" s="146" t="s">
+      <c r="B49" s="143" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="147"/>
-      <c r="D49" s="146" t="s">
+      <c r="C49" s="144"/>
+      <c r="D49" s="143" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="147"/>
-      <c r="F49" s="146" t="s">
+      <c r="E49" s="144"/>
+      <c r="F49" s="143" t="s">
         <v>37</v>
       </c>
-      <c r="G49" s="147"/>
-      <c r="H49" s="145" t="s">
+      <c r="G49" s="144"/>
+      <c r="H49" s="166" t="s">
         <v>38</v>
       </c>
-      <c r="I49" s="145"/>
+      <c r="I49" s="166"/>
       <c r="J49" s="126" t="s">
         <v>39</v>
       </c>
@@ -3475,35 +3480,35 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B50" s="139" t="s">
+      <c r="B50" s="160" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="161"/>
+      <c r="D50" s="150" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="151"/>
+      <c r="F50" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="140"/>
-      <c r="D50" s="148" t="s">
-        <v>66</v>
-      </c>
-      <c r="E50" s="149"/>
-      <c r="F50" s="148" t="s">
-        <v>67</v>
-      </c>
-      <c r="G50" s="149"/>
-      <c r="H50" s="154" t="s">
+      <c r="G50" s="151"/>
+      <c r="H50" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="I50" s="155"/>
+      <c r="I50" s="149"/>
       <c r="J50" s="48"/>
-      <c r="K50" s="161"/>
+      <c r="K50" s="145"/>
     </row>
     <row r="51" spans="1:11" ht="10.5" customHeight="1">
       <c r="A51" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="141"/>
-      <c r="C51" s="142"/>
-      <c r="D51" s="150"/>
-      <c r="E51" s="151"/>
-      <c r="F51" s="150"/>
-      <c r="G51" s="151"/>
+      <c r="B51" s="162"/>
+      <c r="C51" s="163"/>
+      <c r="D51" s="152"/>
+      <c r="E51" s="153"/>
+      <c r="F51" s="152"/>
+      <c r="G51" s="153"/>
       <c r="H51" s="126" t="s">
         <v>45</v>
       </c>
@@ -3513,79 +3518,79 @@
       <c r="J51" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="K51" s="162"/>
+      <c r="K51" s="146"/>
     </row>
     <row r="52" spans="1:11" ht="10.5" customHeight="1">
       <c r="A52" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="141"/>
-      <c r="C52" s="142"/>
-      <c r="D52" s="150"/>
-      <c r="E52" s="151"/>
-      <c r="F52" s="150"/>
-      <c r="G52" s="151"/>
+        <v>66</v>
+      </c>
+      <c r="B52" s="162"/>
+      <c r="C52" s="163"/>
+      <c r="D52" s="152"/>
+      <c r="E52" s="153"/>
+      <c r="F52" s="152"/>
+      <c r="G52" s="153"/>
       <c r="H52" s="50" t="s">
         <v>49</v>
       </c>
       <c r="I52" s="50"/>
       <c r="J52" s="48"/>
-      <c r="K52" s="162"/>
+      <c r="K52" s="146"/>
     </row>
     <row r="53" spans="1:11" ht="10.5" customHeight="1">
       <c r="A53" s="126" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="141"/>
-      <c r="C53" s="142"/>
-      <c r="D53" s="150"/>
-      <c r="E53" s="151"/>
-      <c r="F53" s="150"/>
-      <c r="G53" s="151"/>
+      <c r="B53" s="162"/>
+      <c r="C53" s="163"/>
+      <c r="D53" s="152"/>
+      <c r="E53" s="153"/>
+      <c r="F53" s="152"/>
+      <c r="G53" s="153"/>
       <c r="H53" s="126" t="s">
         <v>51</v>
       </c>
       <c r="I53" s="126"/>
       <c r="J53" s="126"/>
-      <c r="K53" s="162"/>
+      <c r="K53" s="146"/>
     </row>
     <row r="54" spans="1:11" ht="10.5" customHeight="1">
       <c r="A54" s="51">
         <v>922</v>
       </c>
-      <c r="B54" s="143"/>
-      <c r="C54" s="144"/>
-      <c r="D54" s="152"/>
-      <c r="E54" s="153"/>
-      <c r="F54" s="152"/>
-      <c r="G54" s="153"/>
+      <c r="B54" s="164"/>
+      <c r="C54" s="165"/>
+      <c r="D54" s="154"/>
+      <c r="E54" s="155"/>
+      <c r="F54" s="154"/>
+      <c r="G54" s="155"/>
       <c r="H54" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I54" s="50"/>
       <c r="J54" s="48"/>
-      <c r="K54" s="163"/>
+      <c r="K54" s="147"/>
     </row>
     <row r="55" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A55" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B55" s="137" t="s">
+      <c r="B55" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="138"/>
-      <c r="D55" s="137" t="s">
+      <c r="C55" s="141"/>
+      <c r="D55" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="E55" s="138"/>
-      <c r="F55" s="137" t="s">
+      <c r="E55" s="141"/>
+      <c r="F55" s="140" t="s">
         <v>37</v>
       </c>
-      <c r="G55" s="138"/>
-      <c r="H55" s="160" t="s">
+      <c r="G55" s="141"/>
+      <c r="H55" s="138" t="s">
         <v>38</v>
       </c>
-      <c r="I55" s="160"/>
+      <c r="I55" s="138"/>
       <c r="J55" s="117" t="s">
         <v>39</v>
       </c>
@@ -3597,37 +3602,37 @@
       <c r="A56" s="48">
         <v>4</v>
       </c>
-      <c r="B56" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="140"/>
-      <c r="D56" s="148" t="s">
-        <v>66</v>
-      </c>
-      <c r="E56" s="149"/>
-      <c r="F56" s="148" t="s">
+      <c r="B56" s="160" t="s">
         <v>67</v>
       </c>
-      <c r="G56" s="149"/>
+      <c r="C56" s="161"/>
+      <c r="D56" s="150" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="151"/>
+      <c r="F56" s="150" t="s">
+        <v>65</v>
+      </c>
+      <c r="G56" s="151"/>
       <c r="H56" s="156" t="s">
         <v>10</v>
       </c>
       <c r="I56" s="157"/>
       <c r="J56" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="K56" s="161"/>
+        <v>68</v>
+      </c>
+      <c r="K56" s="145"/>
     </row>
     <row r="57" spans="1:11" ht="10.5" customHeight="1">
       <c r="A57" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="141"/>
-      <c r="C57" s="142"/>
-      <c r="D57" s="150"/>
-      <c r="E57" s="151"/>
-      <c r="F57" s="150"/>
-      <c r="G57" s="151"/>
+      <c r="B57" s="162"/>
+      <c r="C57" s="163"/>
+      <c r="D57" s="152"/>
+      <c r="E57" s="153"/>
+      <c r="F57" s="152"/>
+      <c r="G57" s="153"/>
       <c r="H57" s="117" t="s">
         <v>45</v>
       </c>
@@ -3637,39 +3642,39 @@
       <c r="J57" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="K57" s="162"/>
+      <c r="K57" s="146"/>
     </row>
     <row r="58" spans="1:11" ht="10.5" customHeight="1">
       <c r="A58" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="B58" s="141"/>
-      <c r="C58" s="142"/>
-      <c r="D58" s="150"/>
-      <c r="E58" s="151"/>
-      <c r="F58" s="150"/>
-      <c r="G58" s="151"/>
+        <v>69</v>
+      </c>
+      <c r="B58" s="162"/>
+      <c r="C58" s="163"/>
+      <c r="D58" s="152"/>
+      <c r="E58" s="153"/>
+      <c r="F58" s="152"/>
+      <c r="G58" s="153"/>
       <c r="H58" s="50" t="s">
         <v>49</v>
       </c>
       <c r="I58" s="50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J58" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="K58" s="162"/>
+        <v>57</v>
+      </c>
+      <c r="K58" s="146"/>
     </row>
     <row r="59" spans="1:11" ht="10.5" customHeight="1">
       <c r="A59" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="141"/>
-      <c r="C59" s="142"/>
-      <c r="D59" s="150"/>
-      <c r="E59" s="151"/>
-      <c r="F59" s="150"/>
-      <c r="G59" s="151"/>
+      <c r="B59" s="162"/>
+      <c r="C59" s="163"/>
+      <c r="D59" s="152"/>
+      <c r="E59" s="153"/>
+      <c r="F59" s="152"/>
+      <c r="G59" s="153"/>
       <c r="H59" s="117" t="s">
         <v>51</v>
       </c>
@@ -3677,47 +3682,47 @@
         <v>52</v>
       </c>
       <c r="J59" s="117"/>
-      <c r="K59" s="162"/>
+      <c r="K59" s="146"/>
     </row>
     <row r="60" spans="1:11" ht="10.5" customHeight="1">
       <c r="A60" s="51">
         <v>823</v>
       </c>
-      <c r="B60" s="143"/>
-      <c r="C60" s="144"/>
-      <c r="D60" s="152"/>
-      <c r="E60" s="153"/>
-      <c r="F60" s="152"/>
-      <c r="G60" s="153"/>
+      <c r="B60" s="164"/>
+      <c r="C60" s="165"/>
+      <c r="D60" s="154"/>
+      <c r="E60" s="155"/>
+      <c r="F60" s="154"/>
+      <c r="G60" s="155"/>
       <c r="H60" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I60" s="50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J60" s="48"/>
-      <c r="K60" s="163"/>
+      <c r="K60" s="147"/>
     </row>
     <row r="61" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A61" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B61" s="137" t="s">
+      <c r="B61" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="138"/>
-      <c r="D61" s="137" t="s">
+      <c r="C61" s="141"/>
+      <c r="D61" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="138"/>
-      <c r="F61" s="137" t="s">
+      <c r="E61" s="141"/>
+      <c r="F61" s="140" t="s">
         <v>37</v>
       </c>
-      <c r="G61" s="138"/>
-      <c r="H61" s="160" t="s">
+      <c r="G61" s="141"/>
+      <c r="H61" s="138" t="s">
         <v>38</v>
       </c>
-      <c r="I61" s="160"/>
+      <c r="I61" s="138"/>
       <c r="J61" s="117" t="s">
         <v>39</v>
       </c>
@@ -3729,37 +3734,37 @@
       <c r="A62" s="48">
         <v>5</v>
       </c>
-      <c r="B62" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C62" s="140"/>
-      <c r="D62" s="148" t="s">
-        <v>66</v>
-      </c>
-      <c r="E62" s="149"/>
-      <c r="F62" s="148" t="s">
+      <c r="B62" s="160" t="s">
         <v>67</v>
       </c>
-      <c r="G62" s="149"/>
+      <c r="C62" s="161"/>
+      <c r="D62" s="150" t="s">
+        <v>64</v>
+      </c>
+      <c r="E62" s="151"/>
+      <c r="F62" s="150" t="s">
+        <v>65</v>
+      </c>
+      <c r="G62" s="151"/>
       <c r="H62" s="156" t="s">
         <v>10</v>
       </c>
       <c r="I62" s="157"/>
       <c r="J62" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="K62" s="161"/>
+        <v>68</v>
+      </c>
+      <c r="K62" s="145"/>
     </row>
     <row r="63" spans="1:11" ht="10.5" customHeight="1">
       <c r="A63" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="141"/>
-      <c r="C63" s="142"/>
-      <c r="D63" s="150"/>
-      <c r="E63" s="151"/>
-      <c r="F63" s="150"/>
-      <c r="G63" s="151"/>
+      <c r="B63" s="162"/>
+      <c r="C63" s="163"/>
+      <c r="D63" s="152"/>
+      <c r="E63" s="153"/>
+      <c r="F63" s="152"/>
+      <c r="G63" s="153"/>
       <c r="H63" s="117" t="s">
         <v>45</v>
       </c>
@@ -3769,39 +3774,39 @@
       <c r="J63" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="K63" s="162"/>
+      <c r="K63" s="146"/>
     </row>
     <row r="64" spans="1:11" ht="10.5" customHeight="1">
       <c r="A64" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="B64" s="141"/>
-      <c r="C64" s="142"/>
-      <c r="D64" s="150"/>
-      <c r="E64" s="151"/>
-      <c r="F64" s="150"/>
-      <c r="G64" s="151"/>
+        <v>69</v>
+      </c>
+      <c r="B64" s="162"/>
+      <c r="C64" s="163"/>
+      <c r="D64" s="152"/>
+      <c r="E64" s="153"/>
+      <c r="F64" s="152"/>
+      <c r="G64" s="153"/>
       <c r="H64" s="50" t="s">
         <v>49</v>
       </c>
       <c r="I64" s="50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J64" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="K64" s="162"/>
+        <v>57</v>
+      </c>
+      <c r="K64" s="146"/>
     </row>
     <row r="65" spans="1:11" ht="10.5" customHeight="1">
       <c r="A65" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="141"/>
-      <c r="C65" s="142"/>
-      <c r="D65" s="150"/>
-      <c r="E65" s="151"/>
-      <c r="F65" s="150"/>
-      <c r="G65" s="151"/>
+      <c r="B65" s="162"/>
+      <c r="C65" s="163"/>
+      <c r="D65" s="152"/>
+      <c r="E65" s="153"/>
+      <c r="F65" s="152"/>
+      <c r="G65" s="153"/>
       <c r="H65" s="117" t="s">
         <v>51</v>
       </c>
@@ -3809,26 +3814,26 @@
         <v>52</v>
       </c>
       <c r="J65" s="117"/>
-      <c r="K65" s="162"/>
+      <c r="K65" s="146"/>
     </row>
     <row r="66" spans="1:11" ht="10.5" customHeight="1">
       <c r="A66" s="51">
         <v>823</v>
       </c>
-      <c r="B66" s="143"/>
-      <c r="C66" s="144"/>
-      <c r="D66" s="152"/>
-      <c r="E66" s="153"/>
-      <c r="F66" s="152"/>
-      <c r="G66" s="153"/>
+      <c r="B66" s="164"/>
+      <c r="C66" s="165"/>
+      <c r="D66" s="154"/>
+      <c r="E66" s="155"/>
+      <c r="F66" s="154"/>
+      <c r="G66" s="155"/>
       <c r="H66" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I66" s="50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J66" s="48"/>
-      <c r="K66" s="163"/>
+      <c r="K66" s="147"/>
     </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
       <c r="A67" s="62"/>
@@ -4042,6 +4047,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="B50:C54"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="B56:C60"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B62:C66"/>
+    <mergeCell ref="D56:E60"/>
+    <mergeCell ref="D62:E66"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B48:K48"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:E25"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K62:K66"/>
+    <mergeCell ref="F56:G60"/>
+    <mergeCell ref="K56:K60"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="F62:G66"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H55:I55"/>
     <mergeCell ref="H8:I8"/>
@@ -4058,44 +4101,6 @@
     <mergeCell ref="D50:E54"/>
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="F50:G54"/>
-    <mergeCell ref="K62:K66"/>
-    <mergeCell ref="F56:G60"/>
-    <mergeCell ref="K56:K60"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B48:K48"/>
-    <mergeCell ref="D15:E19"/>
-    <mergeCell ref="B15:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B21:C25"/>
-    <mergeCell ref="D21:E25"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B62:C66"/>
-    <mergeCell ref="D56:E60"/>
-    <mergeCell ref="D62:E66"/>
-    <mergeCell ref="F62:G66"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="B50:C54"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="B56:C60"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H62:I62">

</xml_diff>

<commit_message>
test chuc nang thong tin
</commit_message>
<xml_diff>
--- a/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -331,13 +331,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">Không có tham số dòng lệnh
-</t>
-  </si>
-  <si>
-    <t>1. Gõ duy nhất tên chương trình, không có tham số dòng lệnh</t>
-  </si>
-  <si>
     <t>Chạy được</t>
   </si>
   <si>
@@ -451,6 +444,13 @@
   </si>
   <si>
     <t>LongLN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chức năng thông tin
+</t>
+  </si>
+  <si>
+    <t>Click vào button thông tin để xem thông tin của trang web, sẽ hiển thị ra một thông báo về thông tin của trang web</t>
   </si>
 </sst>
 </file>
@@ -1290,95 +1290,95 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2840,8 +2840,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:C25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2976,39 +2976,39 @@
       <c r="A7" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="137" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="137"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="137"/>
-      <c r="H7" s="137"/>
-      <c r="I7" s="137"/>
-      <c r="J7" s="137"/>
-      <c r="K7" s="137"/>
+      <c r="B7" s="165" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="165"/>
+      <c r="H7" s="165"/>
+      <c r="I7" s="165"/>
+      <c r="J7" s="165"/>
+      <c r="K7" s="165"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="140" t="s">
+      <c r="B8" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="141"/>
-      <c r="D8" s="140" t="s">
+      <c r="C8" s="138"/>
+      <c r="D8" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="141"/>
-      <c r="F8" s="140" t="s">
+      <c r="E8" s="138"/>
+      <c r="F8" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="141"/>
-      <c r="H8" s="139" t="s">
+      <c r="G8" s="138"/>
+      <c r="H8" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="139"/>
+      <c r="I8" s="161"/>
       <c r="J8" s="118" t="s">
         <v>39</v>
       </c>
@@ -3020,119 +3020,119 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="160" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="161"/>
-      <c r="D9" s="150" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="151"/>
+      <c r="B9" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="140"/>
+      <c r="D9" s="149" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="150"/>
       <c r="F9" s="120" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="121"/>
-      <c r="H9" s="148" t="s">
+      <c r="H9" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="149"/>
+      <c r="I9" s="156"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="145"/>
+      <c r="K9" s="162"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="117" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="162"/>
-      <c r="C10" s="163"/>
-      <c r="D10" s="152"/>
-      <c r="E10" s="153"/>
+        <v>42</v>
+      </c>
+      <c r="B10" s="141"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="152"/>
       <c r="F10" s="122"/>
       <c r="G10" s="123"/>
       <c r="H10" s="117" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="117" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="146"/>
+      <c r="K10" s="163"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="162"/>
-      <c r="C11" s="163"/>
-      <c r="D11" s="152"/>
-      <c r="E11" s="153"/>
+        <v>46</v>
+      </c>
+      <c r="B11" s="141"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="152"/>
       <c r="F11" s="122"/>
       <c r="G11" s="123"/>
       <c r="H11" s="50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="146"/>
+      <c r="K11" s="163"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="117" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="162"/>
-      <c r="C12" s="163"/>
-      <c r="D12" s="152"/>
-      <c r="E12" s="153"/>
+        <v>48</v>
+      </c>
+      <c r="B12" s="141"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="152"/>
       <c r="F12" s="122"/>
       <c r="G12" s="123"/>
       <c r="H12" s="117" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I12" s="117" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J12" s="117"/>
-      <c r="K12" s="146"/>
+      <c r="K12" s="163"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>981</v>
       </c>
-      <c r="B13" s="164"/>
-      <c r="C13" s="165"/>
-      <c r="D13" s="154"/>
-      <c r="E13" s="155"/>
+      <c r="B13" s="143"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="153"/>
+      <c r="E13" s="154"/>
       <c r="F13" s="124"/>
       <c r="G13" s="125"/>
       <c r="H13" s="53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="147"/>
+      <c r="K13" s="164"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="143" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="144"/>
-      <c r="D14" s="143" t="s">
+      <c r="B14" s="146" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="147"/>
+      <c r="D14" s="146" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="144"/>
-      <c r="F14" s="143" t="s">
+      <c r="E14" s="147"/>
+      <c r="F14" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="144"/>
-      <c r="H14" s="166" t="s">
+      <c r="G14" s="147"/>
+      <c r="H14" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="166"/>
+      <c r="I14" s="145"/>
       <c r="J14" s="126" t="s">
         <v>39</v>
       </c>
@@ -3144,123 +3144,123 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="160" t="s">
+      <c r="B15" s="139" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="140"/>
+      <c r="D15" s="149" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="150"/>
+      <c r="F15" s="120" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="161"/>
-      <c r="D15" s="150" t="s">
+      <c r="G15" s="121"/>
+      <c r="H15" s="157" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="158"/>
+      <c r="J15" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="151"/>
-      <c r="F15" s="120" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="121"/>
-      <c r="H15" s="156" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="157"/>
-      <c r="J15" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="K15" s="145"/>
+      <c r="K15" s="162"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="126" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="162"/>
-      <c r="C16" s="163"/>
-      <c r="D16" s="152"/>
-      <c r="E16" s="153"/>
+        <v>42</v>
+      </c>
+      <c r="B16" s="141"/>
+      <c r="C16" s="142"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="152"/>
       <c r="F16" s="122"/>
       <c r="G16" s="123"/>
       <c r="H16" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="126" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="126" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" s="146"/>
+      <c r="K16" s="163"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="162"/>
-      <c r="C17" s="163"/>
-      <c r="D17" s="152"/>
-      <c r="E17" s="153"/>
+        <v>53</v>
+      </c>
+      <c r="B17" s="141"/>
+      <c r="C17" s="142"/>
+      <c r="D17" s="151"/>
+      <c r="E17" s="152"/>
       <c r="F17" s="122"/>
       <c r="G17" s="123"/>
       <c r="H17" s="50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="K17" s="146"/>
+        <v>77</v>
+      </c>
+      <c r="K17" s="163"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="126" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="162"/>
-      <c r="C18" s="163"/>
-      <c r="D18" s="152"/>
-      <c r="E18" s="153"/>
+        <v>48</v>
+      </c>
+      <c r="B18" s="141"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="151"/>
+      <c r="E18" s="152"/>
       <c r="F18" s="122"/>
       <c r="G18" s="123"/>
       <c r="H18" s="126" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I18" s="126" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J18" s="126"/>
-      <c r="K18" s="146"/>
+      <c r="K18" s="163"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>921</v>
       </c>
-      <c r="B19" s="164"/>
-      <c r="C19" s="165"/>
-      <c r="D19" s="154"/>
-      <c r="E19" s="155"/>
+      <c r="B19" s="143"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="153"/>
+      <c r="E19" s="154"/>
       <c r="F19" s="124"/>
       <c r="G19" s="125"/>
       <c r="H19" s="50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="146"/>
+      <c r="K19" s="163"/>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A20" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="141"/>
-      <c r="D20" s="140" t="s">
+      <c r="C20" s="138"/>
+      <c r="D20" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="141"/>
-      <c r="F20" s="140" t="s">
+      <c r="E20" s="138"/>
+      <c r="F20" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="141"/>
-      <c r="H20" s="139" t="s">
+      <c r="G20" s="138"/>
+      <c r="H20" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="139"/>
+      <c r="I20" s="161"/>
       <c r="J20" s="128" t="s">
         <v>39</v>
       </c>
@@ -3272,98 +3272,98 @@
       <c r="A21" s="48">
         <v>1</v>
       </c>
-      <c r="B21" s="160" t="s">
+      <c r="B21" s="139" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="140"/>
+      <c r="D21" s="149" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="150"/>
+      <c r="F21" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="161"/>
-      <c r="D21" s="150" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="151"/>
-      <c r="F21" s="129" t="s">
-        <v>43</v>
-      </c>
       <c r="G21" s="130"/>
-      <c r="H21" s="148" t="s">
+      <c r="H21" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="149"/>
+      <c r="I21" s="156"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="145"/>
+      <c r="K21" s="162"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="127" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="162"/>
-      <c r="C22" s="163"/>
-      <c r="D22" s="152"/>
-      <c r="E22" s="153"/>
+        <v>42</v>
+      </c>
+      <c r="B22" s="141"/>
+      <c r="C22" s="142"/>
+      <c r="D22" s="151"/>
+      <c r="E22" s="152"/>
       <c r="F22" s="131"/>
       <c r="G22" s="132"/>
       <c r="H22" s="127" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="127" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="127" t="s">
         <v>45</v>
       </c>
-      <c r="I22" s="127" t="s">
-        <v>46</v>
-      </c>
-      <c r="J22" s="127" t="s">
-        <v>47</v>
-      </c>
-      <c r="K22" s="146"/>
+      <c r="K22" s="163"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="162"/>
-      <c r="C23" s="163"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="153"/>
+        <v>46</v>
+      </c>
+      <c r="B23" s="141"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="151"/>
+      <c r="E23" s="152"/>
       <c r="F23" s="131"/>
       <c r="G23" s="132"/>
       <c r="H23" s="50" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="146"/>
+      <c r="K23" s="163"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="127" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="162"/>
-      <c r="C24" s="163"/>
-      <c r="D24" s="152"/>
-      <c r="E24" s="153"/>
+        <v>48</v>
+      </c>
+      <c r="B24" s="141"/>
+      <c r="C24" s="142"/>
+      <c r="D24" s="151"/>
+      <c r="E24" s="152"/>
       <c r="F24" s="131"/>
       <c r="G24" s="132"/>
       <c r="H24" s="127" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I24" s="127" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J24" s="127"/>
-      <c r="K24" s="146"/>
+      <c r="K24" s="163"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>981</v>
       </c>
-      <c r="B25" s="164"/>
-      <c r="C25" s="165"/>
-      <c r="D25" s="154"/>
-      <c r="E25" s="155"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="154"/>
       <c r="F25" s="133"/>
       <c r="G25" s="134"/>
-      <c r="H25" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="53"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="147"/>
+      <c r="H25" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="50"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="164"/>
     </row>
     <row r="40" spans="1:11" s="58" customFormat="1">
       <c r="A40" s="62"/>
@@ -3416,58 +3416,58 @@
     </row>
     <row r="47" spans="1:11" ht="10.5" customHeight="1">
       <c r="A47" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="142" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" s="142"/>
-      <c r="D47" s="137"/>
-      <c r="E47" s="137"/>
-      <c r="F47" s="137"/>
-      <c r="G47" s="137"/>
-      <c r="H47" s="137"/>
-      <c r="I47" s="137"/>
-      <c r="J47" s="137"/>
-      <c r="K47" s="137"/>
+        <v>57</v>
+      </c>
+      <c r="B47" s="166" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="166"/>
+      <c r="D47" s="165"/>
+      <c r="E47" s="165"/>
+      <c r="F47" s="165"/>
+      <c r="G47" s="165"/>
+      <c r="H47" s="165"/>
+      <c r="I47" s="165"/>
+      <c r="J47" s="165"/>
+      <c r="K47" s="165"/>
     </row>
     <row r="48" spans="1:11" ht="10.5" customHeight="1">
       <c r="A48" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="158" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="158"/>
-      <c r="D48" s="159"/>
-      <c r="E48" s="159"/>
-      <c r="F48" s="159"/>
-      <c r="G48" s="159"/>
-      <c r="H48" s="159"/>
-      <c r="I48" s="159"/>
-      <c r="J48" s="159"/>
-      <c r="K48" s="159"/>
+        <v>59</v>
+      </c>
+      <c r="B48" s="159" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="159"/>
+      <c r="D48" s="160"/>
+      <c r="E48" s="160"/>
+      <c r="F48" s="160"/>
+      <c r="G48" s="160"/>
+      <c r="H48" s="160"/>
+      <c r="I48" s="160"/>
+      <c r="J48" s="160"/>
+      <c r="K48" s="160"/>
     </row>
     <row r="49" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A49" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="B49" s="143" t="s">
-        <v>54</v>
-      </c>
-      <c r="C49" s="144"/>
-      <c r="D49" s="143" t="s">
+      <c r="B49" s="146" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="147"/>
+      <c r="D49" s="146" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="144"/>
-      <c r="F49" s="143" t="s">
+      <c r="E49" s="147"/>
+      <c r="F49" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="G49" s="144"/>
-      <c r="H49" s="166" t="s">
+      <c r="G49" s="147"/>
+      <c r="H49" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="I49" s="166"/>
+      <c r="I49" s="145"/>
       <c r="J49" s="126" t="s">
         <v>39</v>
       </c>
@@ -3480,117 +3480,117 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B50" s="160" t="s">
+      <c r="B50" s="139" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="140"/>
+      <c r="D50" s="149" t="s">
+        <v>62</v>
+      </c>
+      <c r="E50" s="150"/>
+      <c r="F50" s="149" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="161"/>
-      <c r="D50" s="150" t="s">
-        <v>64</v>
-      </c>
-      <c r="E50" s="151"/>
-      <c r="F50" s="150" t="s">
-        <v>65</v>
-      </c>
-      <c r="G50" s="151"/>
-      <c r="H50" s="148" t="s">
+      <c r="G50" s="150"/>
+      <c r="H50" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="I50" s="149"/>
+      <c r="I50" s="156"/>
       <c r="J50" s="48"/>
-      <c r="K50" s="145"/>
+      <c r="K50" s="162"/>
     </row>
     <row r="51" spans="1:11" ht="10.5" customHeight="1">
       <c r="A51" s="126" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="141"/>
+      <c r="C51" s="142"/>
+      <c r="D51" s="151"/>
+      <c r="E51" s="152"/>
+      <c r="F51" s="151"/>
+      <c r="G51" s="152"/>
+      <c r="H51" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="I51" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="162"/>
-      <c r="C51" s="163"/>
-      <c r="D51" s="152"/>
-      <c r="E51" s="153"/>
-      <c r="F51" s="152"/>
-      <c r="G51" s="153"/>
-      <c r="H51" s="126" t="s">
+      <c r="J51" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="I51" s="126" t="s">
-        <v>46</v>
-      </c>
-      <c r="J51" s="126" t="s">
-        <v>47</v>
-      </c>
-      <c r="K51" s="146"/>
+      <c r="K51" s="163"/>
     </row>
     <row r="52" spans="1:11" ht="10.5" customHeight="1">
       <c r="A52" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="B52" s="162"/>
-      <c r="C52" s="163"/>
-      <c r="D52" s="152"/>
-      <c r="E52" s="153"/>
-      <c r="F52" s="152"/>
-      <c r="G52" s="153"/>
+        <v>64</v>
+      </c>
+      <c r="B52" s="141"/>
+      <c r="C52" s="142"/>
+      <c r="D52" s="151"/>
+      <c r="E52" s="152"/>
+      <c r="F52" s="151"/>
+      <c r="G52" s="152"/>
       <c r="H52" s="50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I52" s="50"/>
       <c r="J52" s="48"/>
-      <c r="K52" s="146"/>
+      <c r="K52" s="163"/>
     </row>
     <row r="53" spans="1:11" ht="10.5" customHeight="1">
       <c r="A53" s="126" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" s="162"/>
-      <c r="C53" s="163"/>
-      <c r="D53" s="152"/>
-      <c r="E53" s="153"/>
-      <c r="F53" s="152"/>
-      <c r="G53" s="153"/>
+        <v>48</v>
+      </c>
+      <c r="B53" s="141"/>
+      <c r="C53" s="142"/>
+      <c r="D53" s="151"/>
+      <c r="E53" s="152"/>
+      <c r="F53" s="151"/>
+      <c r="G53" s="152"/>
       <c r="H53" s="126" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I53" s="126"/>
       <c r="J53" s="126"/>
-      <c r="K53" s="146"/>
+      <c r="K53" s="163"/>
     </row>
     <row r="54" spans="1:11" ht="10.5" customHeight="1">
       <c r="A54" s="51">
         <v>922</v>
       </c>
-      <c r="B54" s="164"/>
-      <c r="C54" s="165"/>
-      <c r="D54" s="154"/>
-      <c r="E54" s="155"/>
-      <c r="F54" s="154"/>
-      <c r="G54" s="155"/>
+      <c r="B54" s="143"/>
+      <c r="C54" s="144"/>
+      <c r="D54" s="153"/>
+      <c r="E54" s="154"/>
+      <c r="F54" s="153"/>
+      <c r="G54" s="154"/>
       <c r="H54" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I54" s="50"/>
       <c r="J54" s="48"/>
-      <c r="K54" s="147"/>
+      <c r="K54" s="164"/>
     </row>
     <row r="55" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A55" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B55" s="140" t="s">
+      <c r="B55" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="141"/>
-      <c r="D55" s="140" t="s">
+      <c r="C55" s="138"/>
+      <c r="D55" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E55" s="141"/>
-      <c r="F55" s="140" t="s">
+      <c r="E55" s="138"/>
+      <c r="F55" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G55" s="141"/>
-      <c r="H55" s="138" t="s">
+      <c r="G55" s="138"/>
+      <c r="H55" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="I55" s="138"/>
+      <c r="I55" s="148"/>
       <c r="J55" s="117" t="s">
         <v>39</v>
       </c>
@@ -3602,127 +3602,127 @@
       <c r="A56" s="48">
         <v>4</v>
       </c>
-      <c r="B56" s="160" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" s="161"/>
-      <c r="D56" s="150" t="s">
-        <v>64</v>
-      </c>
-      <c r="E56" s="151"/>
-      <c r="F56" s="150" t="s">
+      <c r="B56" s="139" t="s">
         <v>65</v>
       </c>
-      <c r="G56" s="151"/>
-      <c r="H56" s="156" t="s">
+      <c r="C56" s="140"/>
+      <c r="D56" s="149" t="s">
+        <v>62</v>
+      </c>
+      <c r="E56" s="150"/>
+      <c r="F56" s="149" t="s">
+        <v>63</v>
+      </c>
+      <c r="G56" s="150"/>
+      <c r="H56" s="157" t="s">
         <v>10</v>
       </c>
-      <c r="I56" s="157"/>
+      <c r="I56" s="158"/>
       <c r="J56" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="K56" s="145"/>
+        <v>66</v>
+      </c>
+      <c r="K56" s="162"/>
     </row>
     <row r="57" spans="1:11" ht="10.5" customHeight="1">
       <c r="A57" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="141"/>
+      <c r="C57" s="142"/>
+      <c r="D57" s="151"/>
+      <c r="E57" s="152"/>
+      <c r="F57" s="151"/>
+      <c r="G57" s="152"/>
+      <c r="H57" s="117" t="s">
+        <v>43</v>
+      </c>
+      <c r="I57" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="162"/>
-      <c r="C57" s="163"/>
-      <c r="D57" s="152"/>
-      <c r="E57" s="153"/>
-      <c r="F57" s="152"/>
-      <c r="G57" s="153"/>
-      <c r="H57" s="117" t="s">
+      <c r="J57" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="I57" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="J57" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="K57" s="146"/>
+      <c r="K57" s="163"/>
     </row>
     <row r="58" spans="1:11" ht="10.5" customHeight="1">
       <c r="A58" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="B58" s="162"/>
-      <c r="C58" s="163"/>
-      <c r="D58" s="152"/>
-      <c r="E58" s="153"/>
-      <c r="F58" s="152"/>
-      <c r="G58" s="153"/>
+        <v>67</v>
+      </c>
+      <c r="B58" s="141"/>
+      <c r="C58" s="142"/>
+      <c r="D58" s="151"/>
+      <c r="E58" s="152"/>
+      <c r="F58" s="151"/>
+      <c r="G58" s="152"/>
       <c r="H58" s="50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I58" s="50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J58" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="K58" s="146"/>
+        <v>55</v>
+      </c>
+      <c r="K58" s="163"/>
     </row>
     <row r="59" spans="1:11" ht="10.5" customHeight="1">
       <c r="A59" s="117" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="141"/>
+      <c r="C59" s="142"/>
+      <c r="D59" s="151"/>
+      <c r="E59" s="152"/>
+      <c r="F59" s="151"/>
+      <c r="G59" s="152"/>
+      <c r="H59" s="117" t="s">
+        <v>49</v>
+      </c>
+      <c r="I59" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="162"/>
-      <c r="C59" s="163"/>
-      <c r="D59" s="152"/>
-      <c r="E59" s="153"/>
-      <c r="F59" s="152"/>
-      <c r="G59" s="153"/>
-      <c r="H59" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="I59" s="117" t="s">
-        <v>52</v>
-      </c>
       <c r="J59" s="117"/>
-      <c r="K59" s="146"/>
+      <c r="K59" s="163"/>
     </row>
     <row r="60" spans="1:11" ht="10.5" customHeight="1">
       <c r="A60" s="51">
         <v>823</v>
       </c>
-      <c r="B60" s="164"/>
-      <c r="C60" s="165"/>
-      <c r="D60" s="154"/>
-      <c r="E60" s="155"/>
-      <c r="F60" s="154"/>
-      <c r="G60" s="155"/>
+      <c r="B60" s="143"/>
+      <c r="C60" s="144"/>
+      <c r="D60" s="153"/>
+      <c r="E60" s="154"/>
+      <c r="F60" s="153"/>
+      <c r="G60" s="154"/>
       <c r="H60" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I60" s="50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J60" s="48"/>
-      <c r="K60" s="147"/>
+      <c r="K60" s="164"/>
     </row>
     <row r="61" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A61" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B61" s="140" t="s">
+      <c r="B61" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="141"/>
-      <c r="D61" s="140" t="s">
+      <c r="C61" s="138"/>
+      <c r="D61" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="141"/>
-      <c r="F61" s="140" t="s">
+      <c r="E61" s="138"/>
+      <c r="F61" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="G61" s="141"/>
-      <c r="H61" s="138" t="s">
+      <c r="G61" s="138"/>
+      <c r="H61" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="I61" s="138"/>
+      <c r="I61" s="148"/>
       <c r="J61" s="117" t="s">
         <v>39</v>
       </c>
@@ -3734,106 +3734,106 @@
       <c r="A62" s="48">
         <v>5</v>
       </c>
-      <c r="B62" s="160" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="161"/>
-      <c r="D62" s="150" t="s">
-        <v>64</v>
-      </c>
-      <c r="E62" s="151"/>
-      <c r="F62" s="150" t="s">
+      <c r="B62" s="139" t="s">
         <v>65</v>
       </c>
-      <c r="G62" s="151"/>
-      <c r="H62" s="156" t="s">
+      <c r="C62" s="140"/>
+      <c r="D62" s="149" t="s">
+        <v>62</v>
+      </c>
+      <c r="E62" s="150"/>
+      <c r="F62" s="149" t="s">
+        <v>63</v>
+      </c>
+      <c r="G62" s="150"/>
+      <c r="H62" s="157" t="s">
         <v>10</v>
       </c>
-      <c r="I62" s="157"/>
+      <c r="I62" s="158"/>
       <c r="J62" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="K62" s="145"/>
+        <v>66</v>
+      </c>
+      <c r="K62" s="162"/>
     </row>
     <row r="63" spans="1:11" ht="10.5" customHeight="1">
       <c r="A63" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="141"/>
+      <c r="C63" s="142"/>
+      <c r="D63" s="151"/>
+      <c r="E63" s="152"/>
+      <c r="F63" s="151"/>
+      <c r="G63" s="152"/>
+      <c r="H63" s="117" t="s">
+        <v>43</v>
+      </c>
+      <c r="I63" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="162"/>
-      <c r="C63" s="163"/>
-      <c r="D63" s="152"/>
-      <c r="E63" s="153"/>
-      <c r="F63" s="152"/>
-      <c r="G63" s="153"/>
-      <c r="H63" s="117" t="s">
+      <c r="J63" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="I63" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="J63" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="K63" s="146"/>
+      <c r="K63" s="163"/>
     </row>
     <row r="64" spans="1:11" ht="10.5" customHeight="1">
       <c r="A64" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" s="162"/>
-      <c r="C64" s="163"/>
-      <c r="D64" s="152"/>
-      <c r="E64" s="153"/>
-      <c r="F64" s="152"/>
-      <c r="G64" s="153"/>
+        <v>67</v>
+      </c>
+      <c r="B64" s="141"/>
+      <c r="C64" s="142"/>
+      <c r="D64" s="151"/>
+      <c r="E64" s="152"/>
+      <c r="F64" s="151"/>
+      <c r="G64" s="152"/>
       <c r="H64" s="50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I64" s="50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J64" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="K64" s="146"/>
+        <v>55</v>
+      </c>
+      <c r="K64" s="163"/>
     </row>
     <row r="65" spans="1:11" ht="10.5" customHeight="1">
       <c r="A65" s="117" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" s="141"/>
+      <c r="C65" s="142"/>
+      <c r="D65" s="151"/>
+      <c r="E65" s="152"/>
+      <c r="F65" s="151"/>
+      <c r="G65" s="152"/>
+      <c r="H65" s="117" t="s">
+        <v>49</v>
+      </c>
+      <c r="I65" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="162"/>
-      <c r="C65" s="163"/>
-      <c r="D65" s="152"/>
-      <c r="E65" s="153"/>
-      <c r="F65" s="152"/>
-      <c r="G65" s="153"/>
-      <c r="H65" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="I65" s="117" t="s">
-        <v>52</v>
-      </c>
       <c r="J65" s="117"/>
-      <c r="K65" s="146"/>
+      <c r="K65" s="163"/>
     </row>
     <row r="66" spans="1:11" ht="10.5" customHeight="1">
       <c r="A66" s="51">
         <v>823</v>
       </c>
-      <c r="B66" s="164"/>
-      <c r="C66" s="165"/>
-      <c r="D66" s="154"/>
-      <c r="E66" s="155"/>
-      <c r="F66" s="154"/>
-      <c r="G66" s="155"/>
+      <c r="B66" s="143"/>
+      <c r="C66" s="144"/>
+      <c r="D66" s="153"/>
+      <c r="E66" s="154"/>
+      <c r="F66" s="153"/>
+      <c r="G66" s="154"/>
       <c r="H66" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I66" s="50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J66" s="48"/>
-      <c r="K66" s="147"/>
+      <c r="K66" s="164"/>
     </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
       <c r="A67" s="62"/>
@@ -4047,19 +4047,30 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="B50:C54"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="B56:C60"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B47:K47"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="D50:E54"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G54"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K62:K66"/>
+    <mergeCell ref="F56:G60"/>
+    <mergeCell ref="K56:K60"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="F62:G66"/>
     <mergeCell ref="B62:C66"/>
     <mergeCell ref="D56:E60"/>
     <mergeCell ref="D62:E66"/>
@@ -4076,31 +4087,20 @@
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="B21:C25"/>
     <mergeCell ref="D21:E25"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="B56:C60"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="B50:C54"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B49:C49"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="K62:K66"/>
-    <mergeCell ref="F56:G60"/>
-    <mergeCell ref="K56:K60"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="F62:G66"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B47:K47"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="D50:E54"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G54"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H62:I62">

</xml_diff>

<commit_message>
test chuc nang tim kiem noi dung theo noi dung phe duyet
</commit_message>
<xml_diff>
--- a/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -36,7 +36,7 @@
     <author>Nguyen Duc Tien</author>
   </authors>
   <commentList>
-    <comment ref="B48" authorId="0" shapeId="0">
+    <comment ref="B27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H49" authorId="0" shapeId="0">
+    <comment ref="H28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J49" authorId="0" shapeId="0">
+    <comment ref="J28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A50" authorId="0" shapeId="0">
+    <comment ref="A29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H51" authorId="0" shapeId="0">
+    <comment ref="H30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I51" authorId="0" shapeId="0">
+    <comment ref="I30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J51" authorId="0" shapeId="0">
+    <comment ref="J30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A52" authorId="0" shapeId="0">
+    <comment ref="A31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H53" authorId="0" shapeId="0">
+    <comment ref="H32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I53" authorId="0" shapeId="0">
+    <comment ref="I32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A54" authorId="0" shapeId="0">
+    <comment ref="A33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -346,9 +346,6 @@
     <t>Repairer</t>
   </si>
   <si>
-    <t>1.1-1</t>
-  </si>
-  <si>
     <t>DinhPX</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
     <t>Subtopic(abnormality)</t>
   </si>
   <si>
-    <t>1.2.1-1</t>
-  </si>
-  <si>
     <t>AnhDV</t>
   </si>
   <si>
@@ -382,16 +376,7 @@
     <t>2.</t>
   </si>
   <si>
-    <t>Test với tham số chỉ định</t>
-  </si>
-  <si>
     <t>2.1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test với tham số chỉ định \ Test với tham số -r </t>
-  </si>
-  <si>
-    <t>File Mpeg có thời lượng 3s</t>
   </si>
   <si>
     <t>1. Add film mpeg
@@ -415,9 +400,6 @@
     <t>1.1-2</t>
   </si>
   <si>
-    <t>Test chức năng</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chức năng xem
 </t>
   </si>
@@ -451,6 +433,42 @@
   </si>
   <si>
     <t>Click vào button thông tin để xem thông tin của trang web, sẽ hiển thị ra một thông báo về thông tin của trang web</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Trang web confession</t>
+  </si>
+  <si>
+    <t>Test chức năng về phía khách hàng</t>
+  </si>
+  <si>
+    <t>Test chức năng về phía quản trị</t>
+  </si>
+  <si>
+    <t>Test với chức năng tìm kiếm</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nội dung theo nội dung phê duyệt</t>
+  </si>
+  <si>
+    <t>Không tìm kiếm được</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm nội dung theo ngày tạo
+</t>
+  </si>
+  <si>
+    <t>1. Gõ nội dung
+2. Chọn tiêu chí sắp xếp theo nội dung phê duyệt
+3. Lọc</t>
   </si>
 </sst>
 </file>
@@ -961,7 +979,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1283,6 +1301,9 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1290,12 +1311,72 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1314,70 +1395,13 @@
     <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1900,13 +1924,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="135" t="s">
+      <c r="O6" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135"/>
+      <c r="P6" s="136"/>
+      <c r="Q6" s="136"/>
+      <c r="R6" s="136"/>
+      <c r="S6" s="136"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -1916,11 +1940,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="135"/>
-      <c r="R7" s="135"/>
-      <c r="S7" s="135"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="136"/>
+      <c r="R7" s="136"/>
+      <c r="S7" s="136"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -1975,12 +1999,12 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="136">
+      <c r="E11" s="137">
         <f ca="1">TODAY()</f>
         <v>43449</v>
       </c>
-      <c r="F11" s="136"/>
-      <c r="G11" s="136"/>
+      <c r="F11" s="137"/>
+      <c r="G11" s="137"/>
       <c r="H11" s="72"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
@@ -2840,8 +2864,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2857,9 +2881,8 @@
       <c r="A1" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="78" t="str">
-        <f>Overview!E9</f>
-        <v>Hear and Note</v>
+      <c r="B1" s="78" t="s">
+        <v>77</v>
       </c>
       <c r="C1" s="78"/>
       <c r="D1" s="78"/>
@@ -2976,39 +2999,39 @@
       <c r="A7" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="165" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="165"/>
-      <c r="F7" s="165"/>
-      <c r="G7" s="165"/>
-      <c r="H7" s="165"/>
-      <c r="I7" s="165"/>
-      <c r="J7" s="165"/>
-      <c r="K7" s="165"/>
+      <c r="B7" s="138" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="138"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="137" t="s">
+      <c r="B8" s="141" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="138"/>
-      <c r="D8" s="137" t="s">
+      <c r="C8" s="142"/>
+      <c r="D8" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="138"/>
-      <c r="F8" s="137" t="s">
+      <c r="E8" s="142"/>
+      <c r="F8" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="138"/>
-      <c r="H8" s="161" t="s">
+      <c r="G8" s="142"/>
+      <c r="H8" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="161"/>
+      <c r="I8" s="140"/>
       <c r="J8" s="118" t="s">
         <v>39</v>
       </c>
@@ -3020,33 +3043,33 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="149" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="150"/>
+      <c r="B9" s="160" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="161"/>
+      <c r="D9" s="151" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="152"/>
       <c r="F9" s="120" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="121"/>
-      <c r="H9" s="155" t="s">
+      <c r="H9" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="156"/>
+      <c r="I9" s="150"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="162"/>
+      <c r="K9" s="146"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="141"/>
-      <c r="C10" s="142"/>
-      <c r="D10" s="151"/>
-      <c r="E10" s="152"/>
+      <c r="B10" s="162"/>
+      <c r="C10" s="163"/>
+      <c r="D10" s="153"/>
+      <c r="E10" s="154"/>
       <c r="F10" s="122"/>
       <c r="G10" s="123"/>
       <c r="H10" s="117" t="s">
@@ -3058,81 +3081,81 @@
       <c r="J10" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="163"/>
+      <c r="K10" s="147"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="141"/>
-      <c r="C11" s="142"/>
-      <c r="D11" s="151"/>
-      <c r="E11" s="152"/>
+        <v>75</v>
+      </c>
+      <c r="B11" s="162"/>
+      <c r="C11" s="163"/>
+      <c r="D11" s="153"/>
+      <c r="E11" s="154"/>
       <c r="F11" s="122"/>
       <c r="G11" s="123"/>
       <c r="H11" s="50" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="163"/>
+      <c r="K11" s="147"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="141"/>
-      <c r="C12" s="142"/>
-      <c r="D12" s="151"/>
-      <c r="E12" s="152"/>
+        <v>47</v>
+      </c>
+      <c r="B12" s="162"/>
+      <c r="C12" s="163"/>
+      <c r="D12" s="153"/>
+      <c r="E12" s="154"/>
       <c r="F12" s="122"/>
       <c r="G12" s="123"/>
       <c r="H12" s="117" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="117" t="s">
-        <v>50</v>
-      </c>
       <c r="J12" s="117"/>
-      <c r="K12" s="163"/>
+      <c r="K12" s="147"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>981</v>
       </c>
-      <c r="B13" s="143"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="153"/>
-      <c r="E13" s="154"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="165"/>
+      <c r="D13" s="155"/>
+      <c r="E13" s="156"/>
       <c r="F13" s="124"/>
       <c r="G13" s="125"/>
       <c r="H13" s="53" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="164"/>
+      <c r="K13" s="148"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="146" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="147"/>
-      <c r="D14" s="146" t="s">
+      <c r="B14" s="144" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="145"/>
+      <c r="D14" s="144" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="147"/>
-      <c r="F14" s="146" t="s">
+      <c r="E14" s="145"/>
+      <c r="F14" s="144" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="147"/>
-      <c r="H14" s="145" t="s">
+      <c r="G14" s="145"/>
+      <c r="H14" s="157" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="145"/>
+      <c r="I14" s="157"/>
       <c r="J14" s="126" t="s">
         <v>39</v>
       </c>
@@ -3144,35 +3167,35 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="139" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="140"/>
-      <c r="D15" s="149" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="150"/>
+      <c r="B15" s="160" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="161"/>
+      <c r="D15" s="151" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="152"/>
       <c r="F15" s="120" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G15" s="121"/>
-      <c r="H15" s="157" t="s">
+      <c r="H15" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="158"/>
+      <c r="I15" s="159"/>
       <c r="J15" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="K15" s="162"/>
+        <v>70</v>
+      </c>
+      <c r="K15" s="146"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="141"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="151"/>
-      <c r="E16" s="152"/>
+      <c r="B16" s="162"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="153"/>
+      <c r="E16" s="154"/>
       <c r="F16" s="122"/>
       <c r="G16" s="123"/>
       <c r="H16" s="126" t="s">
@@ -3184,83 +3207,83 @@
       <c r="J16" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="163"/>
+      <c r="K16" s="147"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="141"/>
-      <c r="C17" s="142"/>
-      <c r="D17" s="151"/>
-      <c r="E17" s="152"/>
+        <v>76</v>
+      </c>
+      <c r="B17" s="162"/>
+      <c r="C17" s="163"/>
+      <c r="D17" s="153"/>
+      <c r="E17" s="154"/>
       <c r="F17" s="122"/>
       <c r="G17" s="123"/>
       <c r="H17" s="50" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="K17" s="163"/>
+        <v>71</v>
+      </c>
+      <c r="K17" s="147"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="126" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="141"/>
-      <c r="C18" s="142"/>
-      <c r="D18" s="151"/>
-      <c r="E18" s="152"/>
+        <v>47</v>
+      </c>
+      <c r="B18" s="162"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="153"/>
+      <c r="E18" s="154"/>
       <c r="F18" s="122"/>
       <c r="G18" s="123"/>
       <c r="H18" s="126" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="126" t="s">
-        <v>50</v>
-      </c>
       <c r="J18" s="126"/>
-      <c r="K18" s="163"/>
+      <c r="K18" s="147"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>921</v>
       </c>
-      <c r="B19" s="143"/>
-      <c r="C19" s="144"/>
-      <c r="D19" s="153"/>
-      <c r="E19" s="154"/>
+      <c r="B19" s="164"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="155"/>
+      <c r="E19" s="156"/>
       <c r="F19" s="124"/>
       <c r="G19" s="125"/>
       <c r="H19" s="50" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="163"/>
+      <c r="K19" s="147"/>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A20" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="137" t="s">
+      <c r="B20" s="141" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="138"/>
-      <c r="D20" s="137" t="s">
+      <c r="C20" s="142"/>
+      <c r="D20" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="138"/>
-      <c r="F20" s="137" t="s">
+      <c r="E20" s="142"/>
+      <c r="F20" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="138"/>
-      <c r="H20" s="161" t="s">
+      <c r="G20" s="142"/>
+      <c r="H20" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="161"/>
+      <c r="I20" s="140"/>
       <c r="J20" s="128" t="s">
         <v>39</v>
       </c>
@@ -3270,35 +3293,35 @@
     </row>
     <row r="21" spans="1:11" ht="10.5" customHeight="1">
       <c r="A21" s="48">
-        <v>1</v>
-      </c>
-      <c r="B21" s="139" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="140"/>
-      <c r="D21" s="149" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="150"/>
+        <v>3</v>
+      </c>
+      <c r="B21" s="160" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="161"/>
+      <c r="D21" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="152"/>
       <c r="F21" s="129" t="s">
         <v>41</v>
       </c>
       <c r="G21" s="130"/>
-      <c r="H21" s="155" t="s">
+      <c r="H21" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="156"/>
+      <c r="I21" s="150"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="162"/>
+      <c r="K21" s="146"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="141"/>
-      <c r="C22" s="142"/>
-      <c r="D22" s="151"/>
-      <c r="E22" s="152"/>
+      <c r="B22" s="162"/>
+      <c r="C22" s="163"/>
+      <c r="D22" s="153"/>
+      <c r="E22" s="154"/>
       <c r="F22" s="131"/>
       <c r="G22" s="132"/>
       <c r="H22" s="127" t="s">
@@ -3310,102 +3333,481 @@
       <c r="J22" s="127" t="s">
         <v>45</v>
       </c>
-      <c r="K22" s="163"/>
+      <c r="K22" s="147"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="141"/>
-      <c r="C23" s="142"/>
-      <c r="D23" s="151"/>
-      <c r="E23" s="152"/>
+        <v>74</v>
+      </c>
+      <c r="B23" s="162"/>
+      <c r="C23" s="163"/>
+      <c r="D23" s="153"/>
+      <c r="E23" s="154"/>
       <c r="F23" s="131"/>
       <c r="G23" s="132"/>
       <c r="H23" s="50" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="163"/>
+      <c r="K23" s="147"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="127" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="141"/>
-      <c r="C24" s="142"/>
-      <c r="D24" s="151"/>
-      <c r="E24" s="152"/>
+        <v>47</v>
+      </c>
+      <c r="B24" s="162"/>
+      <c r="C24" s="163"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="154"/>
       <c r="F24" s="131"/>
       <c r="G24" s="132"/>
       <c r="H24" s="127" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="127" t="s">
         <v>49</v>
       </c>
-      <c r="I24" s="127" t="s">
-        <v>50</v>
-      </c>
       <c r="J24" s="127"/>
-      <c r="K24" s="163"/>
+      <c r="K24" s="147"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
-        <v>981</v>
-      </c>
-      <c r="B25" s="143"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="154"/>
+        <v>982</v>
+      </c>
+      <c r="B25" s="164"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="155"/>
+      <c r="E25" s="156"/>
       <c r="F25" s="133"/>
       <c r="G25" s="134"/>
       <c r="H25" s="50" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I25" s="50"/>
       <c r="J25" s="48"/>
-      <c r="K25" s="164"/>
-    </row>
-    <row r="40" spans="1:11" s="58" customFormat="1">
-      <c r="A40" s="62"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="62"/>
-    </row>
-    <row r="41" spans="1:11" s="58" customFormat="1">
-      <c r="A41" s="62"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="62"/>
-      <c r="J41" s="62"/>
-      <c r="K41" s="62"/>
-    </row>
-    <row r="42" spans="1:11" s="58" customFormat="1">
-      <c r="A42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
-      <c r="K42" s="62"/>
-    </row>
-    <row r="43" spans="1:11" s="58" customFormat="1">
-      <c r="A43" s="62"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="62"/>
-      <c r="J43" s="62"/>
-      <c r="K43" s="62"/>
-    </row>
-    <row r="44" spans="1:11" s="58" customFormat="1">
-      <c r="A44" s="62"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="62"/>
-      <c r="J44" s="62"/>
-      <c r="K44" s="62"/>
-    </row>
-    <row r="45" spans="1:11" s="58" customFormat="1">
-      <c r="A45" s="62"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="62"/>
-      <c r="J45" s="62"/>
-      <c r="K45" s="62"/>
+      <c r="K25" s="148"/>
+    </row>
+    <row r="26" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A26" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="143" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="143"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="138"/>
+      <c r="F26" s="138"/>
+      <c r="G26" s="138"/>
+      <c r="H26" s="138"/>
+      <c r="I26" s="138"/>
+      <c r="J26" s="138"/>
+      <c r="K26" s="138"/>
+    </row>
+    <row r="27" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A27" s="100" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="166" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="167"/>
+      <c r="D27" s="167"/>
+      <c r="E27" s="167"/>
+      <c r="F27" s="167"/>
+      <c r="G27" s="167"/>
+      <c r="H27" s="167"/>
+      <c r="I27" s="167"/>
+      <c r="J27" s="167"/>
+      <c r="K27" s="168"/>
+    </row>
+    <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A28" s="135" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="144" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="145"/>
+      <c r="D28" s="144" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="145"/>
+      <c r="F28" s="144" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="145"/>
+      <c r="H28" s="157" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="157"/>
+      <c r="J28" s="135" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="135" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A29" s="48">
+        <f>A15+1</f>
+        <v>3</v>
+      </c>
+      <c r="B29" s="160" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="161"/>
+      <c r="D29" s="151" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="152"/>
+      <c r="F29" s="151" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="152"/>
+      <c r="H29" s="149" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="150"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="146"/>
+    </row>
+    <row r="30" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A30" s="126" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="162"/>
+      <c r="C30" s="163"/>
+      <c r="D30" s="153"/>
+      <c r="E30" s="154"/>
+      <c r="F30" s="153"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="J30" s="126" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30" s="147"/>
+    </row>
+    <row r="31" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A31" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="162"/>
+      <c r="C31" s="163"/>
+      <c r="D31" s="153"/>
+      <c r="E31" s="154"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="154"/>
+      <c r="H31" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="50"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="147"/>
+    </row>
+    <row r="32" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A32" s="126" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="162"/>
+      <c r="C32" s="163"/>
+      <c r="D32" s="153"/>
+      <c r="E32" s="154"/>
+      <c r="F32" s="153"/>
+      <c r="G32" s="154"/>
+      <c r="H32" s="126" t="s">
+        <v>48</v>
+      </c>
+      <c r="I32" s="126"/>
+      <c r="J32" s="126"/>
+      <c r="K32" s="147"/>
+    </row>
+    <row r="33" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A33" s="51">
+        <v>922</v>
+      </c>
+      <c r="B33" s="164"/>
+      <c r="C33" s="165"/>
+      <c r="D33" s="155"/>
+      <c r="E33" s="156"/>
+      <c r="F33" s="155"/>
+      <c r="G33" s="156"/>
+      <c r="H33" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="I33" s="50"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="148"/>
+    </row>
+    <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A34" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="141" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="142"/>
+      <c r="D34" s="141" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="142"/>
+      <c r="F34" s="141" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="142"/>
+      <c r="H34" s="139" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34" s="139"/>
+      <c r="J34" s="117" t="s">
+        <v>39</v>
+      </c>
+      <c r="K34" s="119" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A35" s="48">
+        <v>4</v>
+      </c>
+      <c r="B35" s="160" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="161"/>
+      <c r="D35" s="151" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="152"/>
+      <c r="F35" s="151" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" s="152"/>
+      <c r="H35" s="158" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="159"/>
+      <c r="J35" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="K35" s="146"/>
+    </row>
+    <row r="36" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A36" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="162"/>
+      <c r="C36" s="163"/>
+      <c r="D36" s="153"/>
+      <c r="E36" s="154"/>
+      <c r="F36" s="153"/>
+      <c r="G36" s="154"/>
+      <c r="H36" s="117" t="s">
+        <v>43</v>
+      </c>
+      <c r="I36" s="117" t="s">
+        <v>44</v>
+      </c>
+      <c r="J36" s="117" t="s">
+        <v>45</v>
+      </c>
+      <c r="K36" s="147"/>
+    </row>
+    <row r="37" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A37" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="162"/>
+      <c r="C37" s="163"/>
+      <c r="D37" s="153"/>
+      <c r="E37" s="154"/>
+      <c r="F37" s="153"/>
+      <c r="G37" s="154"/>
+      <c r="H37" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="I37" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="K37" s="147"/>
+    </row>
+    <row r="38" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A38" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="162"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="153"/>
+      <c r="E38" s="154"/>
+      <c r="F38" s="153"/>
+      <c r="G38" s="154"/>
+      <c r="H38" s="117" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" s="117" t="s">
+        <v>49</v>
+      </c>
+      <c r="J38" s="117"/>
+      <c r="K38" s="147"/>
+    </row>
+    <row r="39" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A39" s="51">
+        <v>823</v>
+      </c>
+      <c r="B39" s="164"/>
+      <c r="C39" s="165"/>
+      <c r="D39" s="155"/>
+      <c r="E39" s="156"/>
+      <c r="F39" s="155"/>
+      <c r="G39" s="156"/>
+      <c r="H39" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39" s="48"/>
+      <c r="K39" s="148"/>
+    </row>
+    <row r="40" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A40" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="141" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="142"/>
+      <c r="D40" s="141" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="142"/>
+      <c r="F40" s="141" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40" s="142"/>
+      <c r="H40" s="139" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40" s="139"/>
+      <c r="J40" s="117" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="119" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A41" s="48">
+        <v>5</v>
+      </c>
+      <c r="B41" s="160" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="161"/>
+      <c r="D41" s="151" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="152"/>
+      <c r="F41" s="151" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" s="152"/>
+      <c r="H41" s="158" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="159"/>
+      <c r="J41" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="K41" s="146"/>
+    </row>
+    <row r="42" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A42" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="162"/>
+      <c r="C42" s="163"/>
+      <c r="D42" s="153"/>
+      <c r="E42" s="154"/>
+      <c r="F42" s="153"/>
+      <c r="G42" s="154"/>
+      <c r="H42" s="117" t="s">
+        <v>43</v>
+      </c>
+      <c r="I42" s="117" t="s">
+        <v>44</v>
+      </c>
+      <c r="J42" s="117" t="s">
+        <v>45</v>
+      </c>
+      <c r="K42" s="147"/>
+    </row>
+    <row r="43" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A43" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="162"/>
+      <c r="C43" s="163"/>
+      <c r="D43" s="153"/>
+      <c r="E43" s="154"/>
+      <c r="F43" s="153"/>
+      <c r="G43" s="154"/>
+      <c r="H43" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="J43" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="K43" s="147"/>
+    </row>
+    <row r="44" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A44" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="162"/>
+      <c r="C44" s="163"/>
+      <c r="D44" s="153"/>
+      <c r="E44" s="154"/>
+      <c r="F44" s="153"/>
+      <c r="G44" s="154"/>
+      <c r="H44" s="117" t="s">
+        <v>48</v>
+      </c>
+      <c r="I44" s="117" t="s">
+        <v>49</v>
+      </c>
+      <c r="J44" s="117"/>
+      <c r="K44" s="147"/>
+    </row>
+    <row r="45" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A45" s="51">
+        <v>823</v>
+      </c>
+      <c r="B45" s="164"/>
+      <c r="C45" s="165"/>
+      <c r="D45" s="155"/>
+      <c r="E45" s="156"/>
+      <c r="F45" s="155"/>
+      <c r="G45" s="156"/>
+      <c r="H45" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="I45" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="J45" s="48"/>
+      <c r="K45" s="148"/>
     </row>
     <row r="46" spans="1:11" s="58" customFormat="1">
       <c r="A46" s="62"/>
@@ -3414,427 +3816,6 @@
       <c r="J46" s="62"/>
       <c r="K46" s="62"/>
     </row>
-    <row r="47" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A47" s="99" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="166" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="166"/>
-      <c r="D47" s="165"/>
-      <c r="E47" s="165"/>
-      <c r="F47" s="165"/>
-      <c r="G47" s="165"/>
-      <c r="H47" s="165"/>
-      <c r="I47" s="165"/>
-      <c r="J47" s="165"/>
-      <c r="K47" s="165"/>
-    </row>
-    <row r="48" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A48" s="100" t="s">
-        <v>59</v>
-      </c>
-      <c r="B48" s="159" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="159"/>
-      <c r="D48" s="160"/>
-      <c r="E48" s="160"/>
-      <c r="F48" s="160"/>
-      <c r="G48" s="160"/>
-      <c r="H48" s="160"/>
-      <c r="I48" s="160"/>
-      <c r="J48" s="160"/>
-      <c r="K48" s="160"/>
-    </row>
-    <row r="49" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A49" s="126" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49" s="146" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="147"/>
-      <c r="D49" s="146" t="s">
-        <v>36</v>
-      </c>
-      <c r="E49" s="147"/>
-      <c r="F49" s="146" t="s">
-        <v>37</v>
-      </c>
-      <c r="G49" s="147"/>
-      <c r="H49" s="145" t="s">
-        <v>38</v>
-      </c>
-      <c r="I49" s="145"/>
-      <c r="J49" s="126" t="s">
-        <v>39</v>
-      </c>
-      <c r="K49" s="126" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A50" s="48">
-        <f>A15+1</f>
-        <v>3</v>
-      </c>
-      <c r="B50" s="139" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="140"/>
-      <c r="D50" s="149" t="s">
-        <v>62</v>
-      </c>
-      <c r="E50" s="150"/>
-      <c r="F50" s="149" t="s">
-        <v>63</v>
-      </c>
-      <c r="G50" s="150"/>
-      <c r="H50" s="155" t="s">
-        <v>10</v>
-      </c>
-      <c r="I50" s="156"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="162"/>
-    </row>
-    <row r="51" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A51" s="126" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" s="141"/>
-      <c r="C51" s="142"/>
-      <c r="D51" s="151"/>
-      <c r="E51" s="152"/>
-      <c r="F51" s="151"/>
-      <c r="G51" s="152"/>
-      <c r="H51" s="126" t="s">
-        <v>43</v>
-      </c>
-      <c r="I51" s="126" t="s">
-        <v>44</v>
-      </c>
-      <c r="J51" s="126" t="s">
-        <v>45</v>
-      </c>
-      <c r="K51" s="163"/>
-    </row>
-    <row r="52" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A52" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="141"/>
-      <c r="C52" s="142"/>
-      <c r="D52" s="151"/>
-      <c r="E52" s="152"/>
-      <c r="F52" s="151"/>
-      <c r="G52" s="152"/>
-      <c r="H52" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="I52" s="50"/>
-      <c r="J52" s="48"/>
-      <c r="K52" s="163"/>
-    </row>
-    <row r="53" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A53" s="126" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="141"/>
-      <c r="C53" s="142"/>
-      <c r="D53" s="151"/>
-      <c r="E53" s="152"/>
-      <c r="F53" s="151"/>
-      <c r="G53" s="152"/>
-      <c r="H53" s="126" t="s">
-        <v>49</v>
-      </c>
-      <c r="I53" s="126"/>
-      <c r="J53" s="126"/>
-      <c r="K53" s="163"/>
-    </row>
-    <row r="54" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A54" s="51">
-        <v>922</v>
-      </c>
-      <c r="B54" s="143"/>
-      <c r="C54" s="144"/>
-      <c r="D54" s="153"/>
-      <c r="E54" s="154"/>
-      <c r="F54" s="153"/>
-      <c r="G54" s="154"/>
-      <c r="H54" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="I54" s="50"/>
-      <c r="J54" s="48"/>
-      <c r="K54" s="164"/>
-    </row>
-    <row r="55" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A55" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="B55" s="137" t="s">
-        <v>35</v>
-      </c>
-      <c r="C55" s="138"/>
-      <c r="D55" s="137" t="s">
-        <v>36</v>
-      </c>
-      <c r="E55" s="138"/>
-      <c r="F55" s="137" t="s">
-        <v>37</v>
-      </c>
-      <c r="G55" s="138"/>
-      <c r="H55" s="148" t="s">
-        <v>38</v>
-      </c>
-      <c r="I55" s="148"/>
-      <c r="J55" s="117" t="s">
-        <v>39</v>
-      </c>
-      <c r="K55" s="119" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A56" s="48">
-        <v>4</v>
-      </c>
-      <c r="B56" s="139" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="140"/>
-      <c r="D56" s="149" t="s">
-        <v>62</v>
-      </c>
-      <c r="E56" s="150"/>
-      <c r="F56" s="149" t="s">
-        <v>63</v>
-      </c>
-      <c r="G56" s="150"/>
-      <c r="H56" s="157" t="s">
-        <v>10</v>
-      </c>
-      <c r="I56" s="158"/>
-      <c r="J56" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="K56" s="162"/>
-    </row>
-    <row r="57" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A57" s="117" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" s="141"/>
-      <c r="C57" s="142"/>
-      <c r="D57" s="151"/>
-      <c r="E57" s="152"/>
-      <c r="F57" s="151"/>
-      <c r="G57" s="152"/>
-      <c r="H57" s="117" t="s">
-        <v>43</v>
-      </c>
-      <c r="I57" s="117" t="s">
-        <v>44</v>
-      </c>
-      <c r="J57" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="K57" s="163"/>
-    </row>
-    <row r="58" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A58" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" s="141"/>
-      <c r="C58" s="142"/>
-      <c r="D58" s="151"/>
-      <c r="E58" s="152"/>
-      <c r="F58" s="151"/>
-      <c r="G58" s="152"/>
-      <c r="H58" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="I58" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="J58" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="K58" s="163"/>
-    </row>
-    <row r="59" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A59" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="B59" s="141"/>
-      <c r="C59" s="142"/>
-      <c r="D59" s="151"/>
-      <c r="E59" s="152"/>
-      <c r="F59" s="151"/>
-      <c r="G59" s="152"/>
-      <c r="H59" s="117" t="s">
-        <v>49</v>
-      </c>
-      <c r="I59" s="117" t="s">
-        <v>50</v>
-      </c>
-      <c r="J59" s="117"/>
-      <c r="K59" s="163"/>
-    </row>
-    <row r="60" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A60" s="51">
-        <v>823</v>
-      </c>
-      <c r="B60" s="143"/>
-      <c r="C60" s="144"/>
-      <c r="D60" s="153"/>
-      <c r="E60" s="154"/>
-      <c r="F60" s="153"/>
-      <c r="G60" s="154"/>
-      <c r="H60" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="I60" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="J60" s="48"/>
-      <c r="K60" s="164"/>
-    </row>
-    <row r="61" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A61" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="B61" s="137" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" s="138"/>
-      <c r="D61" s="137" t="s">
-        <v>36</v>
-      </c>
-      <c r="E61" s="138"/>
-      <c r="F61" s="137" t="s">
-        <v>37</v>
-      </c>
-      <c r="G61" s="138"/>
-      <c r="H61" s="148" t="s">
-        <v>38</v>
-      </c>
-      <c r="I61" s="148"/>
-      <c r="J61" s="117" t="s">
-        <v>39</v>
-      </c>
-      <c r="K61" s="119" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A62" s="48">
-        <v>5</v>
-      </c>
-      <c r="B62" s="139" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="140"/>
-      <c r="D62" s="149" t="s">
-        <v>62</v>
-      </c>
-      <c r="E62" s="150"/>
-      <c r="F62" s="149" t="s">
-        <v>63</v>
-      </c>
-      <c r="G62" s="150"/>
-      <c r="H62" s="157" t="s">
-        <v>10</v>
-      </c>
-      <c r="I62" s="158"/>
-      <c r="J62" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="K62" s="162"/>
-    </row>
-    <row r="63" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A63" s="117" t="s">
-        <v>42</v>
-      </c>
-      <c r="B63" s="141"/>
-      <c r="C63" s="142"/>
-      <c r="D63" s="151"/>
-      <c r="E63" s="152"/>
-      <c r="F63" s="151"/>
-      <c r="G63" s="152"/>
-      <c r="H63" s="117" t="s">
-        <v>43</v>
-      </c>
-      <c r="I63" s="117" t="s">
-        <v>44</v>
-      </c>
-      <c r="J63" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="K63" s="163"/>
-    </row>
-    <row r="64" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A64" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="B64" s="141"/>
-      <c r="C64" s="142"/>
-      <c r="D64" s="151"/>
-      <c r="E64" s="152"/>
-      <c r="F64" s="151"/>
-      <c r="G64" s="152"/>
-      <c r="H64" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="I64" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="J64" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="K64" s="163"/>
-    </row>
-    <row r="65" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A65" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="B65" s="141"/>
-      <c r="C65" s="142"/>
-      <c r="D65" s="151"/>
-      <c r="E65" s="152"/>
-      <c r="F65" s="151"/>
-      <c r="G65" s="152"/>
-      <c r="H65" s="117" t="s">
-        <v>49</v>
-      </c>
-      <c r="I65" s="117" t="s">
-        <v>50</v>
-      </c>
-      <c r="J65" s="117"/>
-      <c r="K65" s="163"/>
-    </row>
-    <row r="66" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A66" s="51">
-        <v>823</v>
-      </c>
-      <c r="B66" s="143"/>
-      <c r="C66" s="144"/>
-      <c r="D66" s="153"/>
-      <c r="E66" s="154"/>
-      <c r="F66" s="153"/>
-      <c r="G66" s="154"/>
-      <c r="H66" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="I66" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="J66" s="48"/>
-      <c r="K66" s="164"/>
-    </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
       <c r="A67" s="62"/>
       <c r="H67" s="62"/>
@@ -4047,38 +4028,28 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B47:K47"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="D50:E54"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G54"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="K62:K66"/>
-    <mergeCell ref="F56:G60"/>
-    <mergeCell ref="K56:K60"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="F62:G66"/>
-    <mergeCell ref="B62:C66"/>
-    <mergeCell ref="D56:E60"/>
-    <mergeCell ref="D62:E66"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="B35:C39"/>
+    <mergeCell ref="B41:C45"/>
+    <mergeCell ref="D35:E39"/>
+    <mergeCell ref="D41:E45"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="D9:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B48:K48"/>
+    <mergeCell ref="B27:K27"/>
     <mergeCell ref="D15:E19"/>
     <mergeCell ref="B15:C19"/>
     <mergeCell ref="B20:C20"/>
@@ -4087,28 +4058,38 @@
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="B21:C25"/>
     <mergeCell ref="D21:E25"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="B56:C60"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="B50:C54"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K41:K45"/>
+    <mergeCell ref="F35:G39"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="F41:G45"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="D29:E33"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="H62:I62">
+  <conditionalFormatting sqref="H41:I41">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H61:I61">
+  <conditionalFormatting sqref="H40:I40">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>

</xml_diff>

<commit_message>
test chuc nang tim kiem noi dung theo ngay tao
</commit_message>
<xml_diff>
--- a/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>Chạy được</t>
   </si>
   <si>
     <t>ID</t>
@@ -419,9 +416,6 @@
     <t>Click vào button thêm để thêm mới một confession khi muốn chia sẻ tâm sự của mình với mọi người</t>
   </si>
   <si>
-    <t>Không chạy được</t>
-  </si>
-  <si>
     <t>BUG21</t>
   </si>
   <si>
@@ -459,16 +453,30 @@
     <t>Tìm kiếm nội dung theo nội dung phê duyệt</t>
   </si>
   <si>
-    <t>Không tìm kiếm được</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tìm kiếm nội dung theo ngày tạo
 </t>
   </si>
   <si>
     <t>1. Gõ nội dung
+2. Chọn tiêu chí sắp xếp theo ngày tạo
+3. Bấm lọc</t>
+  </si>
+  <si>
+    <t>1. Gõ nội dung
 2. Chọn tiêu chí sắp xếp theo nội dung phê duyệt
-3. Lọc</t>
+3. Bấm lọc</t>
+  </si>
+  <si>
+    <t>Lọc được kết quả</t>
+  </si>
+  <si>
+    <t>Thêm được</t>
+  </si>
+  <si>
+    <t>Xem được thông tin</t>
+  </si>
+  <si>
+    <t>Xem được bài viết</t>
   </si>
 </sst>
 </file>
@@ -2864,8 +2872,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:E33"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2882,7 +2890,7 @@
         <v>20</v>
       </c>
       <c r="B1" s="78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" s="78"/>
       <c r="D1" s="78"/>
@@ -2896,7 +2904,7 @@
       </c>
       <c r="I1" s="101">
         <f>COUNTIF(H1:H786,"OK")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J1" s="82" t="s">
         <v>23</v>
@@ -2920,7 +2928,7 @@
       </c>
       <c r="I2" s="102">
         <f>COUNTIF(H2:H787,"Not OK")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2" s="89" t="s">
         <v>27</v>
@@ -3000,7 +3008,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="138" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="138"/>
       <c r="D7" s="138"/>
@@ -3044,15 +3052,15 @@
         <v>1</v>
       </c>
       <c r="B9" s="160" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="161"/>
       <c r="D9" s="151" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="152"/>
       <c r="F9" s="120" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="G9" s="121"/>
       <c r="H9" s="149" t="s">
@@ -3064,7 +3072,7 @@
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="117" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="162"/>
       <c r="C10" s="163"/>
@@ -3073,19 +3081,19 @@
       <c r="F10" s="122"/>
       <c r="G10" s="123"/>
       <c r="H10" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="117" t="s">
+      <c r="J10" s="117" t="s">
         <v>44</v>
-      </c>
-      <c r="J10" s="117" t="s">
-        <v>45</v>
       </c>
       <c r="K10" s="147"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="162"/>
       <c r="C11" s="163"/>
@@ -3094,7 +3102,7 @@
       <c r="F11" s="122"/>
       <c r="G11" s="123"/>
       <c r="H11" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
@@ -3102,7 +3110,7 @@
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="117" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="162"/>
       <c r="C12" s="163"/>
@@ -3111,10 +3119,10 @@
       <c r="F12" s="122"/>
       <c r="G12" s="123"/>
       <c r="H12" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="117" t="s">
         <v>48</v>
-      </c>
-      <c r="I12" s="117" t="s">
-        <v>49</v>
       </c>
       <c r="J12" s="117"/>
       <c r="K12" s="147"/>
@@ -3130,7 +3138,7 @@
       <c r="F13" s="124"/>
       <c r="G13" s="125"/>
       <c r="H13" s="53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
@@ -3141,7 +3149,7 @@
         <v>34</v>
       </c>
       <c r="B14" s="144" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="145"/>
       <c r="D14" s="144" t="s">
@@ -3168,15 +3176,15 @@
         <v>2</v>
       </c>
       <c r="B15" s="160" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="161"/>
       <c r="D15" s="151" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="152"/>
       <c r="F15" s="120" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="G15" s="121"/>
       <c r="H15" s="158" t="s">
@@ -3184,13 +3192,13 @@
       </c>
       <c r="I15" s="159"/>
       <c r="J15" s="52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K15" s="146"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="126" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="162"/>
       <c r="C16" s="163"/>
@@ -3199,19 +3207,19 @@
       <c r="F16" s="122"/>
       <c r="G16" s="123"/>
       <c r="H16" s="126" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="126" t="s">
+      <c r="J16" s="126" t="s">
         <v>44</v>
-      </c>
-      <c r="J16" s="126" t="s">
-        <v>45</v>
       </c>
       <c r="K16" s="147"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B17" s="162"/>
       <c r="C17" s="163"/>
@@ -3220,17 +3228,17 @@
       <c r="F17" s="122"/>
       <c r="G17" s="123"/>
       <c r="H17" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K17" s="147"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="126" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="162"/>
       <c r="C18" s="163"/>
@@ -3239,10 +3247,10 @@
       <c r="F18" s="122"/>
       <c r="G18" s="123"/>
       <c r="H18" s="126" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="126" t="s">
         <v>48</v>
-      </c>
-      <c r="I18" s="126" t="s">
-        <v>49</v>
       </c>
       <c r="J18" s="126"/>
       <c r="K18" s="147"/>
@@ -3258,7 +3266,7 @@
       <c r="F19" s="124"/>
       <c r="G19" s="125"/>
       <c r="H19" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
@@ -3296,15 +3304,15 @@
         <v>3</v>
       </c>
       <c r="B21" s="160" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C21" s="161"/>
       <c r="D21" s="151" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E21" s="152"/>
       <c r="F21" s="129" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="G21" s="130"/>
       <c r="H21" s="149" t="s">
@@ -3316,7 +3324,7 @@
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="127" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="162"/>
       <c r="C22" s="163"/>
@@ -3325,19 +3333,19 @@
       <c r="F22" s="131"/>
       <c r="G22" s="132"/>
       <c r="H22" s="127" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="127" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="127" t="s">
+      <c r="J22" s="127" t="s">
         <v>44</v>
-      </c>
-      <c r="J22" s="127" t="s">
-        <v>45</v>
       </c>
       <c r="K22" s="147"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" s="162"/>
       <c r="C23" s="163"/>
@@ -3346,7 +3354,7 @@
       <c r="F23" s="131"/>
       <c r="G23" s="132"/>
       <c r="H23" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
@@ -3354,7 +3362,7 @@
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="127" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="162"/>
       <c r="C24" s="163"/>
@@ -3363,10 +3371,10 @@
       <c r="F24" s="131"/>
       <c r="G24" s="132"/>
       <c r="H24" s="127" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="127" t="s">
         <v>48</v>
-      </c>
-      <c r="I24" s="127" t="s">
-        <v>49</v>
       </c>
       <c r="J24" s="127"/>
       <c r="K24" s="147"/>
@@ -3382,7 +3390,7 @@
       <c r="F25" s="133"/>
       <c r="G25" s="134"/>
       <c r="H25" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I25" s="50"/>
       <c r="J25" s="48"/>
@@ -3390,10 +3398,10 @@
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="99" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="143" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" s="143"/>
       <c r="D26" s="138"/>
@@ -3407,10 +3415,10 @@
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="100" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="166" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C27" s="167"/>
       <c r="D27" s="167"/>
@@ -3427,7 +3435,7 @@
         <v>34</v>
       </c>
       <c r="B28" s="144" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="145"/>
       <c r="D28" s="144" t="s">
@@ -3455,15 +3463,15 @@
         <v>3</v>
       </c>
       <c r="B29" s="160" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" s="161"/>
       <c r="D29" s="151" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E29" s="152"/>
       <c r="F29" s="151" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G29" s="152"/>
       <c r="H29" s="149" t="s">
@@ -3475,7 +3483,7 @@
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="126" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="162"/>
       <c r="C30" s="163"/>
@@ -3484,19 +3492,19 @@
       <c r="F30" s="153"/>
       <c r="G30" s="154"/>
       <c r="H30" s="126" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="I30" s="126" t="s">
+      <c r="J30" s="126" t="s">
         <v>44</v>
-      </c>
-      <c r="J30" s="126" t="s">
-        <v>45</v>
       </c>
       <c r="K30" s="147"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="162"/>
       <c r="C31" s="163"/>
@@ -3505,7 +3513,7 @@
       <c r="F31" s="153"/>
       <c r="G31" s="154"/>
       <c r="H31" s="50" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="I31" s="50"/>
       <c r="J31" s="48"/>
@@ -3513,7 +3521,7 @@
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="126" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="162"/>
       <c r="C32" s="163"/>
@@ -3522,7 +3530,7 @@
       <c r="F32" s="153"/>
       <c r="G32" s="154"/>
       <c r="H32" s="126" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I32" s="126"/>
       <c r="J32" s="126"/>
@@ -3539,7 +3547,7 @@
       <c r="F33" s="155"/>
       <c r="G33" s="156"/>
       <c r="H33" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I33" s="50"/>
       <c r="J33" s="48"/>
@@ -3577,29 +3585,29 @@
         <v>4</v>
       </c>
       <c r="B35" s="160" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C35" s="161"/>
       <c r="D35" s="151" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E35" s="152"/>
       <c r="F35" s="151" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G35" s="152"/>
       <c r="H35" s="158" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I35" s="159"/>
       <c r="J35" s="52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K35" s="146"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="117" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="162"/>
       <c r="C36" s="163"/>
@@ -3608,19 +3616,19 @@
       <c r="F36" s="153"/>
       <c r="G36" s="154"/>
       <c r="H36" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="I36" s="117" t="s">
+      <c r="J36" s="117" t="s">
         <v>44</v>
-      </c>
-      <c r="J36" s="117" t="s">
-        <v>45</v>
       </c>
       <c r="K36" s="147"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="162"/>
       <c r="C37" s="163"/>
@@ -3629,19 +3637,19 @@
       <c r="F37" s="153"/>
       <c r="G37" s="154"/>
       <c r="H37" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I37" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J37" s="48" t="s">
         <v>52</v>
-      </c>
-      <c r="J37" s="48" t="s">
-        <v>53</v>
       </c>
       <c r="K37" s="147"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="117" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="162"/>
       <c r="C38" s="163"/>
@@ -3650,10 +3658,10 @@
       <c r="F38" s="153"/>
       <c r="G38" s="154"/>
       <c r="H38" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="I38" s="117" t="s">
         <v>48</v>
-      </c>
-      <c r="I38" s="117" t="s">
-        <v>49</v>
       </c>
       <c r="J38" s="117"/>
       <c r="K38" s="147"/>
@@ -3669,10 +3677,10 @@
       <c r="F39" s="155"/>
       <c r="G39" s="156"/>
       <c r="H39" s="50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I39" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J39" s="48"/>
       <c r="K39" s="148"/>
@@ -3709,15 +3717,15 @@
         <v>5</v>
       </c>
       <c r="B41" s="160" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" s="161"/>
       <c r="D41" s="151" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E41" s="152"/>
       <c r="F41" s="151" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G41" s="152"/>
       <c r="H41" s="158" t="s">
@@ -3725,13 +3733,13 @@
       </c>
       <c r="I41" s="159"/>
       <c r="J41" s="52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K41" s="146"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
       <c r="A42" s="117" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="162"/>
       <c r="C42" s="163"/>
@@ -3740,19 +3748,19 @@
       <c r="F42" s="153"/>
       <c r="G42" s="154"/>
       <c r="H42" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="117" t="s">
+      <c r="J42" s="117" t="s">
         <v>44</v>
-      </c>
-      <c r="J42" s="117" t="s">
-        <v>45</v>
       </c>
       <c r="K42" s="147"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
       <c r="A43" s="49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" s="162"/>
       <c r="C43" s="163"/>
@@ -3761,19 +3769,19 @@
       <c r="F43" s="153"/>
       <c r="G43" s="154"/>
       <c r="H43" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I43" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J43" s="48" t="s">
         <v>52</v>
-      </c>
-      <c r="J43" s="48" t="s">
-        <v>53</v>
       </c>
       <c r="K43" s="147"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
       <c r="A44" s="117" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" s="162"/>
       <c r="C44" s="163"/>
@@ -3782,10 +3790,10 @@
       <c r="F44" s="153"/>
       <c r="G44" s="154"/>
       <c r="H44" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="I44" s="117" t="s">
         <v>48</v>
-      </c>
-      <c r="I44" s="117" t="s">
-        <v>49</v>
       </c>
       <c r="J44" s="117"/>
       <c r="K44" s="147"/>
@@ -3801,10 +3809,10 @@
       <c r="F45" s="155"/>
       <c r="G45" s="156"/>
       <c r="H45" s="50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I45" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J45" s="48"/>
       <c r="K45" s="148"/>
@@ -4095,11 +4103,14 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="86" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;LTest Case Table&amp;CBig Point: &amp;A</oddHeader>
     <oddFooter>&amp;LAI&amp;&amp;T-ART&amp;CLiveSpark Project&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="54" max="10" man="1"/>
+  </rowBreaks>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test chuc nang tim kiem noi dung theo so luong comment
</commit_message>
<xml_diff>
--- a/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -201,12 +201,177 @@
         </r>
       </text>
     </comment>
+    <comment ref="B46" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Point \ Point 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H47" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Kết quả test:
+OK / Not OK</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J47" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Ánh xạ tới ID tương ứng của Bug được ghi nhận trong BugList</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Số thứ tự tăng dần testcase, không phần biệt sheet,...
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Người thực hiện test</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Người chịu trách nhiệm về lỗi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Người sửa lỗi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A50" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SheetNo.Suite.Suite-</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>CaseNo</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+CaseNo tăng dần và lặp lại từ 1 giữa các Suite-Point khác nhau</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H51" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Ngày thực hiện test</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I51" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Ngày test lại, trong trường hợp lần test trước có lỗi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A52" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>ID tương ứng của TestLink</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -376,22 +541,7 @@
     <t>2.1.</t>
   </si>
   <si>
-    <t>1. Add film mpeg
-2. Mo VLC
-3. Gõ địa chỉ 192.168.0.5</t>
-  </si>
-  <si>
-    <t>Xem được phim</t>
-  </si>
-  <si>
     <t>1.2.2-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Mpeg
-</t>
-  </si>
-  <si>
-    <t>BUG213</t>
   </si>
   <si>
     <t>1.1-2</t>
@@ -477,6 +627,24 @@
   </si>
   <si>
     <t>Xem được bài viết</t>
+  </si>
+  <si>
+    <t>BUG212</t>
+  </si>
+  <si>
+    <t>Test với chức năng đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nội dung theo trạng thái phê duyệt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm nội dung theo số lượng comment
+</t>
+  </si>
+  <si>
+    <t>1. Gõ nội dung
+2. Chọn tiêu chí sắp xếp theo số lượng comment
+3. Bấm lọc</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1155,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1312,6 +1480,9 @@
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1319,6 +1490,75 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1337,80 +1577,11 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1932,13 +2103,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="136" t="s">
+      <c r="O6" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="136"/>
-      <c r="Q6" s="136"/>
-      <c r="R6" s="136"/>
-      <c r="S6" s="136"/>
+      <c r="P6" s="137"/>
+      <c r="Q6" s="137"/>
+      <c r="R6" s="137"/>
+      <c r="S6" s="137"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -1948,11 +2119,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="136"/>
-      <c r="P7" s="136"/>
-      <c r="Q7" s="136"/>
-      <c r="R7" s="136"/>
-      <c r="S7" s="136"/>
+      <c r="O7" s="137"/>
+      <c r="P7" s="137"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="137"/>
+      <c r="S7" s="137"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -2007,12 +2178,12 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="137">
+      <c r="E11" s="138">
         <f ca="1">TODAY()</f>
         <v>43449</v>
       </c>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="138"/>
       <c r="H11" s="72"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
@@ -2872,8 +3043,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2890,7 +3061,7 @@
         <v>20</v>
       </c>
       <c r="B1" s="78" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C1" s="78"/>
       <c r="D1" s="78"/>
@@ -2928,7 +3099,7 @@
       </c>
       <c r="I2" s="102">
         <f>COUNTIF(H2:H787,"Not OK")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J2" s="89" t="s">
         <v>27</v>
@@ -2972,7 +3143,7 @@
       <c r="H4" s="85"/>
       <c r="I4" s="102">
         <f>COUNTIF(H3:H788,"Result")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J4" s="89"/>
       <c r="K4" s="90"/>
@@ -3007,39 +3178,39 @@
       <c r="A7" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="138" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="138"/>
-      <c r="H7" s="138"/>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="138"/>
+      <c r="B7" s="162" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="162"/>
+      <c r="H7" s="162"/>
+      <c r="I7" s="162"/>
+      <c r="J7" s="162"/>
+      <c r="K7" s="162"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="142"/>
-      <c r="D8" s="141" t="s">
+      <c r="C8" s="166"/>
+      <c r="D8" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="142"/>
-      <c r="F8" s="141" t="s">
+      <c r="E8" s="166"/>
+      <c r="F8" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="142"/>
-      <c r="H8" s="140" t="s">
+      <c r="G8" s="166"/>
+      <c r="H8" s="164" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="140"/>
+      <c r="I8" s="164"/>
       <c r="J8" s="118" t="s">
         <v>39</v>
       </c>
@@ -3051,33 +3222,33 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="160" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="161"/>
-      <c r="D9" s="151" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="152"/>
+      <c r="B9" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="140"/>
+      <c r="D9" s="145" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="146"/>
       <c r="F9" s="120" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G9" s="121"/>
-      <c r="H9" s="149" t="s">
+      <c r="H9" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="150"/>
+      <c r="I9" s="152"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="146"/>
+      <c r="K9" s="153"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="162"/>
-      <c r="C10" s="163"/>
-      <c r="D10" s="153"/>
-      <c r="E10" s="154"/>
+      <c r="B10" s="141"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="147"/>
+      <c r="E10" s="148"/>
       <c r="F10" s="122"/>
       <c r="G10" s="123"/>
       <c r="H10" s="117" t="s">
@@ -3089,33 +3260,33 @@
       <c r="J10" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="147"/>
+      <c r="K10" s="154"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="162"/>
-      <c r="C11" s="163"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="154"/>
+        <v>69</v>
+      </c>
+      <c r="B11" s="141"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="147"/>
+      <c r="E11" s="148"/>
       <c r="F11" s="122"/>
       <c r="G11" s="123"/>
       <c r="H11" s="50" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="147"/>
+      <c r="K11" s="154"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="162"/>
-      <c r="C12" s="163"/>
-      <c r="D12" s="153"/>
-      <c r="E12" s="154"/>
+      <c r="B12" s="141"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="148"/>
       <c r="F12" s="122"/>
       <c r="G12" s="123"/>
       <c r="H12" s="117" t="s">
@@ -3125,45 +3296,45 @@
         <v>48</v>
       </c>
       <c r="J12" s="117"/>
-      <c r="K12" s="147"/>
+      <c r="K12" s="154"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>981</v>
       </c>
-      <c r="B13" s="164"/>
-      <c r="C13" s="165"/>
-      <c r="D13" s="155"/>
-      <c r="E13" s="156"/>
+      <c r="B13" s="143"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="149"/>
+      <c r="E13" s="150"/>
       <c r="F13" s="124"/>
       <c r="G13" s="125"/>
       <c r="H13" s="53" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="148"/>
+      <c r="K13" s="155"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="144" t="s">
+      <c r="B14" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="145"/>
-      <c r="D14" s="144" t="s">
+      <c r="C14" s="160"/>
+      <c r="D14" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="145"/>
-      <c r="F14" s="144" t="s">
+      <c r="E14" s="160"/>
+      <c r="F14" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="145"/>
-      <c r="H14" s="157" t="s">
+      <c r="G14" s="160"/>
+      <c r="H14" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="157"/>
+      <c r="I14" s="161"/>
       <c r="J14" s="126" t="s">
         <v>39</v>
       </c>
@@ -3175,35 +3346,35 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="160" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="161"/>
-      <c r="D15" s="151" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="152"/>
+      <c r="B15" s="139" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="140"/>
+      <c r="D15" s="145" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="146"/>
       <c r="F15" s="120" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G15" s="121"/>
-      <c r="H15" s="158" t="s">
+      <c r="H15" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="159"/>
+      <c r="I15" s="169"/>
       <c r="J15" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="K15" s="146"/>
+        <v>64</v>
+      </c>
+      <c r="K15" s="153"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="162"/>
-      <c r="C16" s="163"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="154"/>
+      <c r="B16" s="141"/>
+      <c r="C16" s="142"/>
+      <c r="D16" s="147"/>
+      <c r="E16" s="148"/>
       <c r="F16" s="122"/>
       <c r="G16" s="123"/>
       <c r="H16" s="126" t="s">
@@ -3215,35 +3386,35 @@
       <c r="J16" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="147"/>
+      <c r="K16" s="154"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="162"/>
-      <c r="C17" s="163"/>
-      <c r="D17" s="153"/>
-      <c r="E17" s="154"/>
+        <v>70</v>
+      </c>
+      <c r="B17" s="141"/>
+      <c r="C17" s="142"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="148"/>
       <c r="F17" s="122"/>
       <c r="G17" s="123"/>
       <c r="H17" s="50" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="K17" s="147"/>
+        <v>65</v>
+      </c>
+      <c r="K17" s="154"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="162"/>
-      <c r="C18" s="163"/>
-      <c r="D18" s="153"/>
-      <c r="E18" s="154"/>
+      <c r="B18" s="141"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="148"/>
       <c r="F18" s="122"/>
       <c r="G18" s="123"/>
       <c r="H18" s="126" t="s">
@@ -3253,45 +3424,45 @@
         <v>48</v>
       </c>
       <c r="J18" s="126"/>
-      <c r="K18" s="147"/>
+      <c r="K18" s="154"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>921</v>
       </c>
-      <c r="B19" s="164"/>
-      <c r="C19" s="165"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="156"/>
+      <c r="B19" s="143"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="149"/>
+      <c r="E19" s="150"/>
       <c r="F19" s="124"/>
       <c r="G19" s="125"/>
       <c r="H19" s="50" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="147"/>
+      <c r="K19" s="154"/>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A20" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="141" t="s">
+      <c r="B20" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="142"/>
-      <c r="D20" s="141" t="s">
+      <c r="C20" s="166"/>
+      <c r="D20" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="142"/>
-      <c r="F20" s="141" t="s">
+      <c r="E20" s="166"/>
+      <c r="F20" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="142"/>
-      <c r="H20" s="140" t="s">
+      <c r="G20" s="166"/>
+      <c r="H20" s="164" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="140"/>
+      <c r="I20" s="164"/>
       <c r="J20" s="128" t="s">
         <v>39</v>
       </c>
@@ -3303,33 +3474,33 @@
       <c r="A21" s="48">
         <v>3</v>
       </c>
-      <c r="B21" s="160" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="161"/>
-      <c r="D21" s="151" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="152"/>
+      <c r="B21" s="139" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="140"/>
+      <c r="D21" s="145" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="146"/>
       <c r="F21" s="129" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G21" s="130"/>
-      <c r="H21" s="149" t="s">
+      <c r="H21" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="150"/>
+      <c r="I21" s="152"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="146"/>
+      <c r="K21" s="153"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="162"/>
-      <c r="C22" s="163"/>
-      <c r="D22" s="153"/>
-      <c r="E22" s="154"/>
+      <c r="B22" s="141"/>
+      <c r="C22" s="142"/>
+      <c r="D22" s="147"/>
+      <c r="E22" s="148"/>
       <c r="F22" s="131"/>
       <c r="G22" s="132"/>
       <c r="H22" s="127" t="s">
@@ -3341,33 +3512,33 @@
       <c r="J22" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="147"/>
+      <c r="K22" s="154"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="162"/>
-      <c r="C23" s="163"/>
-      <c r="D23" s="153"/>
-      <c r="E23" s="154"/>
+        <v>68</v>
+      </c>
+      <c r="B23" s="141"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="147"/>
+      <c r="E23" s="148"/>
       <c r="F23" s="131"/>
       <c r="G23" s="132"/>
       <c r="H23" s="50" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="147"/>
+      <c r="K23" s="154"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="127" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="162"/>
-      <c r="C24" s="163"/>
-      <c r="D24" s="153"/>
-      <c r="E24" s="154"/>
+      <c r="B24" s="141"/>
+      <c r="C24" s="142"/>
+      <c r="D24" s="147"/>
+      <c r="E24" s="148"/>
       <c r="F24" s="131"/>
       <c r="G24" s="132"/>
       <c r="H24" s="127" t="s">
@@ -3377,79 +3548,79 @@
         <v>48</v>
       </c>
       <c r="J24" s="127"/>
-      <c r="K24" s="147"/>
+      <c r="K24" s="154"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>982</v>
       </c>
-      <c r="B25" s="164"/>
-      <c r="C25" s="165"/>
-      <c r="D25" s="155"/>
-      <c r="E25" s="156"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="149"/>
+      <c r="E25" s="150"/>
       <c r="F25" s="133"/>
       <c r="G25" s="134"/>
       <c r="H25" s="50" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I25" s="50"/>
       <c r="J25" s="48"/>
-      <c r="K25" s="148"/>
+      <c r="K25" s="155"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="143" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="143"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
-      <c r="G26" s="138"/>
-      <c r="H26" s="138"/>
-      <c r="I26" s="138"/>
-      <c r="J26" s="138"/>
-      <c r="K26" s="138"/>
+      <c r="B26" s="167" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="167"/>
+      <c r="D26" s="162"/>
+      <c r="E26" s="162"/>
+      <c r="F26" s="162"/>
+      <c r="G26" s="162"/>
+      <c r="H26" s="162"/>
+      <c r="I26" s="162"/>
+      <c r="J26" s="162"/>
+      <c r="K26" s="162"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="166" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="167"/>
-      <c r="D27" s="167"/>
-      <c r="E27" s="167"/>
-      <c r="F27" s="167"/>
-      <c r="G27" s="167"/>
-      <c r="H27" s="167"/>
-      <c r="I27" s="167"/>
-      <c r="J27" s="167"/>
-      <c r="K27" s="168"/>
+      <c r="B27" s="156" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="157"/>
+      <c r="H27" s="157"/>
+      <c r="I27" s="157"/>
+      <c r="J27" s="157"/>
+      <c r="K27" s="158"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="135" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="144" t="s">
+      <c r="B28" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="145"/>
-      <c r="D28" s="144" t="s">
+      <c r="C28" s="160"/>
+      <c r="D28" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="145"/>
-      <c r="F28" s="144" t="s">
+      <c r="E28" s="160"/>
+      <c r="F28" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="145"/>
-      <c r="H28" s="157" t="s">
+      <c r="G28" s="160"/>
+      <c r="H28" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="I28" s="157"/>
+      <c r="I28" s="161"/>
       <c r="J28" s="135" t="s">
         <v>39</v>
       </c>
@@ -3462,35 +3633,37 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B29" s="160" t="s">
+      <c r="B29" s="139" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="140"/>
+      <c r="D29" s="145" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="146"/>
+      <c r="F29" s="145" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="161"/>
-      <c r="D29" s="151" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="152"/>
-      <c r="F29" s="151" t="s">
+      <c r="G29" s="146"/>
+      <c r="H29" s="151" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="152"/>
+      <c r="J29" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="152"/>
-      <c r="H29" s="149" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="150"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="146"/>
+      <c r="K29" s="153"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="162"/>
-      <c r="C30" s="163"/>
-      <c r="D30" s="153"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="153"/>
-      <c r="G30" s="154"/>
+      <c r="B30" s="141"/>
+      <c r="C30" s="142"/>
+      <c r="D30" s="147"/>
+      <c r="E30" s="148"/>
+      <c r="F30" s="147"/>
+      <c r="G30" s="148"/>
       <c r="H30" s="126" t="s">
         <v>42</v>
       </c>
@@ -3500,79 +3673,79 @@
       <c r="J30" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="K30" s="147"/>
+      <c r="K30" s="154"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="162"/>
-      <c r="C31" s="163"/>
-      <c r="D31" s="153"/>
-      <c r="E31" s="154"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="154"/>
+        <v>56</v>
+      </c>
+      <c r="B31" s="141"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="147"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="147"/>
+      <c r="G31" s="148"/>
       <c r="H31" s="50" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I31" s="50"/>
       <c r="J31" s="48"/>
-      <c r="K31" s="147"/>
+      <c r="K31" s="154"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="162"/>
-      <c r="C32" s="163"/>
-      <c r="D32" s="153"/>
-      <c r="E32" s="154"/>
-      <c r="F32" s="153"/>
-      <c r="G32" s="154"/>
+      <c r="B32" s="141"/>
+      <c r="C32" s="142"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="148"/>
+      <c r="F32" s="147"/>
+      <c r="G32" s="148"/>
       <c r="H32" s="126" t="s">
         <v>47</v>
       </c>
       <c r="I32" s="126"/>
       <c r="J32" s="126"/>
-      <c r="K32" s="147"/>
+      <c r="K32" s="154"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
       <c r="A33" s="51">
         <v>922</v>
       </c>
-      <c r="B33" s="164"/>
-      <c r="C33" s="165"/>
-      <c r="D33" s="155"/>
-      <c r="E33" s="156"/>
-      <c r="F33" s="155"/>
-      <c r="G33" s="156"/>
+      <c r="B33" s="143"/>
+      <c r="C33" s="144"/>
+      <c r="D33" s="149"/>
+      <c r="E33" s="150"/>
+      <c r="F33" s="149"/>
+      <c r="G33" s="150"/>
       <c r="H33" s="50" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I33" s="50"/>
       <c r="J33" s="48"/>
-      <c r="K33" s="148"/>
+      <c r="K33" s="155"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="141" t="s">
+      <c r="B34" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="142"/>
-      <c r="D34" s="141" t="s">
+      <c r="C34" s="166"/>
+      <c r="D34" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="142"/>
-      <c r="F34" s="141" t="s">
+      <c r="E34" s="166"/>
+      <c r="F34" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="142"/>
-      <c r="H34" s="139" t="s">
+      <c r="G34" s="166"/>
+      <c r="H34" s="163" t="s">
         <v>38</v>
       </c>
-      <c r="I34" s="139"/>
+      <c r="I34" s="163"/>
       <c r="J34" s="117" t="s">
         <v>39</v>
       </c>
@@ -3584,37 +3757,35 @@
       <c r="A35" s="48">
         <v>4</v>
       </c>
-      <c r="B35" s="160" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="161"/>
-      <c r="D35" s="151" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" s="152"/>
-      <c r="F35" s="151" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" s="152"/>
-      <c r="H35" s="158" t="s">
+      <c r="B35" s="139" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="140"/>
+      <c r="D35" s="145" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="146"/>
+      <c r="F35" s="145" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="146"/>
+      <c r="H35" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="I35" s="159"/>
-      <c r="J35" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="K35" s="146"/>
+      <c r="I35" s="169"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="153"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="162"/>
-      <c r="C36" s="163"/>
-      <c r="D36" s="153"/>
-      <c r="E36" s="154"/>
-      <c r="F36" s="153"/>
-      <c r="G36" s="154"/>
+      <c r="B36" s="141"/>
+      <c r="C36" s="142"/>
+      <c r="D36" s="147"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="147"/>
+      <c r="G36" s="148"/>
       <c r="H36" s="117" t="s">
         <v>42</v>
       </c>
@@ -3624,18 +3795,18 @@
       <c r="J36" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="147"/>
+      <c r="K36" s="154"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="162"/>
-      <c r="C37" s="163"/>
-      <c r="D37" s="153"/>
-      <c r="E37" s="154"/>
-      <c r="F37" s="153"/>
-      <c r="G37" s="154"/>
+        <v>57</v>
+      </c>
+      <c r="B37" s="141"/>
+      <c r="C37" s="142"/>
+      <c r="D37" s="147"/>
+      <c r="E37" s="148"/>
+      <c r="F37" s="147"/>
+      <c r="G37" s="148"/>
       <c r="H37" s="50" t="s">
         <v>45</v>
       </c>
@@ -3645,18 +3816,18 @@
       <c r="J37" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="K37" s="147"/>
+      <c r="K37" s="154"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="162"/>
-      <c r="C38" s="163"/>
-      <c r="D38" s="153"/>
-      <c r="E38" s="154"/>
-      <c r="F38" s="153"/>
-      <c r="G38" s="154"/>
+      <c r="B38" s="141"/>
+      <c r="C38" s="142"/>
+      <c r="D38" s="147"/>
+      <c r="E38" s="148"/>
+      <c r="F38" s="147"/>
+      <c r="G38" s="148"/>
       <c r="H38" s="117" t="s">
         <v>47</v>
       </c>
@@ -3664,18 +3835,18 @@
         <v>48</v>
       </c>
       <c r="J38" s="117"/>
-      <c r="K38" s="147"/>
+      <c r="K38" s="154"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
       <c r="A39" s="51">
         <v>823</v>
       </c>
-      <c r="B39" s="164"/>
-      <c r="C39" s="165"/>
-      <c r="D39" s="155"/>
-      <c r="E39" s="156"/>
-      <c r="F39" s="155"/>
-      <c r="G39" s="156"/>
+      <c r="B39" s="143"/>
+      <c r="C39" s="144"/>
+      <c r="D39" s="149"/>
+      <c r="E39" s="150"/>
+      <c r="F39" s="149"/>
+      <c r="G39" s="150"/>
       <c r="H39" s="50" t="s">
         <v>49</v>
       </c>
@@ -3683,28 +3854,28 @@
         <v>53</v>
       </c>
       <c r="J39" s="48"/>
-      <c r="K39" s="148"/>
+      <c r="K39" s="155"/>
     </row>
     <row r="40" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A40" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="141" t="s">
+      <c r="B40" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="142"/>
-      <c r="D40" s="141" t="s">
+      <c r="C40" s="166"/>
+      <c r="D40" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="142"/>
-      <c r="F40" s="141" t="s">
+      <c r="E40" s="166"/>
+      <c r="F40" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="G40" s="142"/>
-      <c r="H40" s="139" t="s">
+      <c r="G40" s="166"/>
+      <c r="H40" s="163" t="s">
         <v>38</v>
       </c>
-      <c r="I40" s="139"/>
+      <c r="I40" s="163"/>
       <c r="J40" s="117" t="s">
         <v>39</v>
       </c>
@@ -3716,37 +3887,35 @@
       <c r="A41" s="48">
         <v>5</v>
       </c>
-      <c r="B41" s="160" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="161"/>
-      <c r="D41" s="151" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="152"/>
-      <c r="F41" s="151" t="s">
-        <v>57</v>
-      </c>
-      <c r="G41" s="152"/>
-      <c r="H41" s="158" t="s">
+      <c r="B41" s="139" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="140"/>
+      <c r="D41" s="145" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="146"/>
+      <c r="F41" s="145" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" s="146"/>
+      <c r="H41" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="I41" s="159"/>
-      <c r="J41" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="K41" s="146"/>
+      <c r="I41" s="169"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="153"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
       <c r="A42" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="162"/>
-      <c r="C42" s="163"/>
-      <c r="D42" s="153"/>
-      <c r="E42" s="154"/>
-      <c r="F42" s="153"/>
-      <c r="G42" s="154"/>
+      <c r="B42" s="141"/>
+      <c r="C42" s="142"/>
+      <c r="D42" s="147"/>
+      <c r="E42" s="148"/>
+      <c r="F42" s="147"/>
+      <c r="G42" s="148"/>
       <c r="H42" s="117" t="s">
         <v>42</v>
       </c>
@@ -3756,39 +3925,35 @@
       <c r="J42" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="K42" s="147"/>
+      <c r="K42" s="154"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
       <c r="A43" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="162"/>
-      <c r="C43" s="163"/>
-      <c r="D43" s="153"/>
-      <c r="E43" s="154"/>
-      <c r="F43" s="153"/>
-      <c r="G43" s="154"/>
+        <v>57</v>
+      </c>
+      <c r="B43" s="141"/>
+      <c r="C43" s="142"/>
+      <c r="D43" s="147"/>
+      <c r="E43" s="148"/>
+      <c r="F43" s="147"/>
+      <c r="G43" s="148"/>
       <c r="H43" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="I43" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J43" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="K43" s="147"/>
+        <v>60</v>
+      </c>
+      <c r="I43" s="50"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="154"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
       <c r="A44" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="162"/>
-      <c r="C44" s="163"/>
-      <c r="D44" s="153"/>
-      <c r="E44" s="154"/>
-      <c r="F44" s="153"/>
-      <c r="G44" s="154"/>
+      <c r="B44" s="141"/>
+      <c r="C44" s="142"/>
+      <c r="D44" s="147"/>
+      <c r="E44" s="148"/>
+      <c r="F44" s="147"/>
+      <c r="G44" s="148"/>
       <c r="H44" s="117" t="s">
         <v>47</v>
       </c>
@@ -3796,33 +3961,166 @@
         <v>48</v>
       </c>
       <c r="J44" s="117"/>
-      <c r="K44" s="147"/>
+      <c r="K44" s="154"/>
     </row>
     <row r="45" spans="1:11" ht="10.5" customHeight="1">
       <c r="A45" s="51">
         <v>823</v>
       </c>
-      <c r="B45" s="164"/>
-      <c r="C45" s="165"/>
-      <c r="D45" s="155"/>
-      <c r="E45" s="156"/>
-      <c r="F45" s="155"/>
-      <c r="G45" s="156"/>
+      <c r="B45" s="143"/>
+      <c r="C45" s="144"/>
+      <c r="D45" s="149"/>
+      <c r="E45" s="150"/>
+      <c r="F45" s="149"/>
+      <c r="G45" s="150"/>
       <c r="H45" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I45" s="50" t="s">
-        <v>53</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="I45" s="50"/>
       <c r="J45" s="48"/>
-      <c r="K45" s="148"/>
-    </row>
-    <row r="46" spans="1:11" s="58" customFormat="1">
-      <c r="A46" s="62"/>
-      <c r="H46" s="62"/>
-      <c r="I46" s="62"/>
-      <c r="J46" s="62"/>
-      <c r="K46" s="62"/>
+      <c r="K45" s="155"/>
+    </row>
+    <row r="46" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A46" s="100" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="157"/>
+      <c r="D46" s="157"/>
+      <c r="E46" s="157"/>
+      <c r="F46" s="157"/>
+      <c r="G46" s="157"/>
+      <c r="H46" s="157"/>
+      <c r="I46" s="157"/>
+      <c r="J46" s="157"/>
+      <c r="K46" s="158"/>
+    </row>
+    <row r="47" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A47" s="136" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="159" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="160"/>
+      <c r="D47" s="159" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="160"/>
+      <c r="F47" s="159" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" s="160"/>
+      <c r="H47" s="161" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="161"/>
+      <c r="J47" s="136" t="s">
+        <v>39</v>
+      </c>
+      <c r="K47" s="136" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A48" s="48" t="e">
+        <f>A34+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B48" s="139" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="140"/>
+      <c r="D48" s="145" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" s="146"/>
+      <c r="F48" s="145" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" s="146"/>
+      <c r="H48" s="151" t="s">
+        <v>10</v>
+      </c>
+      <c r="I48" s="152"/>
+      <c r="J48" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="K48" s="153"/>
+    </row>
+    <row r="49" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A49" s="136" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="141"/>
+      <c r="C49" s="142"/>
+      <c r="D49" s="147"/>
+      <c r="E49" s="148"/>
+      <c r="F49" s="147"/>
+      <c r="G49" s="148"/>
+      <c r="H49" s="136" t="s">
+        <v>42</v>
+      </c>
+      <c r="I49" s="136" t="s">
+        <v>43</v>
+      </c>
+      <c r="J49" s="136" t="s">
+        <v>44</v>
+      </c>
+      <c r="K49" s="154"/>
+    </row>
+    <row r="50" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A50" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="141"/>
+      <c r="C50" s="142"/>
+      <c r="D50" s="147"/>
+      <c r="E50" s="148"/>
+      <c r="F50" s="147"/>
+      <c r="G50" s="148"/>
+      <c r="H50" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="I50" s="50"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="154"/>
+    </row>
+    <row r="51" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A51" s="136" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="141"/>
+      <c r="C51" s="142"/>
+      <c r="D51" s="147"/>
+      <c r="E51" s="148"/>
+      <c r="F51" s="147"/>
+      <c r="G51" s="148"/>
+      <c r="H51" s="136" t="s">
+        <v>47</v>
+      </c>
+      <c r="I51" s="136"/>
+      <c r="J51" s="136"/>
+      <c r="K51" s="154"/>
+    </row>
+    <row r="52" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A52" s="51">
+        <v>922</v>
+      </c>
+      <c r="B52" s="143"/>
+      <c r="C52" s="144"/>
+      <c r="D52" s="149"/>
+      <c r="E52" s="150"/>
+      <c r="F52" s="149"/>
+      <c r="G52" s="150"/>
+      <c r="H52" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="I52" s="50"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="155"/>
     </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
       <c r="A67" s="62"/>
@@ -4035,7 +4333,7 @@
       <c r="K96" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="64">
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C13"/>
     <mergeCell ref="H28:I28"/>
@@ -4090,6 +4388,16 @@
     <mergeCell ref="D29:E33"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F29:G33"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="B48:C52"/>
+    <mergeCell ref="D48:E52"/>
+    <mergeCell ref="F48:G52"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="K48:K52"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H41:I41">

</xml_diff>

<commit_message>
test chuc nang doi mat khau va phe duyet bai dang
</commit_message>
<xml_diff>
--- a/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$72</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -47,157 +47,6 @@
           </rPr>
           <t xml:space="preserve">Point \ Point 
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H28" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Kết quả test:
-OK / Not OK</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J28" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Ánh xạ tới ID tương ứng của Bug được ghi nhận trong BugList</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A29" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Số thứ tự tăng dần testcase, không phần biệt sheet,...
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Người thực hiện test</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Người chịu trách nhiệm về lỗi</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Người sửa lỗi</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A31" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>SheetNo.Suite.Suite-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>CaseNo</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-CaseNo tăng dần và lặp lại từ 1 giữa các Suite-Point khác nhau</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H32" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Ngày thực hiện test</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I32" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>Ngày test lại, trong trường hợp lần test trước có lỗi</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>ID tương ứng của TestLink</t>
         </r>
       </text>
     </comment>
@@ -371,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="94">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -598,9 +447,6 @@
   </si>
   <si>
     <t>Test với chức năng tìm kiếm</t>
-  </si>
-  <si>
-    <t>Tìm kiếm nội dung theo nội dung phê duyệt</t>
   </si>
   <si>
     <t xml:space="preserve">Tìm kiếm nội dung theo ngày tạo
@@ -632,9 +478,6 @@
     <t>BUG212</t>
   </si>
   <si>
-    <t>Test với chức năng đổi mật khẩu</t>
-  </si>
-  <si>
     <t>Tìm kiếm nội dung theo trạng thái phê duyệt</t>
   </si>
   <si>
@@ -645,6 +488,33 @@
     <t>1. Gõ nội dung
 2. Chọn tiêu chí sắp xếp theo số lượng comment
 3. Bấm lọc</t>
+  </si>
+  <si>
+    <t>Đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>Khi người quản trị muốn đổi mật khẩu. Bấm vào button đổi mật khẩu để thực hiện.</t>
+  </si>
+  <si>
+    <t>Đổi được mật khẩu</t>
+  </si>
+  <si>
+    <t>BUG213</t>
+  </si>
+  <si>
+    <t>Test với một vài chức năng khác</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phê duyệt bài đăng
+</t>
+  </si>
+  <si>
+    <t>1. Bấm vào nút phê duyệt
+2. Một thông báo xuất hiện để xác nhận
+3. Trạng thái của bài đăng được chuyển sang đã phê duyệt.</t>
+  </si>
+  <si>
+    <t>Phê duyệt được bài đăng</t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1025,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1483,6 +1353,12 @@
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1490,6 +1366,12 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1508,6 +1390,24 @@
     <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1526,11 +1426,23 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1541,54 +1453,32 @@
     <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2103,13 +1993,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="137" t="s">
+      <c r="O6" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="137"/>
-      <c r="Q6" s="137"/>
-      <c r="R6" s="137"/>
-      <c r="S6" s="137"/>
+      <c r="P6" s="139"/>
+      <c r="Q6" s="139"/>
+      <c r="R6" s="139"/>
+      <c r="S6" s="139"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -2119,11 +2009,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="137"/>
-      <c r="P7" s="137"/>
-      <c r="Q7" s="137"/>
-      <c r="R7" s="137"/>
-      <c r="S7" s="137"/>
+      <c r="O7" s="139"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="139"/>
+      <c r="R7" s="139"/>
+      <c r="S7" s="139"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -2178,12 +2068,12 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="138">
+      <c r="E11" s="140">
         <f ca="1">TODAY()</f>
         <v>43449</v>
       </c>
-      <c r="F11" s="138"/>
-      <c r="G11" s="138"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
       <c r="H11" s="72"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
@@ -3043,8 +2933,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41:E45"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54:I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -3075,7 +2965,7 @@
       </c>
       <c r="I1" s="101">
         <f>COUNTIF(H1:H786,"OK")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" s="82" t="s">
         <v>23</v>
@@ -3143,7 +3033,7 @@
       <c r="H4" s="85"/>
       <c r="I4" s="102">
         <f>COUNTIF(H3:H788,"Result")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J4" s="89"/>
       <c r="K4" s="90"/>
@@ -3178,39 +3068,39 @@
       <c r="A7" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="170" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="162"/>
-      <c r="D7" s="162"/>
-      <c r="E7" s="162"/>
-      <c r="F7" s="162"/>
-      <c r="G7" s="162"/>
-      <c r="H7" s="162"/>
-      <c r="I7" s="162"/>
-      <c r="J7" s="162"/>
-      <c r="K7" s="162"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="170"/>
+      <c r="H7" s="170"/>
+      <c r="I7" s="170"/>
+      <c r="J7" s="170"/>
+      <c r="K7" s="170"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="165" t="s">
+      <c r="B8" s="141" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="166"/>
-      <c r="D8" s="165" t="s">
+      <c r="C8" s="142"/>
+      <c r="D8" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="166"/>
-      <c r="F8" s="165" t="s">
+      <c r="E8" s="142"/>
+      <c r="F8" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="166"/>
-      <c r="H8" s="164" t="s">
+      <c r="G8" s="142"/>
+      <c r="H8" s="166" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="164"/>
+      <c r="I8" s="166"/>
       <c r="J8" s="118" t="s">
         <v>39</v>
       </c>
@@ -3222,33 +3112,33 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="139" t="s">
+      <c r="B9" s="143" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="145" t="s">
+      <c r="C9" s="144"/>
+      <c r="D9" s="155" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="146"/>
+      <c r="E9" s="156"/>
       <c r="F9" s="120" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9" s="121"/>
-      <c r="H9" s="151" t="s">
+      <c r="H9" s="152" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="152"/>
+      <c r="I9" s="153"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="153"/>
+      <c r="K9" s="167"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="141"/>
-      <c r="C10" s="142"/>
-      <c r="D10" s="147"/>
-      <c r="E10" s="148"/>
+      <c r="B10" s="145"/>
+      <c r="C10" s="146"/>
+      <c r="D10" s="157"/>
+      <c r="E10" s="158"/>
       <c r="F10" s="122"/>
       <c r="G10" s="123"/>
       <c r="H10" s="117" t="s">
@@ -3260,16 +3150,16 @@
       <c r="J10" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="154"/>
+      <c r="K10" s="168"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="141"/>
-      <c r="C11" s="142"/>
-      <c r="D11" s="147"/>
-      <c r="E11" s="148"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="146"/>
+      <c r="D11" s="157"/>
+      <c r="E11" s="158"/>
       <c r="F11" s="122"/>
       <c r="G11" s="123"/>
       <c r="H11" s="50" t="s">
@@ -3277,16 +3167,16 @@
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="154"/>
+      <c r="K11" s="168"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="141"/>
-      <c r="C12" s="142"/>
-      <c r="D12" s="147"/>
-      <c r="E12" s="148"/>
+      <c r="B12" s="145"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="157"/>
+      <c r="E12" s="158"/>
       <c r="F12" s="122"/>
       <c r="G12" s="123"/>
       <c r="H12" s="117" t="s">
@@ -3296,16 +3186,16 @@
         <v>48</v>
       </c>
       <c r="J12" s="117"/>
-      <c r="K12" s="154"/>
+      <c r="K12" s="168"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>981</v>
       </c>
-      <c r="B13" s="143"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="149"/>
-      <c r="E13" s="150"/>
+      <c r="B13" s="147"/>
+      <c r="C13" s="148"/>
+      <c r="D13" s="159"/>
+      <c r="E13" s="160"/>
       <c r="F13" s="124"/>
       <c r="G13" s="125"/>
       <c r="H13" s="53" t="s">
@@ -3313,28 +3203,28 @@
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="155"/>
+      <c r="K13" s="169"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="159" t="s">
+      <c r="B14" s="150" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="160"/>
-      <c r="D14" s="159" t="s">
+      <c r="C14" s="151"/>
+      <c r="D14" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="159" t="s">
+      <c r="E14" s="151"/>
+      <c r="F14" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="160"/>
-      <c r="H14" s="161" t="s">
+      <c r="G14" s="151"/>
+      <c r="H14" s="149" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="161"/>
+      <c r="I14" s="149"/>
       <c r="J14" s="126" t="s">
         <v>39</v>
       </c>
@@ -3346,35 +3236,35 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="139" t="s">
+      <c r="B15" s="143" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="140"/>
-      <c r="D15" s="145" t="s">
+      <c r="C15" s="144"/>
+      <c r="D15" s="155" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="146"/>
+      <c r="E15" s="156"/>
       <c r="F15" s="120" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15" s="121"/>
-      <c r="H15" s="168" t="s">
+      <c r="H15" s="161" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="169"/>
+      <c r="I15" s="162"/>
       <c r="J15" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="K15" s="153"/>
+      <c r="K15" s="167"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="141"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="147"/>
-      <c r="E16" s="148"/>
+      <c r="B16" s="145"/>
+      <c r="C16" s="146"/>
+      <c r="D16" s="157"/>
+      <c r="E16" s="158"/>
       <c r="F16" s="122"/>
       <c r="G16" s="123"/>
       <c r="H16" s="126" t="s">
@@ -3386,16 +3276,16 @@
       <c r="J16" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="154"/>
+      <c r="K16" s="168"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="141"/>
-      <c r="C17" s="142"/>
-      <c r="D17" s="147"/>
-      <c r="E17" s="148"/>
+      <c r="B17" s="145"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="157"/>
+      <c r="E17" s="158"/>
       <c r="F17" s="122"/>
       <c r="G17" s="123"/>
       <c r="H17" s="50" t="s">
@@ -3405,16 +3295,16 @@
       <c r="J17" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="K17" s="154"/>
+      <c r="K17" s="168"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="141"/>
-      <c r="C18" s="142"/>
-      <c r="D18" s="147"/>
-      <c r="E18" s="148"/>
+      <c r="B18" s="145"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="157"/>
+      <c r="E18" s="158"/>
       <c r="F18" s="122"/>
       <c r="G18" s="123"/>
       <c r="H18" s="126" t="s">
@@ -3424,16 +3314,16 @@
         <v>48</v>
       </c>
       <c r="J18" s="126"/>
-      <c r="K18" s="154"/>
+      <c r="K18" s="168"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>921</v>
       </c>
-      <c r="B19" s="143"/>
-      <c r="C19" s="144"/>
-      <c r="D19" s="149"/>
-      <c r="E19" s="150"/>
+      <c r="B19" s="147"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="159"/>
+      <c r="E19" s="160"/>
       <c r="F19" s="124"/>
       <c r="G19" s="125"/>
       <c r="H19" s="50" t="s">
@@ -3441,28 +3331,28 @@
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="154"/>
+      <c r="K19" s="168"/>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A20" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="165" t="s">
+      <c r="B20" s="141" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="166"/>
-      <c r="D20" s="165" t="s">
+      <c r="C20" s="142"/>
+      <c r="D20" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="166"/>
-      <c r="F20" s="165" t="s">
+      <c r="E20" s="142"/>
+      <c r="F20" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="166"/>
-      <c r="H20" s="164" t="s">
+      <c r="G20" s="142"/>
+      <c r="H20" s="166" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="164"/>
+      <c r="I20" s="166"/>
       <c r="J20" s="128" t="s">
         <v>39</v>
       </c>
@@ -3474,33 +3364,33 @@
       <c r="A21" s="48">
         <v>3</v>
       </c>
-      <c r="B21" s="139" t="s">
+      <c r="B21" s="143" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="140"/>
-      <c r="D21" s="145" t="s">
+      <c r="C21" s="144"/>
+      <c r="D21" s="155" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="146"/>
+      <c r="E21" s="156"/>
       <c r="F21" s="129" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G21" s="130"/>
-      <c r="H21" s="151" t="s">
+      <c r="H21" s="152" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="152"/>
+      <c r="I21" s="153"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="153"/>
+      <c r="K21" s="167"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="141"/>
-      <c r="C22" s="142"/>
-      <c r="D22" s="147"/>
-      <c r="E22" s="148"/>
+      <c r="B22" s="145"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="157"/>
+      <c r="E22" s="158"/>
       <c r="F22" s="131"/>
       <c r="G22" s="132"/>
       <c r="H22" s="127" t="s">
@@ -3512,16 +3402,16 @@
       <c r="J22" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="154"/>
+      <c r="K22" s="168"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="141"/>
-      <c r="C23" s="142"/>
-      <c r="D23" s="147"/>
-      <c r="E23" s="148"/>
+      <c r="B23" s="145"/>
+      <c r="C23" s="146"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="158"/>
       <c r="F23" s="131"/>
       <c r="G23" s="132"/>
       <c r="H23" s="50" t="s">
@@ -3529,16 +3419,16 @@
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="154"/>
+      <c r="K23" s="168"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="127" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="141"/>
-      <c r="C24" s="142"/>
-      <c r="D24" s="147"/>
-      <c r="E24" s="148"/>
+      <c r="B24" s="145"/>
+      <c r="C24" s="146"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="158"/>
       <c r="F24" s="131"/>
       <c r="G24" s="132"/>
       <c r="H24" s="127" t="s">
@@ -3548,16 +3438,16 @@
         <v>48</v>
       </c>
       <c r="J24" s="127"/>
-      <c r="K24" s="154"/>
+      <c r="K24" s="168"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>982</v>
       </c>
-      <c r="B25" s="143"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="149"/>
-      <c r="E25" s="150"/>
+      <c r="B25" s="147"/>
+      <c r="C25" s="148"/>
+      <c r="D25" s="159"/>
+      <c r="E25" s="160"/>
       <c r="F25" s="133"/>
       <c r="G25" s="134"/>
       <c r="H25" s="50" t="s">
@@ -3565,62 +3455,62 @@
       </c>
       <c r="I25" s="50"/>
       <c r="J25" s="48"/>
-      <c r="K25" s="155"/>
+      <c r="K25" s="169"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="167" t="s">
+      <c r="B26" s="171" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="167"/>
-      <c r="D26" s="162"/>
-      <c r="E26" s="162"/>
-      <c r="F26" s="162"/>
-      <c r="G26" s="162"/>
-      <c r="H26" s="162"/>
-      <c r="I26" s="162"/>
-      <c r="J26" s="162"/>
-      <c r="K26" s="162"/>
+      <c r="C26" s="171"/>
+      <c r="D26" s="170"/>
+      <c r="E26" s="170"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="170"/>
+      <c r="I26" s="170"/>
+      <c r="J26" s="170"/>
+      <c r="K26" s="170"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="156" t="s">
+      <c r="B27" s="163" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="157"/>
-      <c r="D27" s="157"/>
-      <c r="E27" s="157"/>
-      <c r="F27" s="157"/>
-      <c r="G27" s="157"/>
-      <c r="H27" s="157"/>
-      <c r="I27" s="157"/>
-      <c r="J27" s="157"/>
-      <c r="K27" s="158"/>
+      <c r="C27" s="164"/>
+      <c r="D27" s="164"/>
+      <c r="E27" s="164"/>
+      <c r="F27" s="164"/>
+      <c r="G27" s="164"/>
+      <c r="H27" s="164"/>
+      <c r="I27" s="164"/>
+      <c r="J27" s="164"/>
+      <c r="K27" s="165"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="135" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="159" t="s">
+      <c r="B28" s="150" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="160"/>
-      <c r="D28" s="159" t="s">
+      <c r="C28" s="151"/>
+      <c r="D28" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="160"/>
-      <c r="F28" s="159" t="s">
+      <c r="E28" s="151"/>
+      <c r="F28" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="160"/>
-      <c r="H28" s="161" t="s">
+      <c r="G28" s="151"/>
+      <c r="H28" s="149" t="s">
         <v>38</v>
       </c>
-      <c r="I28" s="161"/>
+      <c r="I28" s="149"/>
       <c r="J28" s="135" t="s">
         <v>39</v>
       </c>
@@ -3633,37 +3523,37 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B29" s="139" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="140"/>
-      <c r="D29" s="145" t="s">
+      <c r="B29" s="143" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="144"/>
+      <c r="D29" s="155" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="156"/>
+      <c r="F29" s="155" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="146"/>
-      <c r="F29" s="145" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" s="146"/>
-      <c r="H29" s="151" t="s">
+      <c r="G29" s="156"/>
+      <c r="H29" s="152" t="s">
         <v>10</v>
       </c>
-      <c r="I29" s="152"/>
+      <c r="I29" s="153"/>
       <c r="J29" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="K29" s="153"/>
+        <v>82</v>
+      </c>
+      <c r="K29" s="167"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="141"/>
-      <c r="C30" s="142"/>
-      <c r="D30" s="147"/>
-      <c r="E30" s="148"/>
-      <c r="F30" s="147"/>
-      <c r="G30" s="148"/>
+      <c r="B30" s="145"/>
+      <c r="C30" s="146"/>
+      <c r="D30" s="157"/>
+      <c r="E30" s="158"/>
+      <c r="F30" s="157"/>
+      <c r="G30" s="158"/>
       <c r="H30" s="126" t="s">
         <v>42</v>
       </c>
@@ -3673,79 +3563,79 @@
       <c r="J30" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="K30" s="154"/>
+      <c r="K30" s="168"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="141"/>
-      <c r="C31" s="142"/>
-      <c r="D31" s="147"/>
-      <c r="E31" s="148"/>
-      <c r="F31" s="147"/>
-      <c r="G31" s="148"/>
+      <c r="B31" s="145"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="157"/>
+      <c r="E31" s="158"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="158"/>
       <c r="H31" s="50" t="s">
         <v>60</v>
       </c>
       <c r="I31" s="50"/>
       <c r="J31" s="48"/>
-      <c r="K31" s="154"/>
+      <c r="K31" s="168"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="141"/>
-      <c r="C32" s="142"/>
-      <c r="D32" s="147"/>
-      <c r="E32" s="148"/>
-      <c r="F32" s="147"/>
-      <c r="G32" s="148"/>
+      <c r="B32" s="145"/>
+      <c r="C32" s="146"/>
+      <c r="D32" s="157"/>
+      <c r="E32" s="158"/>
+      <c r="F32" s="157"/>
+      <c r="G32" s="158"/>
       <c r="H32" s="126" t="s">
         <v>47</v>
       </c>
       <c r="I32" s="126"/>
       <c r="J32" s="126"/>
-      <c r="K32" s="154"/>
+      <c r="K32" s="168"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
       <c r="A33" s="51">
         <v>922</v>
       </c>
-      <c r="B33" s="143"/>
-      <c r="C33" s="144"/>
-      <c r="D33" s="149"/>
-      <c r="E33" s="150"/>
-      <c r="F33" s="149"/>
-      <c r="G33" s="150"/>
+      <c r="B33" s="147"/>
+      <c r="C33" s="148"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="160"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="160"/>
       <c r="H33" s="50" t="s">
         <v>61</v>
       </c>
       <c r="I33" s="50"/>
       <c r="J33" s="48"/>
-      <c r="K33" s="155"/>
+      <c r="K33" s="169"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="165" t="s">
+      <c r="B34" s="141" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="166"/>
-      <c r="D34" s="165" t="s">
+      <c r="C34" s="142"/>
+      <c r="D34" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="166"/>
-      <c r="F34" s="165" t="s">
+      <c r="E34" s="142"/>
+      <c r="F34" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="166"/>
-      <c r="H34" s="163" t="s">
+      <c r="G34" s="142"/>
+      <c r="H34" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="I34" s="163"/>
+      <c r="I34" s="154"/>
       <c r="J34" s="117" t="s">
         <v>39</v>
       </c>
@@ -3757,35 +3647,35 @@
       <c r="A35" s="48">
         <v>4</v>
       </c>
-      <c r="B35" s="139" t="s">
+      <c r="B35" s="143" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="144"/>
+      <c r="D35" s="155" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="140"/>
-      <c r="D35" s="145" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="146"/>
-      <c r="F35" s="145" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" s="146"/>
-      <c r="H35" s="168" t="s">
+      <c r="E35" s="156"/>
+      <c r="F35" s="155" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="156"/>
+      <c r="H35" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="I35" s="169"/>
+      <c r="I35" s="162"/>
       <c r="J35" s="52"/>
-      <c r="K35" s="153"/>
+      <c r="K35" s="167"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="141"/>
-      <c r="C36" s="142"/>
-      <c r="D36" s="147"/>
-      <c r="E36" s="148"/>
-      <c r="F36" s="147"/>
-      <c r="G36" s="148"/>
+      <c r="B36" s="145"/>
+      <c r="C36" s="146"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="158"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="158"/>
       <c r="H36" s="117" t="s">
         <v>42</v>
       </c>
@@ -3795,18 +3685,18 @@
       <c r="J36" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="154"/>
+      <c r="K36" s="168"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="141"/>
-      <c r="C37" s="142"/>
-      <c r="D37" s="147"/>
-      <c r="E37" s="148"/>
-      <c r="F37" s="147"/>
-      <c r="G37" s="148"/>
+      <c r="B37" s="145"/>
+      <c r="C37" s="146"/>
+      <c r="D37" s="157"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="157"/>
+      <c r="G37" s="158"/>
       <c r="H37" s="50" t="s">
         <v>45</v>
       </c>
@@ -3816,18 +3706,18 @@
       <c r="J37" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="K37" s="154"/>
+      <c r="K37" s="168"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="141"/>
-      <c r="C38" s="142"/>
-      <c r="D38" s="147"/>
-      <c r="E38" s="148"/>
-      <c r="F38" s="147"/>
-      <c r="G38" s="148"/>
+      <c r="B38" s="145"/>
+      <c r="C38" s="146"/>
+      <c r="D38" s="157"/>
+      <c r="E38" s="158"/>
+      <c r="F38" s="157"/>
+      <c r="G38" s="158"/>
       <c r="H38" s="117" t="s">
         <v>47</v>
       </c>
@@ -3835,18 +3725,18 @@
         <v>48</v>
       </c>
       <c r="J38" s="117"/>
-      <c r="K38" s="154"/>
+      <c r="K38" s="168"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
       <c r="A39" s="51">
         <v>823</v>
       </c>
-      <c r="B39" s="143"/>
-      <c r="C39" s="144"/>
-      <c r="D39" s="149"/>
-      <c r="E39" s="150"/>
-      <c r="F39" s="149"/>
-      <c r="G39" s="150"/>
+      <c r="B39" s="147"/>
+      <c r="C39" s="148"/>
+      <c r="D39" s="159"/>
+      <c r="E39" s="160"/>
+      <c r="F39" s="159"/>
+      <c r="G39" s="160"/>
       <c r="H39" s="50" t="s">
         <v>49</v>
       </c>
@@ -3854,28 +3744,28 @@
         <v>53</v>
       </c>
       <c r="J39" s="48"/>
-      <c r="K39" s="155"/>
+      <c r="K39" s="169"/>
     </row>
     <row r="40" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A40" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="165" t="s">
+      <c r="B40" s="141" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="166"/>
-      <c r="D40" s="165" t="s">
+      <c r="C40" s="142"/>
+      <c r="D40" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="166"/>
-      <c r="F40" s="165" t="s">
+      <c r="E40" s="142"/>
+      <c r="F40" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="G40" s="166"/>
-      <c r="H40" s="163" t="s">
+      <c r="G40" s="142"/>
+      <c r="H40" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="I40" s="163"/>
+      <c r="I40" s="154"/>
       <c r="J40" s="117" t="s">
         <v>39</v>
       </c>
@@ -3887,35 +3777,35 @@
       <c r="A41" s="48">
         <v>5</v>
       </c>
-      <c r="B41" s="139" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="140"/>
-      <c r="D41" s="145" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" s="146"/>
-      <c r="F41" s="145" t="s">
-        <v>79</v>
-      </c>
-      <c r="G41" s="146"/>
-      <c r="H41" s="168" t="s">
+      <c r="B41" s="143" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="144"/>
+      <c r="D41" s="155" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="156"/>
+      <c r="F41" s="155" t="s">
+        <v>78</v>
+      </c>
+      <c r="G41" s="156"/>
+      <c r="H41" s="161" t="s">
         <v>10</v>
       </c>
-      <c r="I41" s="169"/>
+      <c r="I41" s="162"/>
       <c r="J41" s="52"/>
-      <c r="K41" s="153"/>
+      <c r="K41" s="167"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
       <c r="A42" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="141"/>
-      <c r="C42" s="142"/>
-      <c r="D42" s="147"/>
-      <c r="E42" s="148"/>
-      <c r="F42" s="147"/>
-      <c r="G42" s="148"/>
+      <c r="B42" s="145"/>
+      <c r="C42" s="146"/>
+      <c r="D42" s="157"/>
+      <c r="E42" s="158"/>
+      <c r="F42" s="157"/>
+      <c r="G42" s="158"/>
       <c r="H42" s="117" t="s">
         <v>42</v>
       </c>
@@ -3925,35 +3815,35 @@
       <c r="J42" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="K42" s="154"/>
+      <c r="K42" s="168"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
       <c r="A43" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="141"/>
-      <c r="C43" s="142"/>
-      <c r="D43" s="147"/>
-      <c r="E43" s="148"/>
-      <c r="F43" s="147"/>
-      <c r="G43" s="148"/>
+      <c r="B43" s="145"/>
+      <c r="C43" s="146"/>
+      <c r="D43" s="157"/>
+      <c r="E43" s="158"/>
+      <c r="F43" s="157"/>
+      <c r="G43" s="158"/>
       <c r="H43" s="50" t="s">
         <v>60</v>
       </c>
       <c r="I43" s="50"/>
       <c r="J43" s="48"/>
-      <c r="K43" s="154"/>
+      <c r="K43" s="168"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
       <c r="A44" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="141"/>
-      <c r="C44" s="142"/>
-      <c r="D44" s="147"/>
-      <c r="E44" s="148"/>
-      <c r="F44" s="147"/>
-      <c r="G44" s="148"/>
+      <c r="B44" s="145"/>
+      <c r="C44" s="146"/>
+      <c r="D44" s="157"/>
+      <c r="E44" s="158"/>
+      <c r="F44" s="157"/>
+      <c r="G44" s="158"/>
       <c r="H44" s="117" t="s">
         <v>47</v>
       </c>
@@ -3961,62 +3851,62 @@
         <v>48</v>
       </c>
       <c r="J44" s="117"/>
-      <c r="K44" s="154"/>
+      <c r="K44" s="168"/>
     </row>
     <row r="45" spans="1:11" ht="10.5" customHeight="1">
       <c r="A45" s="51">
         <v>823</v>
       </c>
-      <c r="B45" s="143"/>
-      <c r="C45" s="144"/>
-      <c r="D45" s="149"/>
-      <c r="E45" s="150"/>
-      <c r="F45" s="149"/>
-      <c r="G45" s="150"/>
+      <c r="B45" s="147"/>
+      <c r="C45" s="148"/>
+      <c r="D45" s="159"/>
+      <c r="E45" s="160"/>
+      <c r="F45" s="159"/>
+      <c r="G45" s="160"/>
       <c r="H45" s="50" t="s">
         <v>61</v>
       </c>
       <c r="I45" s="50"/>
       <c r="J45" s="48"/>
-      <c r="K45" s="155"/>
+      <c r="K45" s="169"/>
     </row>
     <row r="46" spans="1:11" ht="10.5" customHeight="1">
       <c r="A46" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="156" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="157"/>
-      <c r="D46" s="157"/>
-      <c r="E46" s="157"/>
-      <c r="F46" s="157"/>
-      <c r="G46" s="157"/>
-      <c r="H46" s="157"/>
-      <c r="I46" s="157"/>
-      <c r="J46" s="157"/>
-      <c r="K46" s="158"/>
+      <c r="B46" s="163" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="164"/>
+      <c r="D46" s="164"/>
+      <c r="E46" s="164"/>
+      <c r="F46" s="164"/>
+      <c r="G46" s="164"/>
+      <c r="H46" s="164"/>
+      <c r="I46" s="164"/>
+      <c r="J46" s="164"/>
+      <c r="K46" s="165"/>
     </row>
     <row r="47" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A47" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="159" t="s">
+      <c r="B47" s="150" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="160"/>
-      <c r="D47" s="159" t="s">
+      <c r="C47" s="151"/>
+      <c r="D47" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="160"/>
-      <c r="F47" s="159" t="s">
+      <c r="E47" s="151"/>
+      <c r="F47" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="160"/>
-      <c r="H47" s="161" t="s">
+      <c r="G47" s="151"/>
+      <c r="H47" s="149" t="s">
         <v>38</v>
       </c>
-      <c r="I47" s="161"/>
+      <c r="I47" s="149"/>
       <c r="J47" s="136" t="s">
         <v>39</v>
       </c>
@@ -4029,37 +3919,37 @@
         <f>A34+1</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B48" s="139" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="140"/>
-      <c r="D48" s="145" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" s="146"/>
-      <c r="F48" s="145" t="s">
-        <v>79</v>
-      </c>
-      <c r="G48" s="146"/>
-      <c r="H48" s="151" t="s">
+      <c r="B48" s="143" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="144"/>
+      <c r="D48" s="155" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="156"/>
+      <c r="F48" s="155" t="s">
+        <v>88</v>
+      </c>
+      <c r="G48" s="156"/>
+      <c r="H48" s="152" t="s">
         <v>10</v>
       </c>
-      <c r="I48" s="152"/>
+      <c r="I48" s="153"/>
       <c r="J48" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="K48" s="153"/>
+        <v>89</v>
+      </c>
+      <c r="K48" s="167"/>
     </row>
     <row r="49" spans="1:11" ht="10.5" customHeight="1">
       <c r="A49" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="141"/>
-      <c r="C49" s="142"/>
-      <c r="D49" s="147"/>
-      <c r="E49" s="148"/>
-      <c r="F49" s="147"/>
-      <c r="G49" s="148"/>
+      <c r="B49" s="145"/>
+      <c r="C49" s="146"/>
+      <c r="D49" s="157"/>
+      <c r="E49" s="158"/>
+      <c r="F49" s="157"/>
+      <c r="G49" s="158"/>
       <c r="H49" s="136" t="s">
         <v>42</v>
       </c>
@@ -4069,58 +3959,182 @@
       <c r="J49" s="136" t="s">
         <v>44</v>
       </c>
-      <c r="K49" s="154"/>
+      <c r="K49" s="168"/>
     </row>
     <row r="50" spans="1:11" ht="10.5" customHeight="1">
       <c r="A50" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="141"/>
-      <c r="C50" s="142"/>
-      <c r="D50" s="147"/>
-      <c r="E50" s="148"/>
-      <c r="F50" s="147"/>
-      <c r="G50" s="148"/>
+      <c r="B50" s="145"/>
+      <c r="C50" s="146"/>
+      <c r="D50" s="157"/>
+      <c r="E50" s="158"/>
+      <c r="F50" s="157"/>
+      <c r="G50" s="158"/>
       <c r="H50" s="50" t="s">
         <v>60</v>
       </c>
       <c r="I50" s="50"/>
       <c r="J50" s="48"/>
-      <c r="K50" s="154"/>
+      <c r="K50" s="168"/>
     </row>
     <row r="51" spans="1:11" ht="10.5" customHeight="1">
       <c r="A51" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="B51" s="141"/>
-      <c r="C51" s="142"/>
-      <c r="D51" s="147"/>
-      <c r="E51" s="148"/>
-      <c r="F51" s="147"/>
-      <c r="G51" s="148"/>
+      <c r="B51" s="145"/>
+      <c r="C51" s="146"/>
+      <c r="D51" s="157"/>
+      <c r="E51" s="158"/>
+      <c r="F51" s="157"/>
+      <c r="G51" s="158"/>
       <c r="H51" s="136" t="s">
         <v>47</v>
       </c>
       <c r="I51" s="136"/>
       <c r="J51" s="136"/>
-      <c r="K51" s="154"/>
+      <c r="K51" s="168"/>
     </row>
     <row r="52" spans="1:11" ht="10.5" customHeight="1">
       <c r="A52" s="51">
         <v>922</v>
       </c>
-      <c r="B52" s="143"/>
-      <c r="C52" s="144"/>
-      <c r="D52" s="149"/>
-      <c r="E52" s="150"/>
-      <c r="F52" s="149"/>
-      <c r="G52" s="150"/>
+      <c r="B52" s="147"/>
+      <c r="C52" s="148"/>
+      <c r="D52" s="159"/>
+      <c r="E52" s="160"/>
+      <c r="F52" s="159"/>
+      <c r="G52" s="160"/>
       <c r="H52" s="50" t="s">
         <v>61</v>
       </c>
       <c r="I52" s="50"/>
       <c r="J52" s="48"/>
-      <c r="K52" s="155"/>
+      <c r="K52" s="169"/>
+    </row>
+    <row r="53" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A53" s="137" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="141" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="142"/>
+      <c r="D53" s="141" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="142"/>
+      <c r="F53" s="141" t="s">
+        <v>37</v>
+      </c>
+      <c r="G53" s="142"/>
+      <c r="H53" s="154" t="s">
+        <v>38</v>
+      </c>
+      <c r="I53" s="154"/>
+      <c r="J53" s="137" t="s">
+        <v>39</v>
+      </c>
+      <c r="K53" s="138" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A54" s="48">
+        <v>5</v>
+      </c>
+      <c r="B54" s="143" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="144"/>
+      <c r="D54" s="155" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" s="156"/>
+      <c r="F54" s="155" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54" s="156"/>
+      <c r="H54" s="161" t="s">
+        <v>9</v>
+      </c>
+      <c r="I54" s="162"/>
+      <c r="J54" s="52"/>
+      <c r="K54" s="167"/>
+    </row>
+    <row r="55" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A55" s="137" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="145"/>
+      <c r="C55" s="146"/>
+      <c r="D55" s="157"/>
+      <c r="E55" s="158"/>
+      <c r="F55" s="157"/>
+      <c r="G55" s="158"/>
+      <c r="H55" s="137" t="s">
+        <v>42</v>
+      </c>
+      <c r="I55" s="137" t="s">
+        <v>43</v>
+      </c>
+      <c r="J55" s="137" t="s">
+        <v>44</v>
+      </c>
+      <c r="K55" s="168"/>
+    </row>
+    <row r="56" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A56" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="145"/>
+      <c r="C56" s="146"/>
+      <c r="D56" s="157"/>
+      <c r="E56" s="158"/>
+      <c r="F56" s="157"/>
+      <c r="G56" s="158"/>
+      <c r="H56" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="I56" s="50"/>
+      <c r="J56" s="48"/>
+      <c r="K56" s="168"/>
+    </row>
+    <row r="57" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A57" s="137" t="s">
+        <v>46</v>
+      </c>
+      <c r="B57" s="145"/>
+      <c r="C57" s="146"/>
+      <c r="D57" s="157"/>
+      <c r="E57" s="158"/>
+      <c r="F57" s="157"/>
+      <c r="G57" s="158"/>
+      <c r="H57" s="137" t="s">
+        <v>47</v>
+      </c>
+      <c r="I57" s="137" t="s">
+        <v>48</v>
+      </c>
+      <c r="J57" s="137"/>
+      <c r="K57" s="168"/>
+    </row>
+    <row r="58" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A58" s="51">
+        <v>823</v>
+      </c>
+      <c r="B58" s="147"/>
+      <c r="C58" s="148"/>
+      <c r="D58" s="159"/>
+      <c r="E58" s="160"/>
+      <c r="F58" s="159"/>
+      <c r="G58" s="160"/>
+      <c r="H58" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="I58" s="50"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="169"/>
     </row>
     <row r="67" spans="1:11" s="58" customFormat="1">
       <c r="A67" s="62"/>
@@ -4333,21 +4347,50 @@
       <c r="K96" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B35:C39"/>
+  <mergeCells count="73">
+    <mergeCell ref="K54:K58"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B54:C58"/>
+    <mergeCell ref="D54:E58"/>
+    <mergeCell ref="F54:G58"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="B48:C52"/>
+    <mergeCell ref="D48:E52"/>
+    <mergeCell ref="F48:G52"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="K48:K52"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="D29:E33"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G33"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K41:K45"/>
+    <mergeCell ref="F35:G39"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="F41:G45"/>
     <mergeCell ref="B41:C45"/>
     <mergeCell ref="D35:E39"/>
     <mergeCell ref="D41:E45"/>
@@ -4364,60 +4407,50 @@
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="B21:C25"/>
     <mergeCell ref="D21:E25"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="K41:K45"/>
-    <mergeCell ref="F35:G39"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="F41:G45"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="D29:E33"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="B48:C52"/>
-    <mergeCell ref="D48:E52"/>
-    <mergeCell ref="F48:G52"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="K48:K52"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="B35:C39"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H21:I21"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H41:I41">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40:I40">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Not OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54:I54">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40:I40">
+  <conditionalFormatting sqref="H53:I53">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="86" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="71" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;LTest Case Table&amp;CBig Point: &amp;A</oddHeader>
     <oddFooter>&amp;LAI&amp;&amp;T-ART&amp;CLiveSpark Project&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="54" max="10" man="1"/>
+    <brk id="66" max="10" man="1"/>
   </rowBreaks>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
test chuc nang dang xuat va comment
</commit_message>
<xml_diff>
--- a/ProjectCode_Testcase_Template_v2.2.xlsx
+++ b/ProjectCode_Testcase_Template_v2.2.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$78</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -36,7 +36,7 @@
     <author>Nguyen Duc Tien</author>
   </authors>
   <commentList>
-    <comment ref="B27" authorId="0" shapeId="0">
+    <comment ref="B33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0" shapeId="0">
+    <comment ref="B52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H47" authorId="0" shapeId="0">
+    <comment ref="H53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J47" authorId="0" shapeId="0">
+    <comment ref="J53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A48" authorId="0" shapeId="0">
+    <comment ref="A54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H49" authorId="0" shapeId="0">
+    <comment ref="H55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I49" authorId="0" shapeId="0">
+    <comment ref="I55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J49" authorId="0" shapeId="0">
+    <comment ref="J55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A50" authorId="0" shapeId="0">
+    <comment ref="A56" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H51" authorId="0" shapeId="0">
+    <comment ref="H57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I51" authorId="0" shapeId="0">
+    <comment ref="I57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A52" authorId="0" shapeId="0">
+    <comment ref="A58" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="106">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -388,12 +388,6 @@
   </si>
   <si>
     <t>2.1.</t>
-  </si>
-  <si>
-    <t>1.2.2-2</t>
-  </si>
-  <si>
-    <t>1.1-2</t>
   </si>
   <si>
     <t xml:space="preserve">Chức năng xem
@@ -419,13 +413,6 @@
   </si>
   <si>
     <t>LongLN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chức năng thông tin
-</t>
-  </si>
-  <si>
-    <t>Click vào button thông tin để xem thông tin của trang web, sẽ hiển thị ra một thông báo về thông tin của trang web</t>
   </si>
   <si>
     <t>1.3</t>
@@ -469,9 +456,6 @@
     <t>Thêm được</t>
   </si>
   <si>
-    <t>Xem được thông tin</t>
-  </si>
-  <si>
     <t>Xem được bài viết</t>
   </si>
   <si>
@@ -515,6 +499,59 @@
   </si>
   <si>
     <t>Phê duyệt được bài đăng</t>
+  </si>
+  <si>
+    <t>Đăng xuất</t>
+  </si>
+  <si>
+    <t>Đăng xuất được</t>
+  </si>
+  <si>
+    <t>Bấm vào nút logout để đăng xuất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chức năng bình luận
+</t>
+  </si>
+  <si>
+    <t>Khi muốn bày tỏ quan điểm về một bài confession nào đó</t>
+  </si>
+  <si>
+    <t>Bình luận được</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chức năng like/dislike
+</t>
+  </si>
+  <si>
+    <t>Khi muốn thể hiện thích hoặc không thích một bài confession nào đó thì bấm vào nút like/dislike</t>
+  </si>
+  <si>
+    <t>like/dislike được</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>2.1.3</t>
+  </si>
+  <si>
+    <t>2.2.</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>2.2.3</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1062,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1146,9 +1183,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1350,14 +1384,59 @@
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1366,12 +1445,24 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1390,74 +1481,59 @@
     <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1906,7 +1982,7 @@
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
-      <c r="V2" s="69"/>
+      <c r="V2" s="68"/>
       <c r="W2" s="13"/>
       <c r="X2" s="14"/>
     </row>
@@ -1926,7 +2002,7 @@
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
-      <c r="N3" s="68"/>
+      <c r="N3" s="67"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
@@ -1934,7 +2010,7 @@
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
-      <c r="V3" s="70"/>
+      <c r="V3" s="69"/>
       <c r="W3" s="18"/>
       <c r="X3" s="19"/>
     </row>
@@ -1993,13 +2069,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="139" t="s">
+      <c r="O6" s="153" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="139"/>
-      <c r="Q6" s="139"/>
-      <c r="R6" s="139"/>
-      <c r="S6" s="139"/>
+      <c r="P6" s="153"/>
+      <c r="Q6" s="153"/>
+      <c r="R6" s="153"/>
+      <c r="S6" s="153"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -2009,11 +2085,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="139"/>
-      <c r="P7" s="139"/>
-      <c r="Q7" s="139"/>
-      <c r="R7" s="139"/>
-      <c r="S7" s="139"/>
+      <c r="O7" s="153"/>
+      <c r="P7" s="153"/>
+      <c r="Q7" s="153"/>
+      <c r="R7" s="153"/>
+      <c r="S7" s="153"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -2022,7 +2098,7 @@
       <c r="J8" s="29"/>
       <c r="K8" s="29"/>
       <c r="L8" s="31"/>
-      <c r="X8" s="67"/>
+      <c r="X8" s="66"/>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1">
       <c r="B9" s="30"/>
@@ -2035,7 +2111,7 @@
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="72"/>
+      <c r="H9" s="71"/>
       <c r="X9" s="19"/>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1">
@@ -2047,11 +2123,11 @@
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="72"/>
+      <c r="H10" s="71"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
-      <c r="L10" s="114" t="s">
+      <c r="L10" s="113" t="s">
         <v>5</v>
       </c>
       <c r="O10" s="21"/>
@@ -2068,13 +2144,13 @@
       <c r="D11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="140">
+      <c r="E11" s="154">
         <f ca="1">TODAY()</f>
         <v>43449</v>
       </c>
-      <c r="F11" s="140"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="72"/>
+      <c r="F11" s="154"/>
+      <c r="G11" s="154"/>
+      <c r="H11" s="71"/>
       <c r="L11" s="33" t="s">
         <v>7</v>
       </c>
@@ -2105,23 +2181,23 @@
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="63">
+      <c r="O12" s="62">
         <v>2</v>
       </c>
-      <c r="P12" s="63"/>
-      <c r="Q12" s="64">
+      <c r="P12" s="62"/>
+      <c r="Q12" s="63">
         <v>3</v>
       </c>
-      <c r="R12" s="64"/>
-      <c r="S12" s="65">
+      <c r="R12" s="63"/>
+      <c r="S12" s="64">
         <v>4</v>
       </c>
-      <c r="T12" s="65"/>
-      <c r="U12" s="66">
+      <c r="T12" s="64"/>
+      <c r="U12" s="65">
         <f t="shared" ref="U12:U18" si="0">SUM(O12:T12)</f>
         <v>9</v>
       </c>
-      <c r="V12" s="66"/>
+      <c r="V12" s="65"/>
       <c r="X12" s="19"/>
     </row>
     <row r="13" spans="1:24">
@@ -2131,23 +2207,23 @@
       </c>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
-      <c r="O13" s="63">
+      <c r="O13" s="62">
         <v>22</v>
       </c>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="64">
+      <c r="P13" s="62"/>
+      <c r="Q13" s="63">
         <v>22</v>
       </c>
-      <c r="R13" s="64"/>
-      <c r="S13" s="65">
+      <c r="R13" s="63"/>
+      <c r="S13" s="64">
         <v>22</v>
       </c>
-      <c r="T13" s="65"/>
-      <c r="U13" s="66">
+      <c r="T13" s="64"/>
+      <c r="U13" s="65">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="V13" s="66"/>
+      <c r="V13" s="65"/>
       <c r="X13" s="19"/>
     </row>
     <row r="14" spans="1:24">
@@ -2157,23 +2233,23 @@
       </c>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="63">
+      <c r="O14" s="62">
         <v>32</v>
       </c>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="64">
+      <c r="P14" s="62"/>
+      <c r="Q14" s="63">
         <v>32</v>
       </c>
-      <c r="R14" s="64"/>
-      <c r="S14" s="65">
+      <c r="R14" s="63"/>
+      <c r="S14" s="64">
         <v>32</v>
       </c>
-      <c r="T14" s="65"/>
-      <c r="U14" s="66">
+      <c r="T14" s="64"/>
+      <c r="U14" s="65">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="V14" s="66"/>
+      <c r="V14" s="65"/>
       <c r="X14" s="19"/>
     </row>
     <row r="15" spans="1:24">
@@ -2181,32 +2257,32 @@
       <c r="D15" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
       <c r="L15" s="34">
         <v>4</v>
       </c>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
-      <c r="O15" s="63">
+      <c r="O15" s="62">
         <v>42</v>
       </c>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="64">
+      <c r="P15" s="62"/>
+      <c r="Q15" s="63">
         <v>42</v>
       </c>
-      <c r="R15" s="64"/>
-      <c r="S15" s="65">
+      <c r="R15" s="63"/>
+      <c r="S15" s="64">
         <v>42</v>
       </c>
-      <c r="T15" s="65"/>
-      <c r="U15" s="66">
+      <c r="T15" s="64"/>
+      <c r="U15" s="65">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="V15" s="66"/>
+      <c r="V15" s="65"/>
       <c r="X15" s="19"/>
     </row>
     <row r="16" spans="1:24">
@@ -2221,23 +2297,23 @@
       </c>
       <c r="M16" s="35"/>
       <c r="N16" s="35"/>
-      <c r="O16" s="63">
+      <c r="O16" s="62">
         <v>52</v>
       </c>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="64">
+      <c r="P16" s="62"/>
+      <c r="Q16" s="63">
         <v>52</v>
       </c>
-      <c r="R16" s="64"/>
-      <c r="S16" s="65">
+      <c r="R16" s="63"/>
+      <c r="S16" s="64">
         <v>52</v>
       </c>
-      <c r="T16" s="65"/>
-      <c r="U16" s="66">
+      <c r="T16" s="64"/>
+      <c r="U16" s="65">
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
-      <c r="V16" s="66"/>
+      <c r="V16" s="65"/>
       <c r="X16" s="19"/>
     </row>
     <row r="17" spans="2:35">
@@ -2252,23 +2328,23 @@
       </c>
       <c r="M17" s="34"/>
       <c r="N17" s="34"/>
-      <c r="O17" s="63">
+      <c r="O17" s="62">
         <v>62</v>
       </c>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="64">
+      <c r="P17" s="62"/>
+      <c r="Q17" s="63">
         <v>62</v>
       </c>
-      <c r="R17" s="64"/>
-      <c r="S17" s="65">
+      <c r="R17" s="63"/>
+      <c r="S17" s="64">
         <v>62</v>
       </c>
-      <c r="T17" s="65"/>
-      <c r="U17" s="66">
+      <c r="T17" s="64"/>
+      <c r="U17" s="65">
         <f t="shared" si="0"/>
         <v>186</v>
       </c>
-      <c r="V17" s="66"/>
+      <c r="V17" s="65"/>
       <c r="X17" s="19"/>
     </row>
     <row r="18" spans="2:35">
@@ -2283,23 +2359,23 @@
       </c>
       <c r="M18" s="35"/>
       <c r="N18" s="35"/>
-      <c r="O18" s="63">
+      <c r="O18" s="62">
         <v>72</v>
       </c>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="64">
+      <c r="P18" s="62"/>
+      <c r="Q18" s="63">
         <v>72</v>
       </c>
-      <c r="R18" s="64"/>
-      <c r="S18" s="65">
+      <c r="R18" s="63"/>
+      <c r="S18" s="64">
         <v>72</v>
       </c>
-      <c r="T18" s="65"/>
-      <c r="U18" s="66">
+      <c r="T18" s="64"/>
+      <c r="U18" s="65">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="V18" s="66"/>
+      <c r="V18" s="65"/>
       <c r="X18" s="19"/>
     </row>
     <row r="19" spans="2:35">
@@ -2314,27 +2390,27 @@
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
-      <c r="O19" s="112">
+      <c r="O19" s="111">
         <f>SUM(O12:O18)</f>
         <v>284</v>
       </c>
-      <c r="P19" s="112"/>
-      <c r="Q19" s="112">
+      <c r="P19" s="111"/>
+      <c r="Q19" s="111">
         <f>SUM(Q12:Q18)</f>
         <v>285</v>
       </c>
-      <c r="R19" s="112"/>
-      <c r="S19" s="112">
+      <c r="R19" s="111"/>
+      <c r="S19" s="111">
         <f>SUM(S12:S18)</f>
         <v>286</v>
       </c>
-      <c r="T19" s="112"/>
-      <c r="U19" s="113">
+      <c r="T19" s="111"/>
+      <c r="U19" s="112">
         <f>SUM(U12:U18)</f>
         <v>855</v>
       </c>
-      <c r="V19" s="113"/>
-      <c r="W19" s="74"/>
+      <c r="V19" s="112"/>
+      <c r="W19" s="73"/>
       <c r="X19" s="19"/>
     </row>
     <row r="20" spans="2:35">
@@ -2364,10 +2440,10 @@
       <c r="D22" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
       <c r="W22" s="17"/>
       <c r="X22" s="23"/>
     </row>
@@ -2378,7 +2454,7 @@
       <c r="F23" s="44"/>
       <c r="G23" s="44"/>
       <c r="H23" s="44"/>
-      <c r="W23" s="75"/>
+      <c r="W23" s="74"/>
       <c r="X23" s="23"/>
     </row>
     <row r="24" spans="2:35" s="17" customFormat="1">
@@ -2388,20 +2464,20 @@
       <c r="F24" s="44"/>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
-      <c r="L24" s="114" t="s">
+      <c r="L24" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="M24" s="104"/>
-      <c r="N24" s="104"/>
-      <c r="O24" s="104"/>
-      <c r="P24" s="105"/>
-      <c r="Q24" s="105"/>
-      <c r="R24" s="105"/>
-      <c r="S24" s="105"/>
-      <c r="T24" s="105"/>
-      <c r="U24" s="105"/>
-      <c r="V24" s="105"/>
-      <c r="W24" s="73"/>
+      <c r="M24" s="103"/>
+      <c r="N24" s="103"/>
+      <c r="O24" s="103"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
+      <c r="T24" s="104"/>
+      <c r="U24" s="104"/>
+      <c r="V24" s="104"/>
+      <c r="W24" s="72"/>
       <c r="X24" s="23"/>
     </row>
     <row r="25" spans="2:35" s="17" customFormat="1">
@@ -2410,18 +2486,18 @@
       <c r="F25" s="44"/>
       <c r="G25" s="44"/>
       <c r="H25" s="44"/>
-      <c r="L25" s="106"/>
-      <c r="M25" s="107"/>
-      <c r="N25" s="107"/>
-      <c r="O25" s="107"/>
-      <c r="P25" s="108"/>
-      <c r="Q25" s="108"/>
-      <c r="R25" s="108"/>
-      <c r="S25" s="108"/>
-      <c r="T25" s="108"/>
-      <c r="U25" s="108"/>
-      <c r="V25" s="108"/>
-      <c r="W25" s="73"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="106"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="107"/>
+      <c r="R25" s="107"/>
+      <c r="S25" s="107"/>
+      <c r="T25" s="107"/>
+      <c r="U25" s="107"/>
+      <c r="V25" s="107"/>
+      <c r="W25" s="72"/>
       <c r="X25" s="23"/>
     </row>
     <row r="26" spans="2:35" s="17" customFormat="1">
@@ -2430,58 +2506,58 @@
       <c r="F26" s="44"/>
       <c r="G26" s="44"/>
       <c r="H26" s="44"/>
-      <c r="L26" s="106"/>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="108"/>
-      <c r="Q26" s="108"/>
-      <c r="R26" s="108"/>
-      <c r="S26" s="108"/>
-      <c r="T26" s="108"/>
-      <c r="U26" s="108"/>
-      <c r="V26" s="108"/>
-      <c r="W26" s="73"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="106"/>
+      <c r="N26" s="106"/>
+      <c r="O26" s="106"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="107"/>
+      <c r="S26" s="107"/>
+      <c r="T26" s="107"/>
+      <c r="U26" s="107"/>
+      <c r="V26" s="107"/>
+      <c r="W26" s="72"/>
       <c r="X26" s="23"/>
-      <c r="AB26" s="76"/>
+      <c r="AB26" s="75"/>
     </row>
     <row r="27" spans="2:35" s="17" customFormat="1">
       <c r="B27" s="22"/>
       <c r="D27" s="38"/>
       <c r="E27" s="4"/>
-      <c r="L27" s="106"/>
-      <c r="M27" s="107"/>
-      <c r="N27" s="107"/>
-      <c r="O27" s="107"/>
-      <c r="P27" s="108"/>
-      <c r="Q27" s="108"/>
-      <c r="R27" s="108"/>
-      <c r="S27" s="108"/>
-      <c r="T27" s="108"/>
-      <c r="U27" s="108"/>
-      <c r="V27" s="108"/>
-      <c r="W27" s="73"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="106"/>
+      <c r="N27" s="106"/>
+      <c r="O27" s="106"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="107"/>
+      <c r="S27" s="107"/>
+      <c r="T27" s="107"/>
+      <c r="U27" s="107"/>
+      <c r="V27" s="107"/>
+      <c r="W27" s="72"/>
       <c r="X27" s="23"/>
-      <c r="AB27" s="76"/>
+      <c r="AB27" s="75"/>
     </row>
     <row r="28" spans="2:35" s="17" customFormat="1">
       <c r="B28" s="22"/>
       <c r="D28" s="38"/>
       <c r="E28" s="4"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="107"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="108"/>
-      <c r="Q28" s="108"/>
-      <c r="R28" s="108"/>
-      <c r="S28" s="108"/>
-      <c r="T28" s="108"/>
-      <c r="U28" s="108"/>
-      <c r="V28" s="108"/>
-      <c r="W28" s="73"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="106"/>
+      <c r="N28" s="106"/>
+      <c r="O28" s="106"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="107"/>
+      <c r="T28" s="107"/>
+      <c r="U28" s="107"/>
+      <c r="V28" s="107"/>
+      <c r="W28" s="72"/>
       <c r="X28" s="23"/>
-      <c r="AB28" s="76"/>
+      <c r="AB28" s="75"/>
     </row>
     <row r="29" spans="2:35" s="17" customFormat="1">
       <c r="B29" s="22"/>
@@ -2491,34 +2567,34 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="K29" s="31"/>
-      <c r="L29" s="106"/>
-      <c r="M29" s="107"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="108"/>
-      <c r="Q29" s="108"/>
-      <c r="R29" s="108"/>
-      <c r="S29" s="108"/>
-      <c r="T29" s="108"/>
-      <c r="U29" s="108"/>
-      <c r="V29" s="108"/>
-      <c r="W29" s="73"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="106"/>
+      <c r="N29" s="106"/>
+      <c r="O29" s="106"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="107"/>
+      <c r="S29" s="107"/>
+      <c r="T29" s="107"/>
+      <c r="U29" s="107"/>
+      <c r="V29" s="107"/>
+      <c r="W29" s="72"/>
       <c r="X29" s="23"/>
     </row>
     <row r="30" spans="2:35" s="17" customFormat="1">
       <c r="B30" s="22"/>
-      <c r="L30" s="106"/>
-      <c r="M30" s="107"/>
-      <c r="N30" s="107"/>
-      <c r="O30" s="107"/>
-      <c r="P30" s="108"/>
-      <c r="Q30" s="108"/>
-      <c r="R30" s="108"/>
-      <c r="S30" s="108"/>
-      <c r="T30" s="108"/>
-      <c r="U30" s="108"/>
-      <c r="V30" s="108"/>
-      <c r="W30" s="73"/>
+      <c r="L30" s="105"/>
+      <c r="M30" s="106"/>
+      <c r="N30" s="106"/>
+      <c r="O30" s="106"/>
+      <c r="P30" s="107"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="107"/>
+      <c r="S30" s="107"/>
+      <c r="T30" s="107"/>
+      <c r="U30" s="107"/>
+      <c r="V30" s="107"/>
+      <c r="W30" s="72"/>
       <c r="X30" s="23"/>
     </row>
     <row r="31" spans="2:35">
@@ -2534,18 +2610,18 @@
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
       <c r="K31" s="18"/>
-      <c r="L31" s="109"/>
-      <c r="M31" s="107"/>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
-      <c r="P31" s="108"/>
-      <c r="Q31" s="108"/>
-      <c r="R31" s="108"/>
-      <c r="S31" s="108"/>
-      <c r="T31" s="108"/>
-      <c r="U31" s="108"/>
-      <c r="V31" s="108"/>
-      <c r="W31" s="73"/>
+      <c r="L31" s="108"/>
+      <c r="M31" s="106"/>
+      <c r="N31" s="106"/>
+      <c r="O31" s="106"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="107"/>
+      <c r="S31" s="107"/>
+      <c r="T31" s="107"/>
+      <c r="U31" s="107"/>
+      <c r="V31" s="107"/>
+      <c r="W31" s="72"/>
       <c r="X31" s="23"/>
       <c r="AA31" s="17"/>
       <c r="AB31" s="17"/>
@@ -2570,18 +2646,18 @@
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
-      <c r="L32" s="106"/>
-      <c r="M32" s="107"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="107"/>
-      <c r="P32" s="108"/>
-      <c r="Q32" s="108"/>
-      <c r="R32" s="108"/>
-      <c r="S32" s="108"/>
-      <c r="T32" s="108"/>
-      <c r="U32" s="108"/>
-      <c r="V32" s="108"/>
-      <c r="W32" s="73"/>
+      <c r="L32" s="105"/>
+      <c r="M32" s="106"/>
+      <c r="N32" s="106"/>
+      <c r="O32" s="106"/>
+      <c r="P32" s="107"/>
+      <c r="Q32" s="107"/>
+      <c r="R32" s="107"/>
+      <c r="S32" s="107"/>
+      <c r="T32" s="107"/>
+      <c r="U32" s="107"/>
+      <c r="V32" s="107"/>
+      <c r="W32" s="72"/>
       <c r="X32" s="23"/>
       <c r="AA32" s="17"/>
       <c r="AB32" s="17"/>
@@ -2604,18 +2680,18 @@
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="106"/>
-      <c r="M33" s="110"/>
-      <c r="N33" s="107"/>
-      <c r="O33" s="107"/>
-      <c r="P33" s="108"/>
-      <c r="Q33" s="108"/>
-      <c r="R33" s="108"/>
-      <c r="S33" s="108"/>
-      <c r="T33" s="108"/>
-      <c r="U33" s="108"/>
-      <c r="V33" s="111"/>
-      <c r="W33" s="74"/>
+      <c r="L33" s="105"/>
+      <c r="M33" s="109"/>
+      <c r="N33" s="106"/>
+      <c r="O33" s="106"/>
+      <c r="P33" s="107"/>
+      <c r="Q33" s="107"/>
+      <c r="R33" s="107"/>
+      <c r="S33" s="107"/>
+      <c r="T33" s="107"/>
+      <c r="U33" s="107"/>
+      <c r="V33" s="110"/>
+      <c r="W33" s="73"/>
       <c r="X33" s="23"/>
       <c r="AA33" s="17"/>
       <c r="AB33" s="17"/>
@@ -2654,7 +2730,7 @@
       <c r="W34" s="45"/>
       <c r="X34" s="23"/>
       <c r="AA34" s="17"/>
-      <c r="AB34" s="76"/>
+      <c r="AB34" s="75"/>
       <c r="AC34" s="17"/>
       <c r="AD34" s="17"/>
       <c r="AE34" s="17"/>
@@ -2931,10 +3007,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54:I54"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2947,109 +3023,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="58" customFormat="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="80" t="s">
+      <c r="B1" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="101">
-        <f>COUNTIF(H1:H786,"OK")</f>
+      <c r="I1" s="100">
+        <v>6</v>
+      </c>
+      <c r="J1" s="81" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="82"/>
+    </row>
+    <row r="2" spans="1:11" s="58" customFormat="1">
+      <c r="A2" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="87" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="101">
         <v>4</v>
       </c>
-      <c r="J1" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="83"/>
-    </row>
-    <row r="2" spans="1:11" s="58" customFormat="1">
-      <c r="A2" s="116" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="85" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="88" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="102">
-        <f>COUNTIF(H2:H787,"Not OK")</f>
-        <v>4</v>
-      </c>
-      <c r="J2" s="89" t="s">
+      <c r="J2" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="90"/>
+      <c r="K2" s="89"/>
     </row>
     <row r="3" spans="1:11" s="58" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="88" t="s">
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="103">
+      <c r="I3" s="102">
         <f>COUNTIF(H2:H787,"Untested")</f>
         <v>0</v>
       </c>
-      <c r="J3" s="89" t="s">
+      <c r="J3" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="90"/>
+      <c r="K3" s="89"/>
     </row>
     <row r="4" spans="1:11" s="58" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A4" s="91"/>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="92" t="s">
+      <c r="A4" s="90"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="85"/>
-      <c r="I4" s="102">
+      <c r="H4" s="84"/>
+      <c r="I4" s="101">
         <f>COUNTIF(H3:H788,"Result")</f>
-        <v>8</v>
-      </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="90"/>
+        <v>10</v>
+      </c>
+      <c r="J4" s="88"/>
+      <c r="K4" s="89"/>
     </row>
     <row r="5" spans="1:11" s="58" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A5" s="93"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="98"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="97"/>
     </row>
     <row r="6" spans="1:11" s="58" customFormat="1" ht="11.25" customHeight="1">
       <c r="A6" s="59"/>
@@ -3065,43 +3139,43 @@
       <c r="K6" s="57"/>
     </row>
     <row r="7" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="170" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="170"/>
-      <c r="D7" s="170"/>
-      <c r="E7" s="170"/>
-      <c r="F7" s="170"/>
-      <c r="G7" s="170"/>
-      <c r="H7" s="170"/>
-      <c r="I7" s="170"/>
-      <c r="J7" s="170"/>
-      <c r="K7" s="170"/>
+      <c r="B7" s="183" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="183"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="183"/>
+      <c r="G7" s="183"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
+      <c r="J7" s="183"/>
+      <c r="K7" s="183"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="158" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="142"/>
-      <c r="D8" s="141" t="s">
+      <c r="C8" s="159"/>
+      <c r="D8" s="158" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="142"/>
-      <c r="F8" s="141" t="s">
+      <c r="E8" s="159"/>
+      <c r="F8" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="142"/>
-      <c r="H8" s="166" t="s">
+      <c r="G8" s="159"/>
+      <c r="H8" s="184" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="166"/>
-      <c r="J8" s="118" t="s">
+      <c r="I8" s="184"/>
+      <c r="J8" s="117" t="s">
         <v>39</v>
       </c>
       <c r="K8" s="47" t="s">
@@ -3112,120 +3186,120 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="143" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="144"/>
-      <c r="D9" s="155" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="156"/>
-      <c r="F9" s="120" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="121"/>
-      <c r="H9" s="152" t="s">
+      <c r="B9" s="161" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="162"/>
+      <c r="D9" s="167" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="168"/>
+      <c r="F9" s="119" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="120"/>
+      <c r="H9" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="153"/>
+      <c r="I9" s="176"/>
       <c r="J9" s="48"/>
-      <c r="K9" s="167"/>
+      <c r="K9" s="155"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="145"/>
-      <c r="C10" s="146"/>
-      <c r="D10" s="157"/>
-      <c r="E10" s="158"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="117" t="s">
+      <c r="B10" s="163"/>
+      <c r="C10" s="164"/>
+      <c r="D10" s="169"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="116" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="117" t="s">
+      <c r="I10" s="116" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="117" t="s">
+      <c r="J10" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="168"/>
+      <c r="K10" s="156"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="145"/>
-      <c r="C11" s="146"/>
-      <c r="D11" s="157"/>
-      <c r="E11" s="158"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="123"/>
+        <v>65</v>
+      </c>
+      <c r="B11" s="163"/>
+      <c r="C11" s="164"/>
+      <c r="D11" s="169"/>
+      <c r="E11" s="170"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="122"/>
       <c r="H11" s="50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
-      <c r="K11" s="168"/>
+      <c r="K11" s="156"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A12" s="117" t="s">
+      <c r="A12" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="145"/>
-      <c r="C12" s="146"/>
-      <c r="D12" s="157"/>
-      <c r="E12" s="158"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="117" t="s">
+      <c r="B12" s="163"/>
+      <c r="C12" s="164"/>
+      <c r="D12" s="169"/>
+      <c r="E12" s="170"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="117" t="s">
+      <c r="I12" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="117"/>
-      <c r="K12" s="168"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="156"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="51">
         <v>981</v>
       </c>
-      <c r="B13" s="147"/>
-      <c r="C13" s="148"/>
-      <c r="D13" s="159"/>
-      <c r="E13" s="160"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="125"/>
+      <c r="B13" s="165"/>
+      <c r="C13" s="166"/>
+      <c r="D13" s="171"/>
+      <c r="E13" s="172"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="124"/>
       <c r="H13" s="53" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="54"/>
-      <c r="K13" s="169"/>
+      <c r="K13" s="157"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="180" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="151"/>
-      <c r="D14" s="150" t="s">
+      <c r="C14" s="181"/>
+      <c r="D14" s="180" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="151"/>
-      <c r="F14" s="150" t="s">
+      <c r="E14" s="181"/>
+      <c r="F14" s="180" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="151"/>
-      <c r="H14" s="149" t="s">
+      <c r="G14" s="181"/>
+      <c r="H14" s="182" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="149"/>
-      <c r="J14" s="126" t="s">
+      <c r="I14" s="182"/>
+      <c r="J14" s="125" t="s">
         <v>39</v>
       </c>
       <c r="K14" s="56" t="s">
@@ -3236,124 +3310,124 @@
       <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="143" t="s">
+      <c r="B15" s="161" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="162"/>
+      <c r="D15" s="167" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="168"/>
+      <c r="F15" s="119" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="120"/>
+      <c r="H15" s="173" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="174"/>
+      <c r="J15" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="144"/>
-      <c r="D15" s="155" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="156"/>
-      <c r="F15" s="120" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="121"/>
-      <c r="H15" s="161" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="162"/>
-      <c r="J15" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="167"/>
+      <c r="K15" s="155"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A16" s="126" t="s">
+      <c r="A16" s="125" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="145"/>
-      <c r="C16" s="146"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="126" t="s">
+      <c r="B16" s="163"/>
+      <c r="C16" s="164"/>
+      <c r="D16" s="169"/>
+      <c r="E16" s="170"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="122"/>
+      <c r="H16" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="126" t="s">
+      <c r="I16" s="125" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="126" t="s">
+      <c r="J16" s="125" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="168"/>
+      <c r="K16" s="156"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="145"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="157"/>
-      <c r="E17" s="158"/>
-      <c r="F17" s="122"/>
-      <c r="G17" s="123"/>
+        <v>66</v>
+      </c>
+      <c r="B17" s="163"/>
+      <c r="C17" s="164"/>
+      <c r="D17" s="169"/>
+      <c r="E17" s="170"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="122"/>
       <c r="H17" s="50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I17" s="50"/>
       <c r="J17" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="168"/>
+        <v>63</v>
+      </c>
+      <c r="K17" s="156"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A18" s="126" t="s">
+      <c r="A18" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="145"/>
-      <c r="C18" s="146"/>
-      <c r="D18" s="157"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="122"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="126" t="s">
+      <c r="B18" s="163"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="169"/>
+      <c r="E18" s="170"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="122"/>
+      <c r="H18" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="126" t="s">
+      <c r="I18" s="125" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="126"/>
-      <c r="K18" s="168"/>
+      <c r="J18" s="125"/>
+      <c r="K18" s="156"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="51">
         <v>921</v>
       </c>
-      <c r="B19" s="147"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="159"/>
-      <c r="E19" s="160"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="125"/>
+      <c r="B19" s="165"/>
+      <c r="C19" s="166"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="172"/>
+      <c r="F19" s="123"/>
+      <c r="G19" s="124"/>
       <c r="H19" s="50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="168"/>
+      <c r="K19" s="156"/>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A20" s="127" t="s">
+      <c r="A20" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="141" t="s">
+      <c r="B20" s="158" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="142"/>
-      <c r="D20" s="141" t="s">
+      <c r="C20" s="159"/>
+      <c r="D20" s="158" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="142"/>
-      <c r="F20" s="141" t="s">
+      <c r="E20" s="159"/>
+      <c r="F20" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="142"/>
-      <c r="H20" s="166" t="s">
+      <c r="G20" s="159"/>
+      <c r="H20" s="184" t="s">
         <v>38</v>
       </c>
-      <c r="I20" s="166"/>
-      <c r="J20" s="128" t="s">
+      <c r="I20" s="184"/>
+      <c r="J20" s="127" t="s">
         <v>39</v>
       </c>
       <c r="K20" s="47" t="s">
@@ -3364,991 +3438,1092 @@
       <c r="A21" s="48">
         <v>3</v>
       </c>
-      <c r="B21" s="143" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="144"/>
-      <c r="D21" s="155" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="156"/>
-      <c r="F21" s="129" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="130"/>
-      <c r="H21" s="152" t="s">
+      <c r="B21" s="161" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="162"/>
+      <c r="D21" s="167" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="168"/>
+      <c r="F21" s="128" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="129"/>
+      <c r="H21" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="153"/>
+      <c r="I21" s="176"/>
       <c r="J21" s="48"/>
-      <c r="K21" s="167"/>
+      <c r="K21" s="155"/>
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A22" s="127" t="s">
+      <c r="A22" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="145"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="157"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="131"/>
-      <c r="G22" s="132"/>
-      <c r="H22" s="127" t="s">
+      <c r="B22" s="163"/>
+      <c r="C22" s="164"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="170"/>
+      <c r="F22" s="130"/>
+      <c r="G22" s="131"/>
+      <c r="H22" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="127" t="s">
+      <c r="I22" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="127" t="s">
+      <c r="J22" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="168"/>
+      <c r="K22" s="156"/>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
       <c r="A23" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="145"/>
-      <c r="C23" s="146"/>
-      <c r="D23" s="157"/>
-      <c r="E23" s="158"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="132"/>
+        <v>64</v>
+      </c>
+      <c r="B23" s="163"/>
+      <c r="C23" s="164"/>
+      <c r="D23" s="169"/>
+      <c r="E23" s="170"/>
+      <c r="F23" s="130"/>
+      <c r="G23" s="131"/>
       <c r="H23" s="50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="48"/>
-      <c r="K23" s="168"/>
+      <c r="K23" s="156"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A24" s="127" t="s">
+      <c r="A24" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="145"/>
-      <c r="C24" s="146"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="158"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="132"/>
-      <c r="H24" s="127" t="s">
+      <c r="B24" s="163"/>
+      <c r="C24" s="164"/>
+      <c r="D24" s="169"/>
+      <c r="E24" s="170"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="131"/>
+      <c r="H24" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="I24" s="127" t="s">
+      <c r="I24" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="J24" s="127"/>
-      <c r="K24" s="168"/>
+      <c r="J24" s="126"/>
+      <c r="K24" s="156"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="51">
         <v>982</v>
       </c>
-      <c r="B25" s="147"/>
-      <c r="C25" s="148"/>
-      <c r="D25" s="159"/>
-      <c r="E25" s="160"/>
-      <c r="F25" s="133"/>
-      <c r="G25" s="134"/>
+      <c r="B25" s="165"/>
+      <c r="C25" s="166"/>
+      <c r="D25" s="171"/>
+      <c r="E25" s="172"/>
+      <c r="F25" s="132"/>
+      <c r="G25" s="133"/>
       <c r="H25" s="50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I25" s="50"/>
       <c r="J25" s="48"/>
-      <c r="K25" s="169"/>
-    </row>
-    <row r="26" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A26" s="99" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="171" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="171"/>
-      <c r="D26" s="170"/>
-      <c r="E26" s="170"/>
-      <c r="F26" s="170"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="170"/>
-      <c r="K26" s="170"/>
+      <c r="K25" s="157"/>
+    </row>
+    <row r="26" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A26" s="140" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="158" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="159"/>
+      <c r="D26" s="158" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="159"/>
+      <c r="F26" s="158" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="159"/>
+      <c r="H26" s="184" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="184"/>
+      <c r="J26" s="150" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="47" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A27" s="100" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="163" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="164"/>
-      <c r="D27" s="164"/>
-      <c r="E27" s="164"/>
-      <c r="F27" s="164"/>
-      <c r="G27" s="164"/>
-      <c r="H27" s="164"/>
-      <c r="I27" s="164"/>
-      <c r="J27" s="164"/>
-      <c r="K27" s="165"/>
-    </row>
-    <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A28" s="135" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="150" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="151"/>
-      <c r="D28" s="150" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="151"/>
-      <c r="F28" s="150" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="151"/>
-      <c r="H28" s="149" t="s">
-        <v>38</v>
-      </c>
-      <c r="I28" s="149"/>
-      <c r="J28" s="135" t="s">
-        <v>39</v>
-      </c>
-      <c r="K28" s="135" t="s">
-        <v>40</v>
-      </c>
+      <c r="A27" s="48">
+        <v>4</v>
+      </c>
+      <c r="B27" s="161" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="162"/>
+      <c r="D27" s="167" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="168"/>
+      <c r="F27" s="141" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" s="142"/>
+      <c r="H27" s="175" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="176"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="155"/>
+    </row>
+    <row r="28" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A28" s="140" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="163"/>
+      <c r="C28" s="164"/>
+      <c r="D28" s="169"/>
+      <c r="E28" s="170"/>
+      <c r="F28" s="143"/>
+      <c r="G28" s="144"/>
+      <c r="H28" s="140" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28" s="140" t="s">
+        <v>43</v>
+      </c>
+      <c r="J28" s="140" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28" s="156"/>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A29" s="48">
-        <f>A15+1</f>
-        <v>3</v>
-      </c>
-      <c r="B29" s="143" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="144"/>
-      <c r="D29" s="155" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="156"/>
-      <c r="F29" s="155" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="156"/>
-      <c r="H29" s="152" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="153"/>
-      <c r="J29" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="K29" s="167"/>
+      <c r="A29" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="163"/>
+      <c r="C29" s="164"/>
+      <c r="D29" s="169"/>
+      <c r="E29" s="170"/>
+      <c r="F29" s="143"/>
+      <c r="G29" s="144"/>
+      <c r="H29" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I29" s="50"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="156"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A30" s="126" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="145"/>
-      <c r="C30" s="146"/>
-      <c r="D30" s="157"/>
-      <c r="E30" s="158"/>
-      <c r="F30" s="157"/>
-      <c r="G30" s="158"/>
-      <c r="H30" s="126" t="s">
-        <v>42</v>
-      </c>
-      <c r="I30" s="126" t="s">
-        <v>43</v>
-      </c>
-      <c r="J30" s="126" t="s">
-        <v>44</v>
-      </c>
-      <c r="K30" s="168"/>
+      <c r="A30" s="140" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="163"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="169"/>
+      <c r="E30" s="170"/>
+      <c r="F30" s="143"/>
+      <c r="G30" s="144"/>
+      <c r="H30" s="140" t="s">
+        <v>47</v>
+      </c>
+      <c r="I30" s="140" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="140"/>
+      <c r="K30" s="156"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A31" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="145"/>
-      <c r="C31" s="146"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="158"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="158"/>
+      <c r="A31" s="51">
+        <v>983</v>
+      </c>
+      <c r="B31" s="165"/>
+      <c r="C31" s="166"/>
+      <c r="D31" s="171"/>
+      <c r="E31" s="172"/>
+      <c r="F31" s="145"/>
+      <c r="G31" s="146"/>
       <c r="H31" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I31" s="50"/>
       <c r="J31" s="48"/>
-      <c r="K31" s="168"/>
+      <c r="K31" s="157"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A32" s="126" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="145"/>
-      <c r="C32" s="146"/>
-      <c r="D32" s="157"/>
-      <c r="E32" s="158"/>
-      <c r="F32" s="157"/>
-      <c r="G32" s="158"/>
-      <c r="H32" s="126" t="s">
-        <v>47</v>
-      </c>
-      <c r="I32" s="126"/>
-      <c r="J32" s="126"/>
-      <c r="K32" s="168"/>
+      <c r="A32" s="98" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="152" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="152"/>
+      <c r="D32" s="151"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="151"/>
+      <c r="G32" s="151"/>
+      <c r="H32" s="151"/>
+      <c r="I32" s="151"/>
+      <c r="J32" s="151"/>
+      <c r="K32" s="151"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A33" s="51">
-        <v>922</v>
-      </c>
-      <c r="B33" s="147"/>
+      <c r="A33" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="147" t="s">
+        <v>70</v>
+      </c>
       <c r="C33" s="148"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="160"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="160"/>
-      <c r="H33" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="I33" s="50"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="169"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
+      <c r="G33" s="148"/>
+      <c r="H33" s="148"/>
+      <c r="I33" s="148"/>
+      <c r="J33" s="148"/>
+      <c r="K33" s="149"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A34" s="117" t="s">
+      <c r="A34" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="141" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="142"/>
-      <c r="D34" s="141" t="s">
+      <c r="B34" s="138" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="139"/>
+      <c r="D34" s="138" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="142"/>
-      <c r="F34" s="141" t="s">
+      <c r="E34" s="139"/>
+      <c r="F34" s="138" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="142"/>
-      <c r="H34" s="154" t="s">
+      <c r="G34" s="139"/>
+      <c r="H34" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="I34" s="154"/>
-      <c r="J34" s="117" t="s">
+      <c r="I34" s="137"/>
+      <c r="J34" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="119" t="s">
+      <c r="K34" s="137" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="48">
-        <v>4</v>
-      </c>
-      <c r="B35" s="143" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="144"/>
-      <c r="D35" s="155" t="s">
-        <v>76</v>
-      </c>
-      <c r="E35" s="156"/>
-      <c r="F35" s="155" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="161" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="156"/>
-      <c r="H35" s="161" t="s">
-        <v>9</v>
-      </c>
-      <c r="I35" s="162"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="167"/>
+      <c r="C35" s="162"/>
+      <c r="D35" s="167" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="168"/>
+      <c r="F35" s="167" t="s">
+        <v>74</v>
+      </c>
+      <c r="G35" s="168"/>
+      <c r="H35" s="175" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="176"/>
+      <c r="J35" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="K35" s="155"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A36" s="117" t="s">
+      <c r="A36" s="125" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="145"/>
-      <c r="C36" s="146"/>
-      <c r="D36" s="157"/>
-      <c r="E36" s="158"/>
-      <c r="F36" s="157"/>
-      <c r="G36" s="158"/>
-      <c r="H36" s="117" t="s">
+      <c r="B36" s="163"/>
+      <c r="C36" s="164"/>
+      <c r="D36" s="169"/>
+      <c r="E36" s="170"/>
+      <c r="F36" s="169"/>
+      <c r="G36" s="170"/>
+      <c r="H36" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="I36" s="117" t="s">
+      <c r="I36" s="125" t="s">
         <v>43</v>
       </c>
-      <c r="J36" s="117" t="s">
+      <c r="J36" s="125" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="168"/>
+      <c r="K36" s="156"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="145"/>
-      <c r="C37" s="146"/>
-      <c r="D37" s="157"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="157"/>
-      <c r="G37" s="158"/>
+        <v>99</v>
+      </c>
+      <c r="B37" s="163"/>
+      <c r="C37" s="164"/>
+      <c r="D37" s="169"/>
+      <c r="E37" s="170"/>
+      <c r="F37" s="169"/>
+      <c r="G37" s="170"/>
       <c r="H37" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="I37" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J37" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="K37" s="168"/>
+        <v>58</v>
+      </c>
+      <c r="I37" s="50"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="156"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A38" s="117" t="s">
+      <c r="A38" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="145"/>
-      <c r="C38" s="146"/>
-      <c r="D38" s="157"/>
-      <c r="E38" s="158"/>
-      <c r="F38" s="157"/>
-      <c r="G38" s="158"/>
-      <c r="H38" s="117" t="s">
+      <c r="B38" s="163"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="169"/>
+      <c r="E38" s="170"/>
+      <c r="F38" s="169"/>
+      <c r="G38" s="170"/>
+      <c r="H38" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="I38" s="117" t="s">
-        <v>48</v>
-      </c>
-      <c r="J38" s="117"/>
-      <c r="K38" s="168"/>
+      <c r="I38" s="125"/>
+      <c r="J38" s="125"/>
+      <c r="K38" s="156"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
       <c r="A39" s="51">
-        <v>823</v>
-      </c>
-      <c r="B39" s="147"/>
-      <c r="C39" s="148"/>
-      <c r="D39" s="159"/>
-      <c r="E39" s="160"/>
-      <c r="F39" s="159"/>
-      <c r="G39" s="160"/>
+        <v>922</v>
+      </c>
+      <c r="B39" s="165"/>
+      <c r="C39" s="166"/>
+      <c r="D39" s="171"/>
+      <c r="E39" s="172"/>
+      <c r="F39" s="171"/>
+      <c r="G39" s="172"/>
       <c r="H39" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I39" s="50" t="s">
-        <v>53</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="I39" s="50"/>
       <c r="J39" s="48"/>
-      <c r="K39" s="169"/>
+      <c r="K39" s="157"/>
     </row>
     <row r="40" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A40" s="117" t="s">
+      <c r="A40" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="141" t="s">
+      <c r="B40" s="158" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="142"/>
-      <c r="D40" s="141" t="s">
+      <c r="C40" s="159"/>
+      <c r="D40" s="158" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="142"/>
-      <c r="F40" s="141" t="s">
+      <c r="E40" s="159"/>
+      <c r="F40" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="G40" s="142"/>
-      <c r="H40" s="154" t="s">
+      <c r="G40" s="159"/>
+      <c r="H40" s="160" t="s">
         <v>38</v>
       </c>
-      <c r="I40" s="154"/>
-      <c r="J40" s="117" t="s">
+      <c r="I40" s="160"/>
+      <c r="J40" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="K40" s="119" t="s">
+      <c r="K40" s="118" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="10.5" customHeight="1">
       <c r="A41" s="48">
-        <v>5</v>
-      </c>
-      <c r="B41" s="143" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="144"/>
-      <c r="D41" s="155" t="s">
-        <v>85</v>
-      </c>
-      <c r="E41" s="156"/>
-      <c r="F41" s="155" t="s">
-        <v>78</v>
-      </c>
-      <c r="G41" s="156"/>
-      <c r="H41" s="161" t="s">
-        <v>10</v>
-      </c>
-      <c r="I41" s="162"/>
+        <v>6</v>
+      </c>
+      <c r="B41" s="161" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="162"/>
+      <c r="D41" s="167" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="168"/>
+      <c r="F41" s="167" t="s">
+        <v>74</v>
+      </c>
+      <c r="G41" s="168"/>
+      <c r="H41" s="173" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="174"/>
       <c r="J41" s="52"/>
-      <c r="K41" s="167"/>
+      <c r="K41" s="155"/>
     </row>
     <row r="42" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A42" s="117" t="s">
+      <c r="A42" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="145"/>
-      <c r="C42" s="146"/>
-      <c r="D42" s="157"/>
-      <c r="E42" s="158"/>
-      <c r="F42" s="157"/>
-      <c r="G42" s="158"/>
-      <c r="H42" s="117" t="s">
+      <c r="B42" s="163"/>
+      <c r="C42" s="164"/>
+      <c r="D42" s="169"/>
+      <c r="E42" s="170"/>
+      <c r="F42" s="169"/>
+      <c r="G42" s="170"/>
+      <c r="H42" s="116" t="s">
         <v>42</v>
       </c>
-      <c r="I42" s="117" t="s">
+      <c r="I42" s="116" t="s">
         <v>43</v>
       </c>
-      <c r="J42" s="117" t="s">
+      <c r="J42" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="K42" s="168"/>
+      <c r="K42" s="156"/>
     </row>
     <row r="43" spans="1:11" ht="10.5" customHeight="1">
       <c r="A43" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="145"/>
-      <c r="C43" s="146"/>
-      <c r="D43" s="157"/>
-      <c r="E43" s="158"/>
-      <c r="F43" s="157"/>
-      <c r="G43" s="158"/>
+        <v>103</v>
+      </c>
+      <c r="B43" s="163"/>
+      <c r="C43" s="164"/>
+      <c r="D43" s="169"/>
+      <c r="E43" s="170"/>
+      <c r="F43" s="169"/>
+      <c r="G43" s="170"/>
       <c r="H43" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="I43" s="50"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="168"/>
+        <v>45</v>
+      </c>
+      <c r="I43" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J43" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="K43" s="156"/>
     </row>
     <row r="44" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A44" s="117" t="s">
+      <c r="A44" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="145"/>
-      <c r="C44" s="146"/>
-      <c r="D44" s="157"/>
-      <c r="E44" s="158"/>
-      <c r="F44" s="157"/>
-      <c r="G44" s="158"/>
-      <c r="H44" s="117" t="s">
+      <c r="B44" s="163"/>
+      <c r="C44" s="164"/>
+      <c r="D44" s="169"/>
+      <c r="E44" s="170"/>
+      <c r="F44" s="169"/>
+      <c r="G44" s="170"/>
+      <c r="H44" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="I44" s="117" t="s">
+      <c r="I44" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="J44" s="117"/>
-      <c r="K44" s="168"/>
+      <c r="J44" s="116"/>
+      <c r="K44" s="156"/>
     </row>
     <row r="45" spans="1:11" ht="10.5" customHeight="1">
       <c r="A45" s="51">
         <v>823</v>
       </c>
-      <c r="B45" s="147"/>
-      <c r="C45" s="148"/>
-      <c r="D45" s="159"/>
-      <c r="E45" s="160"/>
-      <c r="F45" s="159"/>
-      <c r="G45" s="160"/>
+      <c r="B45" s="165"/>
+      <c r="C45" s="166"/>
+      <c r="D45" s="171"/>
+      <c r="E45" s="172"/>
+      <c r="F45" s="171"/>
+      <c r="G45" s="172"/>
       <c r="H45" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="I45" s="50"/>
+        <v>49</v>
+      </c>
+      <c r="I45" s="50" t="s">
+        <v>53</v>
+      </c>
       <c r="J45" s="48"/>
-      <c r="K45" s="169"/>
-    </row>
-    <row r="46" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A46" s="100" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" s="163" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="164"/>
-      <c r="D46" s="164"/>
-      <c r="E46" s="164"/>
-      <c r="F46" s="164"/>
-      <c r="G46" s="164"/>
-      <c r="H46" s="164"/>
-      <c r="I46" s="164"/>
-      <c r="J46" s="164"/>
-      <c r="K46" s="165"/>
-    </row>
-    <row r="47" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A47" s="136" t="s">
+      <c r="K45" s="157"/>
+    </row>
+    <row r="46" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A46" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="150" t="s">
+      <c r="B46" s="158" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="159"/>
+      <c r="D46" s="158" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="159"/>
+      <c r="F46" s="158" t="s">
+        <v>37</v>
+      </c>
+      <c r="G46" s="159"/>
+      <c r="H46" s="160" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="160"/>
+      <c r="J46" s="116" t="s">
+        <v>39</v>
+      </c>
+      <c r="K46" s="118" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A47" s="48">
+        <v>7</v>
+      </c>
+      <c r="B47" s="161" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="162"/>
+      <c r="D47" s="167" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="168"/>
+      <c r="F47" s="167" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="168"/>
+      <c r="H47" s="173" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="174"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="155"/>
+    </row>
+    <row r="48" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A48" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="163"/>
+      <c r="C48" s="164"/>
+      <c r="D48" s="169"/>
+      <c r="E48" s="170"/>
+      <c r="F48" s="169"/>
+      <c r="G48" s="170"/>
+      <c r="H48" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="I48" s="116" t="s">
+        <v>43</v>
+      </c>
+      <c r="J48" s="116" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48" s="156"/>
+    </row>
+    <row r="49" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A49" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="163"/>
+      <c r="C49" s="164"/>
+      <c r="D49" s="169"/>
+      <c r="E49" s="170"/>
+      <c r="F49" s="169"/>
+      <c r="G49" s="170"/>
+      <c r="H49" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I49" s="50"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="156"/>
+    </row>
+    <row r="50" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A50" s="116" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="163"/>
+      <c r="C50" s="164"/>
+      <c r="D50" s="169"/>
+      <c r="E50" s="170"/>
+      <c r="F50" s="169"/>
+      <c r="G50" s="170"/>
+      <c r="H50" s="116" t="s">
+        <v>47</v>
+      </c>
+      <c r="I50" s="116" t="s">
+        <v>48</v>
+      </c>
+      <c r="J50" s="116"/>
+      <c r="K50" s="156"/>
+    </row>
+    <row r="51" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A51" s="51">
+        <v>824</v>
+      </c>
+      <c r="B51" s="165"/>
+      <c r="C51" s="166"/>
+      <c r="D51" s="171"/>
+      <c r="E51" s="172"/>
+      <c r="F51" s="171"/>
+      <c r="G51" s="172"/>
+      <c r="H51" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="I51" s="50"/>
+      <c r="J51" s="48"/>
+      <c r="K51" s="157"/>
+    </row>
+    <row r="52" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A52" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="177" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="178"/>
+      <c r="D52" s="178"/>
+      <c r="E52" s="178"/>
+      <c r="F52" s="178"/>
+      <c r="G52" s="178"/>
+      <c r="H52" s="178"/>
+      <c r="I52" s="178"/>
+      <c r="J52" s="178"/>
+      <c r="K52" s="179"/>
+    </row>
+    <row r="53" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A53" s="134" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="180" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="151"/>
-      <c r="D47" s="150" t="s">
+      <c r="C53" s="181"/>
+      <c r="D53" s="180" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="151"/>
-      <c r="F47" s="150" t="s">
+      <c r="E53" s="181"/>
+      <c r="F53" s="180" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="151"/>
-      <c r="H47" s="149" t="s">
+      <c r="G53" s="181"/>
+      <c r="H53" s="182" t="s">
         <v>38</v>
       </c>
-      <c r="I47" s="149"/>
-      <c r="J47" s="136" t="s">
+      <c r="I53" s="182"/>
+      <c r="J53" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="K47" s="136" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A48" s="48" t="e">
-        <f>A34+1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B48" s="143" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="144"/>
-      <c r="D48" s="155" t="s">
-        <v>87</v>
-      </c>
-      <c r="E48" s="156"/>
-      <c r="F48" s="155" t="s">
-        <v>88</v>
-      </c>
-      <c r="G48" s="156"/>
-      <c r="H48" s="152" t="s">
-        <v>10</v>
-      </c>
-      <c r="I48" s="153"/>
-      <c r="J48" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="K48" s="167"/>
-    </row>
-    <row r="49" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A49" s="136" t="s">
-        <v>41</v>
-      </c>
-      <c r="B49" s="145"/>
-      <c r="C49" s="146"/>
-      <c r="D49" s="157"/>
-      <c r="E49" s="158"/>
-      <c r="F49" s="157"/>
-      <c r="G49" s="158"/>
-      <c r="H49" s="136" t="s">
-        <v>42</v>
-      </c>
-      <c r="I49" s="136" t="s">
-        <v>43</v>
-      </c>
-      <c r="J49" s="136" t="s">
-        <v>44</v>
-      </c>
-      <c r="K49" s="168"/>
-    </row>
-    <row r="50" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A50" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="145"/>
-      <c r="C50" s="146"/>
-      <c r="D50" s="157"/>
-      <c r="E50" s="158"/>
-      <c r="F50" s="157"/>
-      <c r="G50" s="158"/>
-      <c r="H50" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="I50" s="50"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="168"/>
-    </row>
-    <row r="51" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A51" s="136" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" s="145"/>
-      <c r="C51" s="146"/>
-      <c r="D51" s="157"/>
-      <c r="E51" s="158"/>
-      <c r="F51" s="157"/>
-      <c r="G51" s="158"/>
-      <c r="H51" s="136" t="s">
-        <v>47</v>
-      </c>
-      <c r="I51" s="136"/>
-      <c r="J51" s="136"/>
-      <c r="K51" s="168"/>
-    </row>
-    <row r="52" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A52" s="51">
-        <v>922</v>
-      </c>
-      <c r="B52" s="147"/>
-      <c r="C52" s="148"/>
-      <c r="D52" s="159"/>
-      <c r="E52" s="160"/>
-      <c r="F52" s="159"/>
-      <c r="G52" s="160"/>
-      <c r="H52" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="I52" s="50"/>
-      <c r="J52" s="48"/>
-      <c r="K52" s="169"/>
-    </row>
-    <row r="53" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A53" s="137" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="141" t="s">
-        <v>35</v>
-      </c>
-      <c r="C53" s="142"/>
-      <c r="D53" s="141" t="s">
-        <v>36</v>
-      </c>
-      <c r="E53" s="142"/>
-      <c r="F53" s="141" t="s">
-        <v>37</v>
-      </c>
-      <c r="G53" s="142"/>
-      <c r="H53" s="154" t="s">
-        <v>38</v>
-      </c>
-      <c r="I53" s="154"/>
-      <c r="J53" s="137" t="s">
-        <v>39</v>
-      </c>
-      <c r="K53" s="138" t="s">
+      <c r="K53" s="134" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="10.5" customHeight="1">
       <c r="A54" s="48">
-        <v>5</v>
-      </c>
-      <c r="B54" s="143" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="144"/>
-      <c r="D54" s="155" t="s">
-        <v>92</v>
-      </c>
-      <c r="E54" s="156"/>
-      <c r="F54" s="155" t="s">
-        <v>93</v>
-      </c>
-      <c r="G54" s="156"/>
-      <c r="H54" s="161" t="s">
-        <v>9</v>
-      </c>
-      <c r="I54" s="162"/>
-      <c r="J54" s="52"/>
-      <c r="K54" s="167"/>
+        <v>8</v>
+      </c>
+      <c r="B54" s="161" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" s="162"/>
+      <c r="D54" s="167" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="168"/>
+      <c r="F54" s="167" t="s">
+        <v>83</v>
+      </c>
+      <c r="G54" s="168"/>
+      <c r="H54" s="175" t="s">
+        <v>10</v>
+      </c>
+      <c r="I54" s="176"/>
+      <c r="J54" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="K54" s="155"/>
     </row>
     <row r="55" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A55" s="137" t="s">
+      <c r="A55" s="134" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="145"/>
-      <c r="C55" s="146"/>
-      <c r="D55" s="157"/>
-      <c r="E55" s="158"/>
-      <c r="F55" s="157"/>
-      <c r="G55" s="158"/>
-      <c r="H55" s="137" t="s">
+      <c r="B55" s="163"/>
+      <c r="C55" s="164"/>
+      <c r="D55" s="169"/>
+      <c r="E55" s="170"/>
+      <c r="F55" s="169"/>
+      <c r="G55" s="170"/>
+      <c r="H55" s="134" t="s">
         <v>42</v>
       </c>
-      <c r="I55" s="137" t="s">
+      <c r="I55" s="134" t="s">
         <v>43</v>
       </c>
-      <c r="J55" s="137" t="s">
+      <c r="J55" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="K55" s="168"/>
+      <c r="K55" s="156"/>
     </row>
     <row r="56" spans="1:11" ht="10.5" customHeight="1">
       <c r="A56" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" s="145"/>
-      <c r="C56" s="146"/>
-      <c r="D56" s="157"/>
-      <c r="E56" s="158"/>
-      <c r="F56" s="157"/>
-      <c r="G56" s="158"/>
+        <v>104</v>
+      </c>
+      <c r="B56" s="163"/>
+      <c r="C56" s="164"/>
+      <c r="D56" s="169"/>
+      <c r="E56" s="170"/>
+      <c r="F56" s="169"/>
+      <c r="G56" s="170"/>
       <c r="H56" s="50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I56" s="50"/>
       <c r="J56" s="48"/>
-      <c r="K56" s="168"/>
+      <c r="K56" s="156"/>
     </row>
     <row r="57" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A57" s="137" t="s">
+      <c r="A57" s="134" t="s">
         <v>46</v>
       </c>
-      <c r="B57" s="145"/>
-      <c r="C57" s="146"/>
-      <c r="D57" s="157"/>
-      <c r="E57" s="158"/>
-      <c r="F57" s="157"/>
-      <c r="G57" s="158"/>
-      <c r="H57" s="137" t="s">
+      <c r="B57" s="163"/>
+      <c r="C57" s="164"/>
+      <c r="D57" s="169"/>
+      <c r="E57" s="170"/>
+      <c r="F57" s="169"/>
+      <c r="G57" s="170"/>
+      <c r="H57" s="134" t="s">
         <v>47</v>
       </c>
-      <c r="I57" s="137" t="s">
-        <v>48</v>
-      </c>
-      <c r="J57" s="137"/>
-      <c r="K57" s="168"/>
+      <c r="I57" s="134"/>
+      <c r="J57" s="134"/>
+      <c r="K57" s="156"/>
     </row>
     <row r="58" spans="1:11" ht="10.5" customHeight="1">
       <c r="A58" s="51">
-        <v>823</v>
-      </c>
-      <c r="B58" s="147"/>
-      <c r="C58" s="148"/>
-      <c r="D58" s="159"/>
-      <c r="E58" s="160"/>
-      <c r="F58" s="159"/>
-      <c r="G58" s="160"/>
+        <v>923</v>
+      </c>
+      <c r="B58" s="165"/>
+      <c r="C58" s="166"/>
+      <c r="D58" s="171"/>
+      <c r="E58" s="172"/>
+      <c r="F58" s="171"/>
+      <c r="G58" s="172"/>
       <c r="H58" s="50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I58" s="50"/>
       <c r="J58" s="48"/>
-      <c r="K58" s="169"/>
-    </row>
-    <row r="67" spans="1:11" s="58" customFormat="1">
-      <c r="A67" s="62"/>
-      <c r="H67" s="62"/>
-      <c r="I67" s="62"/>
-      <c r="J67" s="62"/>
-      <c r="K67" s="62"/>
-    </row>
-    <row r="68" spans="1:11" s="58" customFormat="1">
-      <c r="A68" s="62"/>
-      <c r="H68" s="62"/>
-      <c r="I68" s="62"/>
-      <c r="J68" s="62"/>
-      <c r="K68" s="62"/>
-    </row>
-    <row r="69" spans="1:11" s="58" customFormat="1">
-      <c r="A69" s="62"/>
-      <c r="H69" s="62"/>
-      <c r="I69" s="62"/>
-      <c r="J69" s="62"/>
-      <c r="K69" s="62"/>
-    </row>
-    <row r="70" spans="1:11" s="58" customFormat="1">
-      <c r="A70" s="62"/>
-      <c r="H70" s="62"/>
-      <c r="I70" s="62"/>
-      <c r="J70" s="62"/>
-      <c r="K70" s="62"/>
-    </row>
-    <row r="71" spans="1:11" s="58" customFormat="1">
-      <c r="A71" s="62"/>
-      <c r="H71" s="62"/>
-      <c r="I71" s="62"/>
-      <c r="J71" s="62"/>
-      <c r="K71" s="62"/>
-    </row>
-    <row r="72" spans="1:11" s="58" customFormat="1">
-      <c r="A72" s="62"/>
-      <c r="H72" s="62"/>
-      <c r="I72" s="62"/>
-      <c r="J72" s="62"/>
-      <c r="K72" s="62"/>
-    </row>
-    <row r="73" spans="1:11" s="58" customFormat="1">
-      <c r="A73" s="62"/>
-      <c r="H73" s="62"/>
-      <c r="I73" s="62"/>
-      <c r="J73" s="62"/>
-      <c r="K73" s="62"/>
-    </row>
-    <row r="74" spans="1:11" s="58" customFormat="1">
-      <c r="A74" s="62"/>
-      <c r="H74" s="62"/>
-      <c r="I74" s="62"/>
-      <c r="J74" s="62"/>
-      <c r="K74" s="62"/>
-    </row>
-    <row r="75" spans="1:11" s="58" customFormat="1">
-      <c r="A75" s="62"/>
-      <c r="H75" s="62"/>
-      <c r="I75" s="62"/>
-      <c r="J75" s="62"/>
-      <c r="K75" s="62"/>
-    </row>
-    <row r="76" spans="1:11" s="58" customFormat="1">
-      <c r="A76" s="62"/>
-      <c r="H76" s="62"/>
-      <c r="I76" s="62"/>
-      <c r="J76" s="62"/>
-      <c r="K76" s="62"/>
-    </row>
-    <row r="77" spans="1:11" s="58" customFormat="1">
-      <c r="A77" s="62"/>
-      <c r="H77" s="62"/>
-      <c r="I77" s="62"/>
-      <c r="J77" s="62"/>
-      <c r="K77" s="62"/>
-    </row>
-    <row r="78" spans="1:11" s="58" customFormat="1">
-      <c r="A78" s="62"/>
-      <c r="H78" s="62"/>
-      <c r="I78" s="62"/>
-      <c r="J78" s="62"/>
-      <c r="K78" s="62"/>
-    </row>
-    <row r="79" spans="1:11" s="58" customFormat="1">
-      <c r="A79" s="62"/>
-      <c r="H79" s="62"/>
-      <c r="I79" s="62"/>
-      <c r="J79" s="62"/>
-      <c r="K79" s="62"/>
-    </row>
-    <row r="80" spans="1:11" s="58" customFormat="1">
-      <c r="A80" s="62"/>
-      <c r="H80" s="62"/>
-      <c r="I80" s="62"/>
-      <c r="J80" s="62"/>
-      <c r="K80" s="62"/>
-    </row>
-    <row r="81" spans="1:11" s="58" customFormat="1">
-      <c r="A81" s="62"/>
-      <c r="H81" s="62"/>
-      <c r="I81" s="62"/>
-      <c r="J81" s="62"/>
-      <c r="K81" s="62"/>
-    </row>
-    <row r="82" spans="1:11" s="58" customFormat="1">
-      <c r="A82" s="62"/>
-      <c r="H82" s="62"/>
-      <c r="I82" s="62"/>
-      <c r="J82" s="62"/>
-      <c r="K82" s="62"/>
-    </row>
-    <row r="83" spans="1:11" s="58" customFormat="1">
-      <c r="A83" s="62"/>
-      <c r="H83" s="62"/>
-      <c r="I83" s="62"/>
-      <c r="J83" s="62"/>
-      <c r="K83" s="62"/>
-    </row>
-    <row r="84" spans="1:11" s="58" customFormat="1">
-      <c r="A84" s="62"/>
-      <c r="H84" s="62"/>
-      <c r="I84" s="62"/>
-      <c r="J84" s="62"/>
-      <c r="K84" s="62"/>
-    </row>
-    <row r="85" spans="1:11" s="58" customFormat="1">
-      <c r="A85" s="62"/>
-      <c r="H85" s="62"/>
-      <c r="I85" s="62"/>
-      <c r="J85" s="62"/>
-      <c r="K85" s="62"/>
-    </row>
-    <row r="86" spans="1:11" s="58" customFormat="1">
-      <c r="A86" s="62"/>
-      <c r="H86" s="62"/>
-      <c r="I86" s="62"/>
-      <c r="J86" s="62"/>
-      <c r="K86" s="62"/>
-    </row>
-    <row r="87" spans="1:11" s="58" customFormat="1">
-      <c r="A87" s="62"/>
-      <c r="H87" s="62"/>
-      <c r="I87" s="62"/>
-      <c r="J87" s="62"/>
-      <c r="K87" s="62"/>
-    </row>
-    <row r="88" spans="1:11" s="58" customFormat="1">
-      <c r="A88" s="62"/>
-      <c r="H88" s="62"/>
-      <c r="I88" s="62"/>
-      <c r="J88" s="62"/>
-      <c r="K88" s="62"/>
-    </row>
-    <row r="89" spans="1:11" s="58" customFormat="1">
-      <c r="A89" s="62"/>
-      <c r="H89" s="62"/>
-      <c r="I89" s="62"/>
-      <c r="J89" s="62"/>
-      <c r="K89" s="62"/>
-    </row>
-    <row r="90" spans="1:11" s="58" customFormat="1">
-      <c r="A90" s="62"/>
-      <c r="H90" s="62"/>
-      <c r="I90" s="62"/>
-      <c r="J90" s="62"/>
-      <c r="K90" s="62"/>
-    </row>
-    <row r="91" spans="1:11" s="58" customFormat="1">
-      <c r="A91" s="62"/>
-      <c r="H91" s="62"/>
-      <c r="I91" s="62"/>
-      <c r="J91" s="62"/>
-      <c r="K91" s="62"/>
-    </row>
-    <row r="92" spans="1:11" s="58" customFormat="1">
-      <c r="A92" s="62"/>
-      <c r="H92" s="62"/>
-      <c r="I92" s="62"/>
-      <c r="J92" s="62"/>
-      <c r="K92" s="62"/>
-    </row>
-    <row r="93" spans="1:11" s="58" customFormat="1">
-      <c r="A93" s="62"/>
-      <c r="H93" s="62"/>
-      <c r="I93" s="62"/>
-      <c r="J93" s="62"/>
-      <c r="K93" s="62"/>
-    </row>
-    <row r="94" spans="1:11" s="58" customFormat="1">
-      <c r="A94" s="62"/>
-      <c r="H94" s="62"/>
-      <c r="I94" s="62"/>
-      <c r="J94" s="62"/>
-      <c r="K94" s="62"/>
-    </row>
-    <row r="95" spans="1:11" s="58" customFormat="1">
-      <c r="A95" s="62"/>
-      <c r="H95" s="62"/>
-      <c r="I95" s="62"/>
-      <c r="J95" s="62"/>
-      <c r="K95" s="62"/>
-    </row>
-    <row r="96" spans="1:11" s="58" customFormat="1">
-      <c r="A96" s="62"/>
-      <c r="H96" s="62"/>
-      <c r="I96" s="62"/>
-      <c r="J96" s="62"/>
-      <c r="K96" s="62"/>
+      <c r="K58" s="157"/>
+    </row>
+    <row r="59" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A59" s="135" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="158" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="159"/>
+      <c r="D59" s="158" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="159"/>
+      <c r="F59" s="158" t="s">
+        <v>37</v>
+      </c>
+      <c r="G59" s="159"/>
+      <c r="H59" s="160" t="s">
+        <v>38</v>
+      </c>
+      <c r="I59" s="160"/>
+      <c r="J59" s="135" t="s">
+        <v>39</v>
+      </c>
+      <c r="K59" s="136" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A60" s="48">
+        <v>9</v>
+      </c>
+      <c r="B60" s="161" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="162"/>
+      <c r="D60" s="167" t="s">
+        <v>87</v>
+      </c>
+      <c r="E60" s="168"/>
+      <c r="F60" s="167" t="s">
+        <v>88</v>
+      </c>
+      <c r="G60" s="168"/>
+      <c r="H60" s="173" t="s">
+        <v>9</v>
+      </c>
+      <c r="I60" s="174"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="155"/>
+    </row>
+    <row r="61" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A61" s="135" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" s="163"/>
+      <c r="C61" s="164"/>
+      <c r="D61" s="169"/>
+      <c r="E61" s="170"/>
+      <c r="F61" s="169"/>
+      <c r="G61" s="170"/>
+      <c r="H61" s="135" t="s">
+        <v>42</v>
+      </c>
+      <c r="I61" s="135" t="s">
+        <v>43</v>
+      </c>
+      <c r="J61" s="135" t="s">
+        <v>44</v>
+      </c>
+      <c r="K61" s="156"/>
+    </row>
+    <row r="62" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A62" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B62" s="163"/>
+      <c r="C62" s="164"/>
+      <c r="D62" s="169"/>
+      <c r="E62" s="170"/>
+      <c r="F62" s="169"/>
+      <c r="G62" s="170"/>
+      <c r="H62" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I62" s="50"/>
+      <c r="J62" s="48"/>
+      <c r="K62" s="156"/>
+    </row>
+    <row r="63" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A63" s="135" t="s">
+        <v>46</v>
+      </c>
+      <c r="B63" s="163"/>
+      <c r="C63" s="164"/>
+      <c r="D63" s="169"/>
+      <c r="E63" s="170"/>
+      <c r="F63" s="169"/>
+      <c r="G63" s="170"/>
+      <c r="H63" s="135" t="s">
+        <v>47</v>
+      </c>
+      <c r="I63" s="135" t="s">
+        <v>48</v>
+      </c>
+      <c r="J63" s="135"/>
+      <c r="K63" s="156"/>
+    </row>
+    <row r="64" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A64" s="51">
+        <v>825</v>
+      </c>
+      <c r="B64" s="165"/>
+      <c r="C64" s="166"/>
+      <c r="D64" s="171"/>
+      <c r="E64" s="172"/>
+      <c r="F64" s="171"/>
+      <c r="G64" s="172"/>
+      <c r="H64" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="I64" s="50"/>
+      <c r="J64" s="48"/>
+      <c r="K64" s="157"/>
+    </row>
+    <row r="65" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A65" s="137" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="180" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" s="181"/>
+      <c r="D65" s="180" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="181"/>
+      <c r="F65" s="180" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" s="181"/>
+      <c r="H65" s="182" t="s">
+        <v>38</v>
+      </c>
+      <c r="I65" s="182"/>
+      <c r="J65" s="137" t="s">
+        <v>39</v>
+      </c>
+      <c r="K65" s="137" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A66" s="48">
+        <v>10</v>
+      </c>
+      <c r="B66" s="161" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="162"/>
+      <c r="D66" s="167" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" s="168"/>
+      <c r="F66" s="167" t="s">
+        <v>90</v>
+      </c>
+      <c r="G66" s="168"/>
+      <c r="H66" s="175" t="s">
+        <v>10</v>
+      </c>
+      <c r="I66" s="176"/>
+      <c r="J66" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="K66" s="155"/>
+    </row>
+    <row r="67" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A67" s="137" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="163"/>
+      <c r="C67" s="164"/>
+      <c r="D67" s="169"/>
+      <c r="E67" s="170"/>
+      <c r="F67" s="169"/>
+      <c r="G67" s="170"/>
+      <c r="H67" s="137" t="s">
+        <v>42</v>
+      </c>
+      <c r="I67" s="137" t="s">
+        <v>43</v>
+      </c>
+      <c r="J67" s="137" t="s">
+        <v>44</v>
+      </c>
+      <c r="K67" s="156"/>
+    </row>
+    <row r="68" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A68" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" s="163"/>
+      <c r="C68" s="164"/>
+      <c r="D68" s="169"/>
+      <c r="E68" s="170"/>
+      <c r="F68" s="169"/>
+      <c r="G68" s="170"/>
+      <c r="H68" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I68" s="50"/>
+      <c r="J68" s="48"/>
+      <c r="K68" s="156"/>
+    </row>
+    <row r="69" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A69" s="137" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69" s="163"/>
+      <c r="C69" s="164"/>
+      <c r="D69" s="169"/>
+      <c r="E69" s="170"/>
+      <c r="F69" s="169"/>
+      <c r="G69" s="170"/>
+      <c r="H69" s="137" t="s">
+        <v>47</v>
+      </c>
+      <c r="I69" s="137"/>
+      <c r="J69" s="137"/>
+      <c r="K69" s="156"/>
+    </row>
+    <row r="70" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A70" s="51">
+        <v>924</v>
+      </c>
+      <c r="B70" s="165"/>
+      <c r="C70" s="166"/>
+      <c r="D70" s="171"/>
+      <c r="E70" s="172"/>
+      <c r="F70" s="171"/>
+      <c r="G70" s="172"/>
+      <c r="H70" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="I70" s="50"/>
+      <c r="J70" s="48"/>
+      <c r="K70" s="157"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
-    <mergeCell ref="K54:K58"/>
+  <mergeCells count="84">
+    <mergeCell ref="K66:K70"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B27:C31"/>
+    <mergeCell ref="D27:E31"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="K27:K31"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="B66:C70"/>
+    <mergeCell ref="D66:E70"/>
+    <mergeCell ref="F66:G70"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="B35:C39"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="B41:C45"/>
+    <mergeCell ref="B47:C51"/>
+    <mergeCell ref="D41:E45"/>
+    <mergeCell ref="D47:E51"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:E25"/>
+    <mergeCell ref="K21:K25"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K47:K51"/>
+    <mergeCell ref="F41:G45"/>
+    <mergeCell ref="K41:K45"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="F47:G51"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="K9:K13"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="D35:E39"/>
+    <mergeCell ref="F35:G39"/>
+    <mergeCell ref="B52:K52"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="F53:G53"/>
@@ -4357,101 +4532,44 @@
     <mergeCell ref="D54:E58"/>
     <mergeCell ref="F54:G58"/>
     <mergeCell ref="H54:I54"/>
-    <mergeCell ref="B48:C52"/>
-    <mergeCell ref="D48:E52"/>
-    <mergeCell ref="F48:G52"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="K48:K52"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="K9:K13"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="D29:E33"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K21:K25"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="K41:K45"/>
-    <mergeCell ref="F35:G39"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="F41:G45"/>
-    <mergeCell ref="B41:C45"/>
-    <mergeCell ref="D35:E39"/>
-    <mergeCell ref="D41:E45"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="D15:E19"/>
-    <mergeCell ref="B15:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B21:C25"/>
-    <mergeCell ref="D21:E25"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B35:C39"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="K54:K58"/>
+    <mergeCell ref="K60:K64"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="B60:C64"/>
+    <mergeCell ref="D60:E64"/>
+    <mergeCell ref="F60:G64"/>
+    <mergeCell ref="H60:I60"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="H41:I41">
+  <conditionalFormatting sqref="H47:I47">
     <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40:I40">
+  <conditionalFormatting sqref="H46:I46">
     <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H54:I54">
+  <conditionalFormatting sqref="H60:I60">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H53:I53">
+  <conditionalFormatting sqref="H59:I59">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Not OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="71" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;LTest Case Table&amp;CBig Point: &amp;A</oddHeader>
     <oddFooter>&amp;LAI&amp;&amp;T-ART&amp;CLiveSpark Project&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="66" max="10" man="1"/>
-  </rowBreaks>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>